<commit_message>
created the POI interactor with the datasheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="133">
   <si>
     <t>URL</t>
   </si>
@@ -36,13 +36,395 @@
   </si>
   <si>
     <t>BreadCrumbsLinks</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/no.+famous+cigars</t>
+  </si>
+  <si>
+    <t># Famous Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>#Famous cigars are a unique aromatic blend created for cigar smokers who enjoy flavor-infused cigars. Using a secret Nicaraguan tobacco blend, the smoke is...</t>
+  </si>
+  <si>
+    <t># Famous Cigars</t>
+  </si>
+  <si>
+    <t>#Famous cigars are a unique aromatic blend created for cigar smokers who enjoy flavor-infused cigars. Using a secret Nicaraguan tobacco blend, the smoke is ultra-mellow and hits you with a fragrant mélange of vanilla, caramel, and sweet coffee &amp; cream. Made in 2 sizes - Toro and Petite Corona - presented in a refillable vacuum-sealed humidor jar for guaranteed freshness, you'll be as surprised by the low price as you will by their awesome bouquet. Get your #Famous cigar shape now and #goforit!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » # Famous</t>
+  </si>
+  <si>
+    <t>Famous Smoke Shop Cigars&gt;&gt;https://www.famous-smoke.com/,Discount Cigars Online&gt;&gt;https://www.famous-smoke.com/cigars,Cigar Brand List&gt;&gt;https://www.famous-smoke.com/cigar-brand-list</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/1502+cigars</t>
+  </si>
+  <si>
+    <t>1502 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Searching for 1502 Cigars on sale? Save big when you shop our complete selection now at Famous Smoke Shop!</t>
+  </si>
+  <si>
+    <t>1502 Cigars</t>
+  </si>
+  <si>
+    <t>Years of blending, generations of expertise and centuries of tradition have all factored into the making of great cigars — and 1502 Cigars is no exception. Innovation, passion and development by companies such as theirs have been key in the effort to bring you the best cigar smoking experience known to man since he first rolled up a leaf and smoked it. And it’s hard to argue that with hard work like this, the premium cigar world is now the best it’s ever been. They’re committed to delighting the senses each and every time you set flame to the foot, with your preferences in mind. And that’s the beauty of all of the premium cigars on sale at Famous Smoke Shop — fitting all ranges of tastes, likes and prices, there is truly a cigar for everyone here at Famous.
+... more</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 1502 Cigars</t>
+  </si>
+  <si>
+    <t>Famous Smoke Shop Cigars&gt;&gt;https://www.famous-smoke.com/,Cigars&gt;&gt;https://www.famous-smoke.com/cigars/,Cigar Brand List&gt;&gt;https://www.famous-smoke.com/cigar-brand-list/</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+black+gold+cigars</t>
+  </si>
+  <si>
+    <t>1502 Black Gold Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Black Gold cigars are artisan-crafted premiums made in Estelí, Nicaragua. Created for savvy cigar smokers who crave dark, robust and complex tobacco...</t>
+  </si>
+  <si>
+    <t>1502 Black Gold Cigars</t>
+  </si>
+  <si>
+    <t>1502 Black Gold cigars are artisan-crafted premiums made in Estelí, Nicaragua. Created for savvy cigar smokers who crave dark, robust and complex tobacco flavor, these BOX-PRESSED Nicaraguans boast a sun-grown maduro wrapper that lends a hearty character to this multi-faceted blend. The smoke simmers with earthy, nutty, woody notes, a pinch of chili pepper, plus subtly sweet chocolate and fruity notes. Price reasonably, try some of these fine boutique cigars today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Black Gold</t>
+  </si>
+  <si>
+    <t>Famous Smoke Shop Cigars&gt;&gt;https://www.famous-smoke.com/,Discount Cigars Online&gt;&gt;https://www.famous-smoke.com/cigars,Cigar Brand List&gt;&gt;https://www.famous-smoke.com/cigar-brand-list,All 1502 Brands&gt;&gt;https://www.famous-smoke.com/brandgroup/1502+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+emerald+cigars</t>
+  </si>
+  <si>
+    <t>1502 Emerald Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery...</t>
+  </si>
+  <si>
+    <t>1502 Emerald Cigars</t>
+  </si>
+  <si>
+    <t>1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery Nicaragua Corojo wrappers that cap a carefully selected blend of Mexican San Andres long-fillers, plus Nicaraguan Estelí &amp; Condega tobaccos. Velvety smoke reveals delicate apple and other citrusy elements, plus a dash of sweet cedar, as the aroma lends fragrances of honey, vanilla and floral notes. Order some of these fine cigars today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Emerald</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+nicaragua+cigars</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua cigars are super-premium, boutique selection from Nicaragua. Medium-full in body, these BOX-PRESSED puros boast master-level craftsmanship...</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua Cigars</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua cigars are super-premium, boutique selection from Nicaragua. Medium-full in body, these BOX-PRESSED puros boast master-level craftsmanship using a blend of perfectly-aged long-filler tobaccos from Esteli, Condega, Jalapa, and Ometepe. Expect a velvety smooth, medium-full smoke multi-layered with fruity, nutty and floral notes, plus a dash of Ometepe spice, enhanced by aromas of honey and vanilla. Reasonably-priced, too. Try these distinctive cigars by ordering some today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Nicaragua</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+ruby+cigars</t>
+  </si>
+  <si>
+    <t>1502 Ruby Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Ruby cigars are an artisan quality selection handcrafted in Estelí, Nicaragua. These aesthetically appealing cigars offer you a medium-full blend of...</t>
+  </si>
+  <si>
+    <t>1502 Ruby Cigars</t>
+  </si>
+  <si>
+    <t>1502 Ruby cigars are an artisan quality selection handcrafted in Estelí, Nicaragua. These aesthetically appealing cigars offer you a medium-full blend of the most select Nicaraguan Estelí &amp; Jalapa tobaccos BOX-PRESSED in an attractively dark, oily Cuban-seed wrapper grown in Ecuador. The smoke is exceptionally well-balanced, serving-up an earthy-woody flavor profile with notes of sweet cedar and toasted nuts. Try this real gem of a cigar by adding some to your cart today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Ruby</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1994+by+la+flor+dominicana+cigars</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana holds a very special meaning to the company that brought you some of the highest rated cigars year after year. The 1994...</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana Cigars</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana holds a very special meaning to the company that brought you some of the highest rated cigars year after year. The 1994 commemorates Litto and Ines Gomez's 20th year with the LFD cigar brand they created. Dominican longfillers and binders are dressed in an oily Mexican San Andres natural wrapper, with 4 sizes to choose from. If you're a fan of LFD, you should only expect yet another cigar with stellar flavor and a full bodied strength profile. Get yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All La Flor Dominicana Brands » 1994 By La Flor Dominicana</t>
+  </si>
+  <si>
+    <t>Famous Smoke Shop Cigars&gt;&gt;https://www.famous-smoke.com/,Discount Cigars Online&gt;&gt;https://www.famous-smoke.com/cigars,Cigar Brand List&gt;&gt;https://www.famous-smoke.com/cigar-brand-list,All La Flor Dominicana Brands&gt;&gt;https://www.famous-smoke.com/brandgroup/la+flor+dominicana+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/262+cigars</t>
+  </si>
+  <si>
+    <t>262 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 cigars for sale at Famous Smoke Shop's online cigar store. These boutique cigars present a revolution in premium cigar quality, taste, and complexity.</t>
+  </si>
+  <si>
+    <t>262 Cigars</t>
+  </si>
+  <si>
+    <t>The brainchild of Clint Aaron and Mike Justice, 262 Cigars is a collective of premium cigar brands that have been riding the new wave of boutique cigars into the marketplace since 2010. The name stands for February 1962, the month and year that President John F. Kennedy signed the Cuban Trade Embargo. It also stands for something more than just really good cigars; it stands for a new paradigm and an ideology to which Aaron and Justice have assigned the slogan, ""Smoke the Revolution.""
+" ... more</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 262 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+allegiance+cigars</t>
+  </si>
+  <si>
+    <t>262 Allegiance Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>I pledge allegiance to the cigar called 262 Allegiance. Originally planned as a seasonal blend, Allegiance was met with such an enthusiastic response the...</t>
+  </si>
+  <si>
+    <t>262 Allegiance Cigars</t>
+  </si>
+  <si>
+    <t>I pledge allegiance to the cigar called 262 Allegiance. Originally planned as a seasonal blend, Allegiance was met with such an enthusiastic response the company decided to make it a full production cigar handcrafted at Tabacalera Carreras factory in Esteli, Nicaragua with a Brazilian Mata Fina wrapper, Nicaraguan binder and a Honduran-Nicaraguan filler blend. Expect an effortless, enjoyable, and very affordable smoke that's mild to medium in body, yet very rich in flavor. Order yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Allegiance</t>
+  </si>
+  <si>
+    <t>Famous Smoke Shop Cigars&gt;&gt;https://www.famous-smoke.com/,Discount Cigars Online&gt;&gt;https://www.famous-smoke.com/cigars,Cigar Brand List&gt;&gt;https://www.famous-smoke.com/cigar-brand-list,All 262 Brands&gt;&gt;https://www.famous-smoke.com/brandgroup/262+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+ideology+cigars</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262...</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Ideology is Mild yet complex smoke with Nicaraguan, Mexican, and Dominican fillers, a Nicaraguan binder, and a Nicaraguan Habano Rosado wrapper that ads a buttery creaminess to an outstanding smoke. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Ideology</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+paradigm+cigars</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262...</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Paradigm is a medium to full bodied complex smoke with Nicaraguan and rare Colombian fillers, a Honduran binder, and a rich and creamy Brazilian Mata Fina wrapper. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Paradigm</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+revere+1+cigars</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is...</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Revere is a full bodied Nicaraguan Puro with a blend of fillers from Esteli, Jalapa, and Condega, a binder with Esteli and Jalapa tobaccos, and a Jalapa Valley wrapper. The result is a complex and bold cigar packed with unbelievable flavor. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Revere</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/4th+generation+pipe+accessories</t>
+  </si>
+  <si>
+    <t>4th Generation Pipe | Famous Smoke</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>4th Generation Pipe</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Accessories » Accessories » Tobacco Brand List » 4th Generation Pipe</t>
+  </si>
+  <si>
+    <t>Famous Smoke Shop Accessories&gt;&gt;https://www.famous-smoke.com/,Accessories&gt;&gt;https://www.famous-smoke.com/accessories,Tobacco Brand List&gt;&gt;https://www.famous-smoke.com/tobacco-brand-list</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/6+pack+samplers+cigars</t>
+  </si>
+  <si>
+    <t>6 Pack Cigar Samplers | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Sure, you're used to seeing cigars presented in 5-packs, but we've taken them one step beyond in this delicious series of 6-Packs presented in a wide...</t>
+  </si>
+  <si>
+    <t>6 Pack Cigar Samplers</t>
+  </si>
+  <si>
+    <t>Sure, you're used to seeing cigars presented in 5-packs, but we've taken them one step beyond in this delicious series of 6-Packs presented in a wide variety of strengths, wrappers, and even a couple of coffee flavored combos. Starring the bestselling cigars in the business at nice prices, now you can get a 6-pack without working out. Browse through the list now and order the Best Sellers 6-Packs that are right for you. There's no better or thriftier way to own great cigars!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » 6 Pack Samplers</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/601+cigars</t>
+  </si>
+  <si>
+    <t>601 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Looking for 601 Cigars? Get huge savings and a complete selection at Famous Smoke.</t>
+  </si>
+  <si>
+    <t>601 Cigars</t>
+  </si>
+  <si>
+    <t>601 Cigars is known throughout the industry as being some of the most delicious, well made, heavy hitting stogies around. Making use of virtually every priming of numerous types of tobacco, Erik Espinosa along with then partner Eddie Ortega blended and released the 601 cigar line in the mid 2000s with the infamous Blue, Red, and Green labels. From there, the brand only kept expanding with the La Bomba and Warhead. Now you can have your own slice of stogie heaven with Famous Smoke Shop discount prices on all lines of this wonderful cigar. Get yours today from our massive inventory and save today!
+... more</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 601 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+accesories+and+samplers+cigars</t>
+  </si>
+  <si>
+    <t>601 Accesories And Cigar Samplers | Famous Smoke</t>
+  </si>
+  <si>
+    <t>601 cigars were originally created by Amilcar Perez-Castro in August of 2006, and have since taken off like wildfire. Now manufactured at Tavicusa S.A in...</t>
+  </si>
+  <si>
+    <t>601 Accesories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>601 cigars were originally created by Amilcar Perez-Castro in August of 2006, and have since taken off like wildfire. Now manufactured at Tavicusa S.A in Estelí, Nicaragua under the direction of Erik Espinosa, since its debut, the 601 series has received heaps of praise from cigar media and cigar smokers alike. Ranging from medium to full-bodied, the line offers something wonderful for even the most discerning palates. Try one of these supreme selections today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Accesories And Samplers</t>
+  </si>
+  <si>
+    <t>Famous Smoke Shop Cigars&gt;&gt;https://www.famous-smoke.com/,Discount Cigars Online&gt;&gt;https://www.famous-smoke.com/cigars,Cigar Brand List&gt;&gt;https://www.famous-smoke.com/cigar-brand-list,All 601 Brands&gt;&gt;https://www.famous-smoke.com/brandgroup/601+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+blue+label+cigars</t>
+  </si>
+  <si>
+    <t>601 Blue Label Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>The 601 'Blue' cigar series are slightly box-pressed, medium to full-bodied premium cigars. Manufactured by Tavicusa S.A., they boast an exquisite recipe...</t>
+  </si>
+  <si>
+    <t>601 Blue Label Cigars</t>
+  </si>
+  <si>
+    <t>The 601 'Blue' cigar series are slightly box-pressed, medium to full-bodied premium cigars. Manufactured by Tavicusa S.A., they boast an exquisite recipe of perfectly-aged Nicaraguan longfillers finished in a dark Nicaraguan Habano wrapper. Precisely blended to offer a rich, well-balanced medley of dark and naturally sweet tobacco flavors enhanced by an arousing aroma, if you prefer taste over strength, this is the 601 for you. Make sure you have a box on-hand for those special occasions.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Blue Label</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+green+label+oscuro+cigars</t>
+  </si>
+  <si>
+    <t>601 Green Label Oscuro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>The 601 'Green' cigar series comprises a full-bodied blend created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan long-filler...</t>
+  </si>
+  <si>
+    <t>601 Green Label Oscuro Cigars</t>
+  </si>
+  <si>
+    <t>The 601 'Green' cigar series comprises a full-bodied blend created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan long-filler tobaccos. Rolled in an exquisite Nicaraguan Habano Oscuro wrapper leaf, these puros are, by far, among the most full-flavored in the 601 series. Each cigar is precisely blended to offer a well-balanced, robust smoke brimming with juicy, complex flavors. If you crave big, bold flavor and aroma in your cigars, add a box to your cart now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Green Label Oscuro</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+la+bomba+1+cigars</t>
+  </si>
+  <si>
+    <t>601 La Bomba Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Calling this new addition to the highly-acclaimed 601 cigars selection The Bomb is an understatement. The blend consists of an all-Nicaraguan longfiller &amp;...</t>
+  </si>
+  <si>
+    <t>601 La Bomba Cigars</t>
+  </si>
+  <si>
+    <t>Calling this new addition to the highly-acclaimed 601 cigars selection The Bomb is an understatement. The blend consists of an all-Nicaraguan longfiller &amp; binder core rolled in a savory Habano wrapper leaf. If you love lots'a Ligero, you'll enjoy this explosive, extra-strength smoke in a Nicaraguan puro format. Presented in boxes of 10 cigars spanning several popular sizes, La Bomba is chock full of dark, spicy tobacco flavor. Order your box now (Experienced smokers preferred).</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 La Bomba</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+red+label+habano+cigars</t>
+  </si>
+  <si>
+    <t>601 Red Label Habano Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>601 Red Label cigars are full-bodied premium cigars created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan longfillers topped...</t>
+  </si>
+  <si>
+    <t>601 Red Label Habano Cigars</t>
+  </si>
+  <si>
+    <t>601 Red Label cigars are full-bodied premium cigars created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan longfillers topped with an attractively oily Nicaraguan Natural Habano wrapper. The 601 'Red' is blended for the experienced cigar smoker providing a stunning mosaic of well-balanced flavors, while maintaining its complex flavor profile from start to finish with an enticing aroma. If you love robust and peppery Nicaraguan puros, order a box or a 5-pack now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Red Label Habano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,14 +436,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,30 +479,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,63 +800,503 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="50" style="4" customWidth="1"/>
-    <col min="7" max="7" width="53.77734375" style="5" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="34.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="35.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="24.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="28.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="64.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="50.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="53.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
+    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added cell formatting to the workbook
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
   <si>
     <t>URL</t>
   </si>
@@ -159,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -182,11 +182,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -196,6 +232,30 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,9 +561,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -543,107 +605,107 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="11" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
method extraction in the DataWorkbook class
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>URL</t>
   </si>
@@ -103,24 +103,6 @@
   </si>
   <si>
     <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/1502+cigars</t>
-  </si>
-  <si>
-    <t>https://www.famous-smoke.com/brand/1502+emerald+cigars</t>
-  </si>
-  <si>
-    <t>1502 Emerald Cigars | Famous Smoke</t>
-  </si>
-  <si>
-    <t>1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery...</t>
-  </si>
-  <si>
-    <t>1502 Emerald Cigars</t>
-  </si>
-  <si>
-    <t>1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery Nicaragua Corojo wrappers that cap a carefully selected blend of Mexican San Andres long-fillers, plus Nicaraguan Estelí &amp; Condega tobaccos. Velvety smoke reveals delicate apple and other citrusy elements, plus a dash of sweet cedar, as the aroma lends fragrances of honey, vanilla and floral notes. Order some of these fine cigars today!</t>
-  </si>
-  <si>
-    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Emerald</t>
   </si>
 </sst>
 </file>
@@ -159,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -200,29 +182,11 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -234,27 +198,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
-      <alignment vertical="bottom" wrapText="true"/>
+      <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
-      <alignment vertical="bottom" wrapText="true"/>
+      <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
-      <alignment vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
-      <alignment vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -561,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,107 +554,81 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4">
+      <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="H4" s="6" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved the pageobjects and api to the test source folder
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>URL</t>
   </si>
@@ -44,19 +44,19 @@
     <t>https://www.famous-smoke.com/brand/no.+famous+cigars</t>
   </si>
   <si>
-    <t># Famous Cigars | Famous Smoke</t>
+    <t># Famous | Famous Smoke</t>
   </si>
   <si>
     <t>#Famous cigars are a unique aromatic blend created for cigar smokers who enjoy flavor-infused cigars. Using a secret Nicaraguan tobacco blend, the smoke is...</t>
   </si>
   <si>
-    <t># Famous Cigars</t>
+    <t># Famous</t>
   </si>
   <si>
     <t>#Famous cigars are a unique aromatic blend created for cigar smokers who enjoy flavor-infused cigars. Using a secret Nicaraguan tobacco blend, the smoke is ultra-mellow and hits you with a fragrant mélange of vanilla, caramel, and sweet coffee &amp; cream. Made in 2 sizes - Toro and Petite Corona - presented in a refillable vacuum-sealed humidor jar for guaranteed freshness, you'll be as surprised by the low price as you will by their awesome bouquet. Get your #Famous cigar shape now and #goforit!</t>
   </si>
   <si>
-    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » # Famous</t>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » # Famous Cigars</t>
   </si>
   <si>
     <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list</t>
@@ -87,22 +87,155 @@
     <t>https://www.famous-smoke.com/brand/1502+black+gold+cigars</t>
   </si>
   <si>
-    <t>1502 Black Gold Cigars | Famous Smoke</t>
+    <t>1502 Black Gold | Famous Smoke</t>
   </si>
   <si>
     <t>1502 Black Gold cigars are artisan-crafted premiums made in Estelí, Nicaragua. Created for savvy cigar smokers who crave dark, robust and complex tobacco...</t>
   </si>
   <si>
-    <t>1502 Black Gold Cigars</t>
+    <t>1502 Black Gold</t>
   </si>
   <si>
     <t>1502 Black Gold cigars are artisan-crafted premiums made in Estelí, Nicaragua. Created for savvy cigar smokers who crave dark, robust and complex tobacco flavor, these BOX-PRESSED Nicaraguans boast a sun-grown maduro wrapper that lends a hearty character to this multi-faceted blend. The smoke simmers with earthy, nutty, woody notes, a pinch of chili pepper, plus subtly sweet chocolate and fruity notes. Price reasonably, try some of these fine boutique cigars today!</t>
   </si>
   <si>
-    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Black Gold</t>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Black Gold Cigars</t>
   </si>
   <si>
     <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/1502+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+emerald+cigars</t>
+  </si>
+  <si>
+    <t>1502 Emerald | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery...</t>
+  </si>
+  <si>
+    <t>1502 Emerald</t>
+  </si>
+  <si>
+    <t>1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery Nicaragua Corojo wrappers that cap a carefully selected blend of Mexican San Andres long-fillers, plus Nicaraguan Estelí &amp; Condega tobaccos. Velvety smoke reveals delicate apple and other citrusy elements, plus a dash of sweet cedar, as the aroma lends fragrances of honey, vanilla and floral notes. Order some of these fine cigars today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Emerald Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+nicaragua+cigars</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua cigars are super-premium, boutique selection from Nicaragua. Medium-full in body, these BOX-PRESSED puros boast master-level craftsmanship...</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua cigars are super-premium, boutique selection from Nicaragua. Medium-full in body, these BOX-PRESSED puros boast master-level craftsmanship using a blend of perfectly-aged long-filler tobaccos from Esteli, Condega, Jalapa, and Ometepe. Expect a velvety smooth, medium-full smoke multi-layered with fruity, nutty and floral notes, plus a dash of Ometepe spice, enhanced by aromas of honey and vanilla. Reasonably-priced, too. Try these distinctive cigars by ordering some today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Nicaragua Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+ruby+cigars</t>
+  </si>
+  <si>
+    <t>1502 Ruby | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Ruby cigars are an artisan quality selection handcrafted in Estelí, Nicaragua. These aesthetically appealing cigars offer you a medium-full blend of...</t>
+  </si>
+  <si>
+    <t>1502 Ruby</t>
+  </si>
+  <si>
+    <t>1502 Ruby cigars are an artisan quality selection handcrafted in Estelí, Nicaragua. These aesthetically appealing cigars offer you a medium-full blend of the most select Nicaraguan Estelí &amp; Jalapa tobaccos BOX-PRESSED in an attractively dark, oily Cuban-seed wrapper grown in Ecuador. The smoke is exceptionally well-balanced, serving-up an earthy-woody flavor profile with notes of sweet cedar and toasted nuts. Try this real gem of a cigar by adding some to your cart today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Ruby Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1994+by+la+flor+dominicana+cigars</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana holds a very special meaning to the company that brought you some of the highest rated cigars year after year. The 1994...</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana holds a very special meaning to the company that brought you some of the highest rated cigars year after year. The 1994 commemorates Litto and Ines Gomez's 20th year with the LFD cigar brand they created. Dominican longfillers and binders are dressed in an oily Mexican San Andres natural wrapper, with 4 sizes to choose from. If you're a fan of LFD, you should only expect yet another cigar with stellar flavor and a full bodied strength profile. Get yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All La Flor Dominicana Brands » 1994 By La Flor Dominicana Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/la+flor+dominicana+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/262+cigars</t>
+  </si>
+  <si>
+    <t>262 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 cigars for sale at Famous Smoke Shop's online cigar store. These boutique cigars present a revolution in premium cigar quality, taste, and complexity.</t>
+  </si>
+  <si>
+    <t>262 Cigars</t>
+  </si>
+  <si>
+    <t>The brainchild of Clint Aaron and Mike Justice, 262 Cigars is a collective of premium cigar brands that have been riding the new wave of boutique cigars into the marketplace since 2010. The name stands for February 1962, the month and year that President John F. Kennedy signed the Cuban Trade Embargo. It also stands for something more than just really good cigars; it stands for a new paradigm and an ideology to which Aaron and Justice have assigned the slogan, ""Smoke the Revolution.""
+" ... more</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 262 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+allegiance+cigars</t>
+  </si>
+  <si>
+    <t>262 Allegiance | Famous Smoke</t>
+  </si>
+  <si>
+    <t>I pledge allegiance to the cigar called 262 Allegiance. Originally planned as a seasonal blend, Allegiance was met with such an enthusiastic response the...</t>
+  </si>
+  <si>
+    <t>262 Allegiance</t>
+  </si>
+  <si>
+    <t>I pledge allegiance to the cigar called 262 Allegiance. Originally planned as a seasonal blend, Allegiance was met with such an enthusiastic response the company decided to make it a full production cigar handcrafted at Tabacalera Carreras factory in Esteli, Nicaragua with a Brazilian Mata Fina wrapper, Nicaraguan binder and a Honduran-Nicaraguan filler blend. Expect an effortless, enjoyable, and very affordable smoke that's mild to medium in body, yet very rich in flavor. Order yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Allegiance Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/262+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+ideology+cigars</t>
+  </si>
+  <si>
+    <t>262 Ideology | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262...</t>
+  </si>
+  <si>
+    <t>262 Ideology</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Ideology is Mild yet complex smoke with Nicaraguan, Mexican, and Dominican fillers, a Nicaraguan binder, and a Nicaraguan Habano Rosado wrapper that ads a buttery creaminess to an outstanding smoke. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Ideology Cigars</t>
   </si>
 </sst>
 </file>
@@ -186,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -196,6 +329,27 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
@@ -513,7 +667,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,6 +786,188 @@
         <v>28</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added the CheckLogo Action
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="73">
   <si>
     <t>URL</t>
   </si>
@@ -274,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -315,11 +315,155 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -358,6 +502,246 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -709,262 +1093,262 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="84" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="85" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="86" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="87" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="88" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="89" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="90" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="91" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="92" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="93" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
expanded the maximum brands for the crawler
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6328" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6408" uniqueCount="73">
   <si>
     <t>URL</t>
   </si>
@@ -274,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="315">
+  <borders count="319">
     <border>
       <left/>
       <right/>
@@ -1716,11 +1716,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="794">
+  <cellXfs count="804">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4099,6 +4117,36 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="314" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -4450,262 +4498,262 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="784" t="s">
+      <c r="A2" s="794" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="784" t="s">
+      <c r="B2" s="794" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="784" t="s">
+      <c r="C2" s="794" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="784" t="s">
+      <c r="D2" s="794" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="784" t="s">
+      <c r="E2" s="794" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="784" t="s">
+      <c r="F2" s="794" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="784" t="s">
+      <c r="G2" s="794" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="784" t="s">
+      <c r="H2" s="794" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="785" t="s">
+      <c r="A3" s="795" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="785" t="s">
+      <c r="B3" s="795" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="785" t="s">
+      <c r="C3" s="795" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="785" t="s">
+      <c r="D3" s="795" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="785" t="s">
+      <c r="E3" s="795" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="785" t="s">
+      <c r="F3" s="795" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="785" t="s">
+      <c r="G3" s="795" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="785" t="s">
+      <c r="H3" s="795" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="786" t="s">
+      <c r="A4" s="796" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="786" t="s">
+      <c r="B4" s="796" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="786" t="s">
+      <c r="C4" s="796" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="786" t="s">
+      <c r="D4" s="796" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="786" t="s">
+      <c r="E4" s="796" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="786" t="s">
+      <c r="F4" s="796" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="786" t="s">
+      <c r="G4" s="796" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="786" t="s">
+      <c r="H4" s="796" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="787" t="s">
+      <c r="A5" s="797" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="787" t="s">
+      <c r="B5" s="797" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="787" t="s">
+      <c r="C5" s="797" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="787" t="s">
+      <c r="D5" s="797" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="787" t="s">
+      <c r="E5" s="797" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="787" t="s">
+      <c r="F5" s="797" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="787" t="s">
+      <c r="G5" s="797" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="787" t="s">
+      <c r="H5" s="797" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="788" t="s">
+      <c r="A6" s="798" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="788" t="s">
+      <c r="B6" s="798" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="788" t="s">
+      <c r="C6" s="798" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="788" t="s">
+      <c r="D6" s="798" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="788" t="s">
+      <c r="E6" s="798" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="788" t="s">
+      <c r="F6" s="798" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="788" t="s">
+      <c r="G6" s="798" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="788" t="s">
+      <c r="H6" s="798" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="789" t="s">
+      <c r="A7" s="799" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="789" t="s">
+      <c r="B7" s="799" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="789" t="s">
+      <c r="C7" s="799" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="789" t="s">
+      <c r="D7" s="799" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="789" t="s">
+      <c r="E7" s="799" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="789" t="s">
+      <c r="F7" s="799" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="789" t="s">
+      <c r="G7" s="799" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="789" t="s">
+      <c r="H7" s="799" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="790" t="s">
+      <c r="A8" s="800" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="790" t="s">
+      <c r="B8" s="800" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="790" t="s">
+      <c r="C8" s="800" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="790" t="s">
+      <c r="D8" s="800" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="790" t="s">
+      <c r="E8" s="800" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="790" t="s">
+      <c r="F8" s="800" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="790" t="s">
+      <c r="G8" s="800" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="790" t="s">
+      <c r="H8" s="800" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="791" t="s">
+      <c r="A9" s="801" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="791" t="s">
+      <c r="B9" s="801" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="791" t="s">
+      <c r="C9" s="801" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="791" t="s">
+      <c r="D9" s="801" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="791" t="s">
+      <c r="E9" s="801" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="791" t="s">
+      <c r="F9" s="801" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="791" t="s">
+      <c r="G9" s="801" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="791" t="s">
+      <c r="H9" s="801" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="792" t="s">
+      <c r="A10" s="802" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="792" t="s">
+      <c r="B10" s="802" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="792" t="s">
+      <c r="C10" s="802" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="792" t="s">
+      <c r="D10" s="802" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="792" t="s">
+      <c r="E10" s="802" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="792" t="s">
+      <c r="F10" s="802" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="792" t="s">
+      <c r="G10" s="802" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="792" t="s">
+      <c r="H10" s="802" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="793" t="s">
+      <c r="A11" s="803" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="793" t="s">
+      <c r="B11" s="803" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="793" t="s">
+      <c r="C11" s="803" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="793" t="s">
+      <c r="D11" s="803" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="793" t="s">
+      <c r="E11" s="803" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="793" t="s">
+      <c r="F11" s="803" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="793" t="s">
+      <c r="G11" s="803" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="793" t="s">
+      <c r="H11" s="803" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
management of the crawler through a single driver
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6408" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7024" uniqueCount="79">
   <si>
     <t>URL</t>
   </si>
@@ -236,6 +236,24 @@
   </si>
   <si>
     <t>BREADCRUMBSLINKS</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+paradigm+cigars</t>
+  </si>
+  <si>
+    <t>262 Paradigm | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262...</t>
+  </si>
+  <si>
+    <t>262 Paradigm</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Paradigm is a medium to full bodied complex smoke with Nicaraguan and rare Colombian fillers, a Honduran binder, and a rich and creamy Brazilian Mata Fina wrapper. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Paradigm Cigars</t>
   </si>
 </sst>
 </file>
@@ -274,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="319">
+  <borders count="347">
     <border>
       <left/>
       <right/>
@@ -1734,11 +1752,137 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="804">
+  <cellXfs count="881">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4147,6 +4291,237 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="326" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="334" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="338" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="346" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -4498,262 +4873,288 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="794" t="s">
+      <c r="A2" s="870" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="794" t="s">
+      <c r="B2" s="870" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="794" t="s">
+      <c r="C2" s="870" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="794" t="s">
+      <c r="D2" s="870" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="794" t="s">
+      <c r="E2" s="870" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="794" t="s">
+      <c r="F2" s="870" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="794" t="s">
+      <c r="G2" s="870" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="794" t="s">
+      <c r="H2" s="870" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="795" t="s">
+      <c r="A3" s="871" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="795" t="s">
+      <c r="B3" s="871" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="795" t="s">
+      <c r="C3" s="871" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="795" t="s">
+      <c r="D3" s="871" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="795" t="s">
+      <c r="E3" s="871" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="795" t="s">
+      <c r="F3" s="871" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="795" t="s">
+      <c r="G3" s="871" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="795" t="s">
+      <c r="H3" s="871" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="796" t="s">
+      <c r="A4" s="872" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="796" t="s">
+      <c r="B4" s="872" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="796" t="s">
+      <c r="C4" s="872" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="796" t="s">
+      <c r="D4" s="872" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="796" t="s">
+      <c r="E4" s="872" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="796" t="s">
+      <c r="F4" s="872" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="796" t="s">
+      <c r="G4" s="872" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="796" t="s">
+      <c r="H4" s="872" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="797" t="s">
+      <c r="A5" s="873" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="797" t="s">
+      <c r="B5" s="873" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="797" t="s">
+      <c r="C5" s="873" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="797" t="s">
+      <c r="D5" s="873" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="797" t="s">
+      <c r="E5" s="873" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="797" t="s">
+      <c r="F5" s="873" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="797" t="s">
+      <c r="G5" s="873" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="797" t="s">
+      <c r="H5" s="873" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="798" t="s">
+      <c r="A6" s="874" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="798" t="s">
+      <c r="B6" s="874" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="798" t="s">
+      <c r="C6" s="874" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="798" t="s">
+      <c r="D6" s="874" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="798" t="s">
+      <c r="E6" s="874" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="798" t="s">
+      <c r="F6" s="874" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="798" t="s">
+      <c r="G6" s="874" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="798" t="s">
+      <c r="H6" s="874" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="799" t="s">
+      <c r="A7" s="875" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="799" t="s">
+      <c r="B7" s="875" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="799" t="s">
+      <c r="C7" s="875" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="799" t="s">
+      <c r="D7" s="875" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="799" t="s">
+      <c r="E7" s="875" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="799" t="s">
+      <c r="F7" s="875" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="799" t="s">
+      <c r="G7" s="875" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="799" t="s">
+      <c r="H7" s="875" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="800" t="s">
+      <c r="A8" s="876" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="800" t="s">
+      <c r="B8" s="876" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="800" t="s">
+      <c r="C8" s="876" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="800" t="s">
+      <c r="D8" s="876" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="800" t="s">
+      <c r="E8" s="876" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="800" t="s">
+      <c r="F8" s="876" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="800" t="s">
+      <c r="G8" s="876" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="800" t="s">
+      <c r="H8" s="876" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="801" t="s">
+      <c r="A9" s="877" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="801" t="s">
+      <c r="B9" s="877" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="801" t="s">
+      <c r="C9" s="877" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="801" t="s">
+      <c r="D9" s="877" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="801" t="s">
+      <c r="E9" s="877" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="801" t="s">
+      <c r="F9" s="877" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="801" t="s">
+      <c r="G9" s="877" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="801" t="s">
+      <c r="H9" s="877" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="802" t="s">
+      <c r="A10" s="878" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="802" t="s">
+      <c r="B10" s="878" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="802" t="s">
+      <c r="C10" s="878" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="802" t="s">
+      <c r="D10" s="878" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="802" t="s">
+      <c r="E10" s="878" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="802" t="s">
+      <c r="F10" s="878" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="802" t="s">
+      <c r="G10" s="878" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="802" t="s">
+      <c r="H10" s="878" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="803" t="s">
+      <c r="A11" s="879" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="803" t="s">
+      <c r="B11" s="879" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="803" t="s">
+      <c r="C11" s="879" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="803" t="s">
+      <c r="D11" s="879" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="803" t="s">
+      <c r="E11" s="879" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="803" t="s">
+      <c r="F11" s="879" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="803" t="s">
+      <c r="G11" s="879" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="803" t="s">
+      <c r="H11" s="879" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="880" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="880" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="880" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="880" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="880" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="880" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="880" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="880" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added additional steps to the PageContent feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="35">
   <si>
     <t>URL</t>
   </si>
@@ -159,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -254,11 +254,101 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -315,6 +405,66 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -624,7 +774,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,106 +816,106 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="37" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="38" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="39" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
splitted the verification of brands and brand groups
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="35">
   <si>
     <t>URL</t>
   </si>
@@ -159,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="90">
     <border>
       <left/>
       <right/>
@@ -344,11 +344,245 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -465,6 +699,162 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -816,106 +1206,106 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="88" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="89" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="90" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="91" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improved the performance and added the data sheet automatic clearance
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5952"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5952" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="TestData" r:id="rId6" sheetId="4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="44">
   <si>
     <t>URL</t>
   </si>
@@ -39,12 +39,122 @@
   </si>
   <si>
     <t>BREADCRUMBSLINKS</t>
+  </si>
+  <si>
+    <t>META DESCRIPTION</t>
+  </si>
+  <si>
+    <t>BREADCRUMBS TEXT</t>
+  </si>
+  <si>
+    <t>BREADCRUMBS LINKS</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/no.+famous+cigars</t>
+  </si>
+  <si>
+    <t># Famous Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>#Famous cigars are a unique aromatic blend created for cigar smokers who enjoy flavor-infused cigars. Using a secret Nicaraguan tobacco blend, the smoke is...</t>
+  </si>
+  <si>
+    <t># Famous Cigars</t>
+  </si>
+  <si>
+    <t>#Famous cigars are a unique aromatic blend created for cigar smokers who enjoy flavor-infused cigars. Using a secret Nicaraguan tobacco blend, the smoke is ultra-mellow and hits you with a fragrant mélange of vanilla, caramel, and sweet coffee &amp; cream. Made in 2 sizes - Toro and Petite Corona - presented in a refillable vacuum-sealed humidor jar for guaranteed freshness, you'll be as surprised by the low price as you will by their awesome bouquet. Get your #Famous cigar shape now and #goforit!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » # Famous Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/1502+cigars</t>
+  </si>
+  <si>
+    <t>1502 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Searching for 1502 Cigars on sale? Save big when you shop our complete selection now at Famous Smoke Shop!</t>
+  </si>
+  <si>
+    <t>1502 Cigars</t>
+  </si>
+  <si>
+    <t>Years of blending, generations of expertise and centuries of tradition have all factored into the making of great cigars — and 1502 Cigars is no exception. Innovation, passion and development by companies such as theirs have been key in the effort to bring you the best cigar smoking experience known to man since he first rolled up a leaf and smoked it. And it’s hard to argue that with hard work like this, the premium cigar world is now the best it’s ever been. They’re committed to delighting the senses each and every time you set flame to the foot, with your preferences in mind. And that’s the beauty of all of the premium cigars on sale at Famous Smoke Shop — fitting all ranges of tastes, likes and prices, there is truly a cigar for everyone here at Famous.
+... more</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 1502 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars/,https://www.famous-smoke.com/cigar-brand-list/</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+black+gold+cigars</t>
+  </si>
+  <si>
+    <t>1502 Black Gold Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Black Gold cigars are artisan-crafted premiums made in Estelí, Nicaragua. Created for savvy cigar smokers who crave dark, robust and complex tobacco...</t>
+  </si>
+  <si>
+    <t>1502 Black Gold Cigars</t>
+  </si>
+  <si>
+    <t>1502 Black Gold cigars are artisan-crafted premiums made in Estelí, Nicaragua. Created for savvy cigar smokers who crave dark, robust and complex tobacco flavor, these BOX-PRESSED Nicaraguans boast a sun-grown maduro wrapper that lends a hearty character to this multi-faceted blend. The smoke simmers with earthy, nutty, woody notes, a pinch of chili pepper, plus subtly sweet chocolate and fruity notes. Price reasonably, try some of these fine boutique cigars today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Black Gold Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/1502+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+emerald+cigars</t>
+  </si>
+  <si>
+    <t>1502 Emerald Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery...</t>
+  </si>
+  <si>
+    <t>1502 Emerald Cigars</t>
+  </si>
+  <si>
+    <t>1502 Emerald cigars are masterfully-crafted by hand in Estelí, Nicaragua. What you have here is a complex, medium-bodied cigar BOX-PRESSED in shimmery Nicaragua Corojo wrappers that cap a carefully selected blend of Mexican San Andres long-fillers, plus Nicaraguan Estelí &amp; Condega tobaccos. Velvety smoke reveals delicate apple and other citrusy elements, plus a dash of sweet cedar, as the aroma lends fragrances of honey, vanilla and floral notes. Order some of these fine cigars today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Emerald Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+nicaragua+cigars</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua cigars are super-premium, boutique selection from Nicaragua. Medium-full in body, these BOX-PRESSED puros boast master-level craftsmanship...</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua Cigars</t>
+  </si>
+  <si>
+    <t>1502 Nicaragua cigars are super-premium, boutique selection from Nicaragua. Medium-full in body, these BOX-PRESSED puros boast master-level craftsmanship using a blend of perfectly-aged long-filler tobaccos from Esteli, Condega, Jalapa, and Ometepe. Expect a velvety smooth, medium-full smoke multi-layered with fruity, nutty and floral notes, plus a dash of Ometepe spice, enhanced by aromas of honey and vanilla. Reasonably-priced, too. Try these distinctive cigars by ordering some today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Nicaragua Cigars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -62,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,8 +185,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -99,11 +239,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -113,6 +361,114 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,58 +772,6 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A1186"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="34.77734375" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.77734375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.77734375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.21875" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="64.5546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="50" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="53.77734375" style="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -478,4 +782,183 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
restructured the steps and features. added basic header seo
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="44">
   <si>
     <t>URL</t>
   </si>
@@ -172,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,8 +215,53 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -347,11 +392,173 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -468,6 +675,114 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="37" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="41" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="45" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="53" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="57" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="61" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -795,7 +1110,7 @@
     <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
@@ -803,158 +1118,106 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="72" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="73" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="39" t="s">
+      <c r="H4" s="75" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
major restructuring of the Testing Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="44">
   <si>
     <t>URL</t>
   </si>
@@ -172,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +260,33 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="62">
+  <borders count="82">
     <border>
       <left/>
       <right/>
@@ -554,11 +579,101 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -783,6 +898,66 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="65" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="69" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="73" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="77" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="81" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1118,106 +1293,106 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="92" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="93" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="74" t="s">
+      <c r="F3" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="94" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="75" t="s">
+      <c r="E4" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="75" t="s">
+      <c r="F4" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="G4" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="75" t="s">
+      <c r="H4" s="95" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Major changes in the Test Framework now working in a more static scripted way
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="47">
   <si>
     <t>URL</t>
   </si>
@@ -148,6 +148,16 @@
   </si>
   <si>
     <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Nicaragua Cigars</t>
+  </si>
+  <si>
+    <t># FAMOUS CIGARS</t>
+  </si>
+  <si>
+    <t>1502 CIGARS</t>
+  </si>
+  <si>
+    <t>Years of blending, generations of expertise and centuries of tradition have all factored into the making of great cigars — and 1502 Cigars is no exception. Innovation, passion and development by companies such as theirs have been key in the effort to bring you the best cigar smoking experience known to man since he first rolled up a leaf and smoked it. And it’s hard to argue that with hard work like this, the premium cigar world is now the best it’s ever been. They’re committed to delighting the senses each and every time you set flame to the foot, with your preferences in mind. And that’s the beauty of all of the premium cigars on sale at Famous Smoke Shop — fitting all ranges of tastes, likes and prices, there is truly a cigar for everyone here at Famous.
+You share our passion for a good cigar; and here, like every smoke we sell, when you buy 1502 Cigars online from Famous Smoke Shop you’re assured a flavorful experience, backed by our freshness guarantee. Buy 1502 Cigars on sale now, with confidence — and you’ll be telling your friends, “Here’s my new favorite thing from Famous Smoke Shop…”</t>
   </si>
 </sst>
 </file>
@@ -172,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,8 +295,63 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="82">
+  <borders count="126">
     <border>
       <left/>
       <right/>
@@ -669,11 +734,209 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -958,6 +1221,123 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="85" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="89" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="93" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="97" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="101" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="101" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="101" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="105" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="105" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="105" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="109" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="109" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="109" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="113" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="113" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="113" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="117" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="117" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="117" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="121" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="121" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="121" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="125" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="125" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="125" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1282,118 +1662,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="54.546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="54.546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="31.0078125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="17.7265625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="81.71875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="114.3515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="92" t="s">
+      <c r="H1" s="132" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="133" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="93" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="93" t="s">
+      <c r="E2" s="133" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="133" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="94" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="94" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="94" t="s">
+      <c r="E3" s="134" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="134" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="134" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="94" t="s">
+      <c r="H3" s="134" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="95" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="95" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="95" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="95" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="95" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the testconfig for webdriver instantation and support for chrome and firefox
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="47">
   <si>
     <t>URL</t>
   </si>
@@ -182,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,8 +350,28 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="126">
+  <borders count="142">
     <border>
       <left/>
       <right/>
@@ -932,11 +952,83 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1338,6 +1430,42 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="125" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="129" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="129" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="129" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="133" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="133" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="133" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="137" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="137" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="137" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="141" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="141" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="141" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1673,80 +1801,80 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="132" t="s">
+      <c r="C1" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="132" t="s">
+      <c r="D1" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="132" t="s">
+      <c r="E1" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="132" t="s">
+      <c r="F1" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="132" t="s">
+      <c r="G1" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="132" t="s">
+      <c r="H1" s="144" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="133" t="s">
+      <c r="C2" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="133" t="s">
+      <c r="D2" s="145" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="133" t="s">
+      <c r="E2" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="133" t="s">
+      <c r="F2" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="133" t="s">
+      <c r="G2" s="145" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="133" t="s">
+      <c r="H2" s="145" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="134" t="s">
+      <c r="A3" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="134" t="s">
+      <c r="B3" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="134" t="s">
+      <c r="D3" s="146" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="134" t="s">
+      <c r="E3" s="146" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="134" t="s">
+      <c r="F3" s="146" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="134" t="s">
+      <c r="G3" s="146" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="134" t="s">
+      <c r="H3" s="146" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed the properties files
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="47">
   <si>
     <t>URL</t>
   </si>
@@ -182,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,8 +370,18 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="142">
+  <borders count="150">
     <border>
       <left/>
       <right/>
@@ -1024,11 +1034,47 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1466,6 +1512,24 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="141" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="145" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="145" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="145" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="149" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="149" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="149" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1801,80 +1865,80 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="144" t="s">
+      <c r="B1" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="144" t="s">
+      <c r="C1" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="144" t="s">
+      <c r="D1" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="144" t="s">
+      <c r="E1" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="144" t="s">
+      <c r="G1" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="144" t="s">
+      <c r="H1" s="150" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="145" t="s">
+      <c r="C2" s="151" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="145" t="s">
+      <c r="D2" s="151" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="145" t="s">
+      <c r="E2" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="145" t="s">
+      <c r="F2" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="145" t="s">
+      <c r="G2" s="151" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="145" t="s">
+      <c r="H2" s="151" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="152" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="152" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="152" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="152" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="146" t="s">
+      <c r="E3" s="152" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="146" t="s">
+      <c r="F3" s="152" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="146" t="s">
+      <c r="G3" s="152" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="146" t="s">
+      <c r="H3" s="152" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
incremented the maximum crawls
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="47">
   <si>
     <t>URL</t>
   </si>
@@ -182,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,8 +385,18 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="154">
+  <borders count="162">
     <border>
       <left/>
       <right/>
@@ -1093,11 +1103,47 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1562,6 +1608,24 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="153" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="157" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="157" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="157" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="161" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="161" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="161" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1890,87 +1954,87 @@
     <col min="2" max="2" width="54.546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="31.0078125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.48046875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="17.7265625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="81.71875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="114.3515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="153" t="s">
+      <c r="B1" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="153" t="s">
+      <c r="C1" s="159" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="153" t="s">
+      <c r="D1" s="159" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="153" t="s">
+      <c r="E1" s="159" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="153" t="s">
+      <c r="F1" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="153" t="s">
+      <c r="G1" s="159" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="153" t="s">
+      <c r="H1" s="159" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="160" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="160" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154" t="s">
+      <c r="C2" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="154" t="s">
+      <c r="D2" s="160" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="154" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="154" t="s">
+      <c r="E2" s="160" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="160" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="154" t="s">
+      <c r="G2" s="160" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="154" t="s">
+      <c r="H2" s="160" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="161" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="155" t="s">
+      <c r="B3" s="161" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="155" t="s">
+      <c r="C3" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="155" t="s">
+      <c r="D3" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="155" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="155" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="155" t="s">
+      <c r="E3" s="161" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="161" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="161" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="155" t="s">
+      <c r="H3" s="161" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added support to the remote driver instantiation
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="47">
   <si>
     <t>URL</t>
   </si>
@@ -182,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,8 +395,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="162">
+  <borders count="166">
     <border>
       <left/>
       <right/>
@@ -1139,11 +1144,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1626,6 +1649,15 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="161" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="165" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="165" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="165" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1961,80 +1993,80 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="159" t="s">
+      <c r="B1" s="162" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="159" t="s">
+      <c r="C1" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="159" t="s">
+      <c r="D1" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="159" t="s">
+      <c r="E1" s="162" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="159" t="s">
+      <c r="F1" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="159" t="s">
+      <c r="G1" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="159" t="s">
+      <c r="H1" s="162" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="160" t="s">
+      <c r="C2" s="163" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="163" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="160" t="s">
+      <c r="E2" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="160" t="s">
+      <c r="F2" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="160" t="s">
+      <c r="G2" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="160" t="s">
+      <c r="H2" s="163" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="161" t="s">
+      <c r="D3" s="164" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="161" t="s">
+      <c r="E3" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="161" t="s">
+      <c r="F3" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="161" t="s">
+      <c r="G3" s="164" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="161" t="s">
+      <c r="H3" s="164" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added support to cucumber reports jenkins plugin
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="47">
   <si>
     <t>URL</t>
   </si>
@@ -182,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,8 +400,33 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="166">
+  <borders count="186">
     <border>
       <left/>
       <right/>
@@ -1162,11 +1187,101 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1658,6 +1773,51 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="165" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="169" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="169" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="169" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="173" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="173" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="173" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="177" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="177" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="177" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="181" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="181" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="181" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="185" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="185" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="185" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1986,87 +2146,87 @@
     <col min="2" max="2" width="54.546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="31.0078125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="17.7265625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.48046875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="81.71875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="114.3515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="177" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="162" t="s">
+      <c r="C1" s="177" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="162" t="s">
+      <c r="D1" s="177" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="162" t="s">
+      <c r="E1" s="177" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="162" t="s">
+      <c r="F1" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="162" t="s">
+      <c r="G1" s="177" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="162" t="s">
+      <c r="H1" s="177" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="163" t="s">
+      <c r="A2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="163" t="s">
+      <c r="D2" s="178" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="163" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="163" t="s">
+      <c r="E2" s="178" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="178" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="163" t="s">
+      <c r="G2" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="163" t="s">
+      <c r="H2" s="178" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="164" t="s">
+      <c r="B3" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="164" t="s">
+      <c r="D3" s="179" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="164" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="164" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="164" t="s">
+      <c r="E3" s="179" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="179" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="179" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="164" t="s">
+      <c r="H3" s="179" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Separated the setup and processed features run, added annotation to the features and improved the FeaturesProcessor
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3080" uniqueCount="140">
   <si>
     <t>URL</t>
   </si>
@@ -158,6 +158,296 @@
   <si>
     <t>Years of blending, generations of expertise and centuries of tradition have all factored into the making of great cigars — and 1502 Cigars is no exception. Innovation, passion and development by companies such as theirs have been key in the effort to bring you the best cigar smoking experience known to man since he first rolled up a leaf and smoked it. And it’s hard to argue that with hard work like this, the premium cigar world is now the best it’s ever been. They’re committed to delighting the senses each and every time you set flame to the foot, with your preferences in mind. And that’s the beauty of all of the premium cigars on sale at Famous Smoke Shop — fitting all ranges of tastes, likes and prices, there is truly a cigar for everyone here at Famous.
 You share our passion for a good cigar; and here, like every smoke we sell, when you buy 1502 Cigars online from Famous Smoke Shop you’re assured a flavorful experience, backed by our freshness guarantee. Buy 1502 Cigars on sale now, with confidence — and you’ll be telling your friends, “Here’s my new favorite thing from Famous Smoke Shop…”</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1502+ruby+cigars</t>
+  </si>
+  <si>
+    <t>1502 Ruby Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1502 Ruby cigars are an artisan quality selection handcrafted in Estelí, Nicaragua. These aesthetically appealing cigars offer you a medium-full blend of...</t>
+  </si>
+  <si>
+    <t>1502 Ruby Cigars</t>
+  </si>
+  <si>
+    <t>1502 Ruby cigars are an artisan quality selection handcrafted in Estelí, Nicaragua. These aesthetically appealing cigars offer you a medium-full blend of the most select Nicaraguan Estelí &amp; Jalapa tobaccos BOX-PRESSED in an attractively dark, oily Cuban-seed wrapper grown in Ecuador. The smoke is exceptionally well-balanced, serving-up an earthy-woody flavor profile with notes of sweet cedar and toasted nuts. Try this real gem of a cigar by adding some to your cart today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 1502 Brands » 1502 Ruby Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/1994+by+la+flor+dominicana+cigars</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana holds a very special meaning to the company that brought you some of the highest rated cigars year after year. The 1994...</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana Cigars</t>
+  </si>
+  <si>
+    <t>1994 By La Flor Dominicana holds a very special meaning to the company that brought you some of the highest rated cigars year after year. The 1994 commemorates Litto and Ines Gomez's 20th year with the LFD cigar brand they created. Dominican longfillers and binders are dressed in an oily Mexican San Andres natural wrapper, with 4 sizes to choose from. If you're a fan of LFD, you should only expect yet another cigar with stellar flavor and a full bodied strength profile. Get yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All La Flor Dominicana Brands » 1994 By La Flor Dominicana Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/la+flor+dominicana+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/262+cigars</t>
+  </si>
+  <si>
+    <t>262 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 cigars for sale at Famous Smoke Shop's online cigar store. These boutique cigars present a revolution in premium cigar quality, taste, and complexity.</t>
+  </si>
+  <si>
+    <t>262 Cigars</t>
+  </si>
+  <si>
+    <t>The brainchild of Clint Aaron and Mike Justice, 262 Cigars is a collective of premium cigar brands that have been riding the new wave of boutique cigars into the marketplace since 2010. The name stands for February 1962, the month and year that President John F. Kennedy signed the Cuban Trade Embargo. It also stands for something more than just really good cigars; it stands for a new paradigm and an ideology to which Aaron and Justice have assigned the slogan, "Smoke the Revolution."
+No revolution would be complete without a manifesto, and the 262 Manifesto is a call to action for cigar smokers to band together and tell local, state, and federal government officials that they will not stand for excessive tobacco taxation and unconstitutional smoking bans. "I believe in the constitution and fully trust what the founders setup for us," says Mike Justice. "Our Ideologies are the foundations of how we live our lives, the decisions we make, and the people we associate with."
+Made in Honduras Paradigm cigars start with Nicaraguan Seco and Ligero tobaccos from Estelí and Jalapa, a Colombian Cuban-seed Cubito leaf, and a Honduran binder wrapped in a luscious Brazilian Mata Fina leaf that pulls everything together to deliver a creamy, complex, and medium-full smoke that exhibits notes of citrus, coffee, pepper, cedar, cocoa and sweet tobacco.
+Our Ideologies are what make us who we are, and 262 Ideology cigars represent the passion to create great cigars, the fortitude to transcend the opposition, and the resolve to smoke free. Using a mild 3-nation core blend rolled in flawless Nicaraguan Habano Rosado wrappers, the 262 Ideology will ring home with your palate and remind you what is was about cigars that made you fall in love with them. Their effortless draw offers a toasty, buttery, and creamy-smooth smoke that pledges to put your troubles on "hold" for a most relaxing experience.
+During the events leading up to our nation's revolution, Paul Revere was among those who answered the call for freedom with selfless courage, and made his mark on history. That passion is reflected in the 262 Revere cigars selection. If you love the bold taste of Nicaraguan puros, the Revere selection embraces a blend of long-fillers from Estelí, Condega, and Jalapa rolled in a glossy and naturally sweet-tasting Jalapa wrapper. The smoke is full-bodied, offering a multitude of floral and herbal notes with citrus peel, cocoa, and spice in the mix, making the 262 Revere a marvelous choice for lovers of the best Nicaraguan cigars.
+While all of the above brands have a cigar revolution theme, 262 Allegiance cigars takes a stronger tone. State by state, town by town, and at the Federal level, too, there is a growing opposition to our cigar culture, and it's time to take a side. So, in an effort to thwart those efforts, Clint Aaron has created a medium-bodied cigar that will appeal to cigar smokers at every level. Made in Estelí, Nicaragua, Allegiance marries Nicaraguan and Honduran long-fillers to an oily Brazilian Mata Fina wrapper for a satisfying smoke with an exotic mix of spice, citrus, and earthy flavors. If you want a cigar made with outstanding quality and taste, turn your allegiance to this selection.
+"</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 262 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+allegiance+cigars</t>
+  </si>
+  <si>
+    <t>262 Allegiance Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>I pledge allegiance to the cigar called 262 Allegiance. Originally planned as a seasonal blend, Allegiance was met with such an enthusiastic response the...</t>
+  </si>
+  <si>
+    <t>262 Allegiance Cigars</t>
+  </si>
+  <si>
+    <t>I pledge allegiance to the cigar called 262 Allegiance. Originally planned as a seasonal blend, Allegiance was met with such an enthusiastic response the company decided to make it a full production cigar handcrafted at Tabacalera Carreras factory in Esteli, Nicaragua with a Brazilian Mata Fina wrapper, Nicaraguan binder and a Honduran-Nicaraguan filler blend. Expect an effortless, enjoyable, and very affordable smoke that's mild to medium in body, yet very rich in flavor. Order yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Allegiance Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/262+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+ideology+cigars</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262...</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars</t>
+  </si>
+  <si>
+    <t>262 Ideology Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Ideology is Mild yet complex smoke with Nicaraguan, Mexican, and Dominican fillers, a Nicaraguan binder, and a Nicaraguan Habano Rosado wrapper that ads a buttery creaminess to an outstanding smoke. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Ideology Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+paradigm+cigars</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262...</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars</t>
+  </si>
+  <si>
+    <t>262 Paradigm Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Paradigm is a medium to full bodied complex smoke with Nicaraguan and rare Colombian fillers, a Honduran binder, and a rich and creamy Brazilian Mata Fina wrapper. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Paradigm Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/262+revere+1+cigars</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is...</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars</t>
+  </si>
+  <si>
+    <t>262 Revere Cigars represent the bold new wave of the cigar industry. Cigars are getting bolder, more flavorful, and a heck of a lot more complex and 262 is coming to the front of the pack. The Revere is a full bodied Nicaraguan Puro with a blend of fillers from Esteli, Jalapa, and Condega, a binder with Esteli and Jalapa tobaccos, and a Jalapa Valley wrapper. The result is a complex and bold cigar packed with unbelievable flavor. Step into the future of cigars and pick some up today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 262 Brands » 262 Revere Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/4th+generation+pipe+accessories</t>
+  </si>
+  <si>
+    <t>4th Generation Pipe | Famous Smoke</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>4th Generation Pipe</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Accessories » Accessories » Tobacco Brand List » 4th Generation Pipe</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/accessories,https://www.famous-smoke.com/tobacco-brand-list</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/6+pack+samplers+cigars</t>
+  </si>
+  <si>
+    <t>6 Pack Cigar Samplers | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Sure, you're used to seeing cigars presented in 5-packs, but we've taken them one step beyond in this delicious series of 6-Packs presented in a wide...</t>
+  </si>
+  <si>
+    <t>6 Pack Cigar Samplers</t>
+  </si>
+  <si>
+    <t>Sure, you're used to seeing cigars presented in 5-packs, but we've taken them one step beyond in this delicious series of 6-Packs presented in a wide variety of strengths, wrappers, and even a couple of coffee flavored combos. Starring the bestselling cigars in the business at nice prices, now you can get a 6-pack without working out. Browse through the list now and order the Best Sellers 6-Packs that are right for you. There's no better or thriftier way to own great cigars!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » 6 Pack Cigar Samplers</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/601+cigars</t>
+  </si>
+  <si>
+    <t>601 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>601 Cigars is known within the industry as being some of the most delicious, well made, heavy hitting smokes around. Famous offers discount prices on 601 Cigars</t>
+  </si>
+  <si>
+    <t>601 Cigars</t>
+  </si>
+  <si>
+    <t>601 Cigars is known throughout the industry as being some of the most delicious, well made, heavy hitting stogies around. Making use of virtually every priming of numerous types of tobacco, Erik Espinosa along with then partner Eddie Ortega blended and released the 601 cigar line in the mid 2000s with the infamous Blue, Red, and Green labels. From there, the brand only kept expanding with the La Bomba and Warhead. Now you can have your own slice of stogie heaven with Famous Smoke Shop discount prices on all lines of this wonderful cigar. Get yours today from our massive inventory and save today!
+About 601 Cigars
+At the age of 3 months old, Erik Espinosa and his family moved to Miami in search of a more prosperous life. Of course, being only 3 months old, it was hard for him to find any work, but we all agree here that he had a lot of ambition to make such a drastic move at such a young age. As he got older, he adopted his passion for cigars from his father who worked in the industry, and in 1997 began his career in this highly competitive market. Gaining knowledge from leading cigar manufacturers such as Alec Bradley, Gurkha, Rocky Patel, and Drew Estate, Erik soaked in as much information as he could to learn every single detail he can to prepare himself when the time came that he would open his own factory.
+Finally, in 2004, Mr. Espinosa along with former partner Eddie Ortega, EO Brands was formed, and the 601 Cigars line was born with innovative new blends not seen in any other line before. They were one of the first companies to incorporate a Mexican San Andreas wrapper in their blends which started a massive trend in using this inexpensive and flavorful tobacco. For close to a decade, Erik Espinosa released new blends consistently, but he really hit his stride in 2012 with the birth of La Zona Premium Cigar Company. This gave him complete power to create even more blends on his own and re-release cigars he had made over at EO Brands.
+Now working with his son Erik Jr., Mr. Espinosa has had nothing but success reaching cigar lovers both young and old with 601 cigars being one of the main attractions. Lines like the 601 Blue Label and 601 Green label has been filling older cigar smoker’s humidors for over a decade now, with 601 La Bomba and Warhead appealing to a younger market of full strength, full bodied smokers. But no matter what a customer prefers, La Zona has a stogie to satisfy anyone’s craving.
+Now you can experience 601 Cigars at massively discounted prices made available through Famous Smoke Shop and its large inventory. Famous Smoke Shop holds the most cigars in stock through buying from each of it’s suppliers directly, ensuring you get the cigars you want in any size available. Get your 601 Cigars today from Famous and save money on these premium hand rolled stogies.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 601 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+accesories+and+samplers+cigars</t>
+  </si>
+  <si>
+    <t>601 Accesories And Cigar Samplers | Famous Smoke</t>
+  </si>
+  <si>
+    <t>601 cigars were originally created by Amilcar Perez-Castro in August of 2006, and have since taken off like wildfire. Now manufactured at Tavicusa S.A in...</t>
+  </si>
+  <si>
+    <t>601 Accesories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>601 cigars were originally created by Amilcar Perez-Castro in August of 2006, and have since taken off like wildfire. Now manufactured at Tavicusa S.A in Estelí, Nicaragua under the direction of Erik Espinosa, since its debut, the 601 series has received heaps of praise from cigar media and cigar smokers alike. Ranging from medium to full-bodied, the line offers something wonderful for even the most discerning palates. Try one of these supreme selections today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Accesories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/601+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+blue+label+cigars</t>
+  </si>
+  <si>
+    <t>601 Blue Label Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>The 601 'Blue' cigar series are slightly box-pressed, medium to full-bodied premium cigars. Manufactured by Tavicusa S.A., they boast an exquisite recipe...</t>
+  </si>
+  <si>
+    <t>601 Blue Label Cigars</t>
+  </si>
+  <si>
+    <t>The 601 'Blue' cigar series are slightly box-pressed, medium to full-bodied premium cigars. Manufactured by Tavicusa S.A., they boast an exquisite recipe of perfectly-aged Nicaraguan longfillers finished in a dark Nicaraguan Habano wrapper. Precisely blended to offer a rich, well-balanced medley of dark and naturally sweet tobacco flavors enhanced by an arousing aroma, if you prefer taste over strength, this is the 601 for you. Make sure you have a box on-hand for those special occasions.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Blue Label Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+green+label+oscuro+cigars</t>
+  </si>
+  <si>
+    <t>601 Green Label Oscuro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>The 601 'Green' cigar series comprises a full-bodied blend created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan long-filler...</t>
+  </si>
+  <si>
+    <t>601 Green Label Oscuro Cigars</t>
+  </si>
+  <si>
+    <t>The 601 'Green' cigar series comprises a full-bodied blend created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan long-filler tobaccos. Rolled in an exquisite Nicaraguan Habano Oscuro wrapper leaf, these puros are, by far, among the most full-flavored in the 601 series. Each cigar is precisely blended to offer a well-balanced, robust smoke brimming with juicy, complex flavors. If you crave big, bold flavor and aroma in your cigars, add a box to your cart now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Green Label Oscuro Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+la+bomba+1+cigars</t>
+  </si>
+  <si>
+    <t>601 La Bomba Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Calling this new addition to the highly-acclaimed 601 cigars selection The Bomb is an understatement. The blend consists of an all-Nicaraguan longfiller &amp;...</t>
+  </si>
+  <si>
+    <t>601 La Bomba Cigars</t>
+  </si>
+  <si>
+    <t>Calling this new addition to the highly-acclaimed 601 cigars selection The Bomb is an understatement. The blend consists of an all-Nicaraguan longfiller &amp; binder core rolled in a savory Habano wrapper leaf. If you love lots'a Ligero, you'll enjoy this explosive, extra-strength smoke in a Nicaraguan puro format. Presented in boxes of 10 cigars spanning several popular sizes, La Bomba is chock full of dark, spicy tobacco flavor. Order your box now (Experienced smokers preferred).</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 La Bomba Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+red+label+habano+cigars</t>
+  </si>
+  <si>
+    <t>601 Red Label Habano Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>601 Red Label cigars are full-bodied premium cigars created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan longfillers topped...</t>
+  </si>
+  <si>
+    <t>601 Red Label Habano Cigars</t>
+  </si>
+  <si>
+    <t>601 Red Label cigars are full-bodied premium cigars created by Amilcar Perez Castro with an exquisite blend of perfectly-aged Nicaraguan longfillers topped with an attractively oily Nicaraguan Natural Habano wrapper. The 601 'Red' is blended for the experienced cigar smoker providing a stunning mosaic of well-balanced flavors, while maintaining its complex flavor profile from start to finish with an enticing aroma. If you love robust and peppery Nicaraguan puros, order a box or a 5-pack now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Red Label Habano Cigars</t>
   </si>
 </sst>
 </file>
@@ -182,7 +472,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="65">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,8 +715,88 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="186">
+  <borders count="250">
     <border>
       <left/>
       <right/>
@@ -1277,11 +1647,299 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="388">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1818,6 +2476,630 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="185" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="189" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="189" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="189" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="193" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="193" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="193" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="197" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="197" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="197" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="201" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="201" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="201" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="205" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="205" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="205" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="54" borderId="209" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="209" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="209" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="55" borderId="213" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="217" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="221" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="225" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="229" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="233" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="237" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="62" borderId="241" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="245" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="64" borderId="249" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -2142,92 +3424,560 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="54.546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="54.546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="31.0078125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.48046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="71.23046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="71.23046875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="47.58203125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="145.84375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="32.0546875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="81.71875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="114.3515625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="126.45703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="178.8125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="367" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177" t="s">
+      <c r="B1" s="367" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="177" t="s">
+      <c r="C1" s="367" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="177" t="s">
+      <c r="D1" s="367" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="177" t="s">
+      <c r="E1" s="367" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="177" t="s">
+      <c r="F1" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="177" t="s">
+      <c r="G1" s="367" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="177" t="s">
+      <c r="H1" s="367" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="178" t="s">
+      <c r="A2" s="368" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="368" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="368" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="178" t="s">
+      <c r="D2" s="368" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="178" t="s">
+      <c r="E2" s="368" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="178" t="s">
+      <c r="F2" s="368" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="178" t="s">
+      <c r="G2" s="368" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="178" t="s">
+      <c r="H2" s="368" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="179" t="s">
+      <c r="A3" s="369" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="369" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="179" t="s">
+      <c r="C3" s="369" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="179" t="s">
+      <c r="D3" s="369" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="179" t="s">
+      <c r="E3" s="369" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="179" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="179" t="s">
+      <c r="F3" s="369" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="369" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="179" t="s">
+      <c r="H3" s="369" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="370" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="370" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="370" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="370" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="370" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="370" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="370" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="370" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="371" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="371" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="371" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="371" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="371" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="371" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="371" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="371" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="372" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="372" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="372" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="372" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="372" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="372" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="372" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="372" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="373" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="373" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="373" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="373" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="373" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="373" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="373" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="373" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="374" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="374" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="374" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="374" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="374" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="374" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="374" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="374" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="375" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="375" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="375" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="375" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="375" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="375" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="375" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="375" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="376" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="376" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="376" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="376" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="376" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="376" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="376" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="376" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="377" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="377" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="377" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="377" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="377" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="377" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="377" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="377" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="378" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="378" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="378" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="378" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="378" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="378" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="378" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="378" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="379" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="379" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="379" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="379" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="379" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="379" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="379" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="379" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="380" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="380" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="380" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="380" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="380" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="380" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="380" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="380" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="381" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="381" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="381" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="381" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="381" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="381" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="381" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="381" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="382" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="382" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="382" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="382" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="382" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="382" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="382" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" s="382" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="383" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="383" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="383" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="383" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="383" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="383" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="383" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" s="383" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="384" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="384" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="384" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="384" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="384" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="384" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="384" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" s="384" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="385" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="385" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="385" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="385" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="385" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="385" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" s="385" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="385" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="386" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="386" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="386" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="386" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="386" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="386" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="386" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="386" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="387" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="387" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="387" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="387" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="387" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="387" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="387" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="387" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed dependency of allure
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3080" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3248" uniqueCount="140">
   <si>
     <t>URL</t>
   </si>
@@ -472,7 +472,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="65">
+  <fills count="66">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,8 +795,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="250">
+  <borders count="254">
     <border>
       <left/>
       <right/>
@@ -1935,11 +1940,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="388">
+  <cellXfs count="409">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3100,6 +3123,69 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="65" borderId="253" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3435,548 +3521,548 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="367" t="s">
+      <c r="A1" s="388" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="367" t="s">
+      <c r="B1" s="388" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="367" t="s">
+      <c r="C1" s="388" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="367" t="s">
+      <c r="D1" s="388" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="367" t="s">
+      <c r="E1" s="388" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="367" t="s">
+      <c r="F1" s="388" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="367" t="s">
+      <c r="G1" s="388" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="367" t="s">
+      <c r="H1" s="388" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="368" t="s">
+      <c r="A2" s="389" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="368" t="s">
+      <c r="B2" s="389" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="368" t="s">
+      <c r="C2" s="389" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="368" t="s">
+      <c r="D2" s="389" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="368" t="s">
+      <c r="E2" s="389" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="368" t="s">
+      <c r="F2" s="389" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="368" t="s">
+      <c r="G2" s="389" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="368" t="s">
+      <c r="H2" s="389" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="369" t="s">
+      <c r="A3" s="390" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="369" t="s">
+      <c r="B3" s="390" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="369" t="s">
+      <c r="C3" s="390" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="369" t="s">
+      <c r="D3" s="390" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="369" t="s">
+      <c r="E3" s="390" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="369" t="s">
+      <c r="F3" s="390" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="369" t="s">
+      <c r="G3" s="390" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="369" t="s">
+      <c r="H3" s="390" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="370" t="s">
+      <c r="A4" s="391" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="370" t="s">
+      <c r="B4" s="391" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="370" t="s">
+      <c r="C4" s="391" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="370" t="s">
+      <c r="D4" s="391" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="370" t="s">
+      <c r="E4" s="391" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="370" t="s">
+      <c r="F4" s="391" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="370" t="s">
+      <c r="G4" s="391" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="370" t="s">
+      <c r="H4" s="391" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="371" t="s">
+      <c r="A5" s="392" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="371" t="s">
+      <c r="B5" s="392" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="371" t="s">
+      <c r="C5" s="392" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="371" t="s">
+      <c r="D5" s="392" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="371" t="s">
+      <c r="E5" s="392" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="371" t="s">
+      <c r="F5" s="392" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="371" t="s">
+      <c r="G5" s="392" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="371" t="s">
+      <c r="H5" s="392" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="372" t="s">
+      <c r="A6" s="393" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="372" t="s">
+      <c r="B6" s="393" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="372" t="s">
+      <c r="C6" s="393" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="372" t="s">
+      <c r="D6" s="393" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="372" t="s">
+      <c r="E6" s="393" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="372" t="s">
+      <c r="F6" s="393" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="372" t="s">
+      <c r="G6" s="393" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="372" t="s">
+      <c r="H6" s="393" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="373" t="s">
+      <c r="A7" s="394" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="373" t="s">
+      <c r="B7" s="394" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="373" t="s">
+      <c r="C7" s="394" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="373" t="s">
+      <c r="D7" s="394" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="373" t="s">
+      <c r="E7" s="394" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="373" t="s">
+      <c r="F7" s="394" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="373" t="s">
+      <c r="G7" s="394" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="373" t="s">
+      <c r="H7" s="394" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="374" t="s">
+      <c r="A8" s="395" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="374" t="s">
+      <c r="B8" s="395" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="374" t="s">
+      <c r="C8" s="395" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="374" t="s">
+      <c r="D8" s="395" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="374" t="s">
+      <c r="E8" s="395" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="374" t="s">
+      <c r="F8" s="395" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="374" t="s">
+      <c r="G8" s="395" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="374" t="s">
+      <c r="H8" s="395" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="375" t="s">
+      <c r="A9" s="396" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="375" t="s">
+      <c r="B9" s="396" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="375" t="s">
+      <c r="C9" s="396" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="375" t="s">
+      <c r="D9" s="396" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="375" t="s">
+      <c r="E9" s="396" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="375" t="s">
+      <c r="F9" s="396" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="375" t="s">
+      <c r="G9" s="396" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="375" t="s">
+      <c r="H9" s="396" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="376" t="s">
+      <c r="A10" s="397" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="376" t="s">
+      <c r="B10" s="397" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="376" t="s">
+      <c r="C10" s="397" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="376" t="s">
+      <c r="D10" s="397" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="376" t="s">
+      <c r="E10" s="397" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="376" t="s">
+      <c r="F10" s="397" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="376" t="s">
+      <c r="G10" s="397" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="376" t="s">
+      <c r="H10" s="397" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="377" t="s">
+      <c r="A11" s="398" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="377" t="s">
+      <c r="B11" s="398" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="377" t="s">
+      <c r="C11" s="398" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="377" t="s">
+      <c r="D11" s="398" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="377" t="s">
+      <c r="E11" s="398" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="377" t="s">
+      <c r="F11" s="398" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="377" t="s">
+      <c r="G11" s="398" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="377" t="s">
+      <c r="H11" s="398" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="378" t="s">
+      <c r="A12" s="399" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="378" t="s">
+      <c r="B12" s="399" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="378" t="s">
+      <c r="C12" s="399" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="378" t="s">
+      <c r="D12" s="399" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="378" t="s">
+      <c r="E12" s="399" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="378" t="s">
+      <c r="F12" s="399" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="378" t="s">
+      <c r="G12" s="399" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="378" t="s">
+      <c r="H12" s="399" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="379" t="s">
+      <c r="A13" s="400" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="379" t="s">
+      <c r="B13" s="400" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="379" t="s">
+      <c r="C13" s="400" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="379" t="s">
+      <c r="D13" s="400" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="379" t="s">
+      <c r="E13" s="400" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="379" t="s">
+      <c r="F13" s="400" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="379" t="s">
+      <c r="G13" s="400" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="379" t="s">
+      <c r="H13" s="400" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="380" t="s">
+      <c r="A14" s="401" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="380" t="s">
+      <c r="B14" s="401" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="380" t="s">
+      <c r="C14" s="401" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="380" t="s">
+      <c r="D14" s="401" t="s">
         <v>93</v>
       </c>
-      <c r="E14" s="380" t="s">
+      <c r="E14" s="401" t="s">
         <v>94</v>
       </c>
-      <c r="F14" s="380" t="s">
+      <c r="F14" s="401" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="380" t="s">
+      <c r="G14" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="H14" s="380" t="s">
+      <c r="H14" s="401" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="381" t="s">
+      <c r="A15" s="402" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="381" t="s">
+      <c r="B15" s="402" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="381" t="s">
+      <c r="C15" s="402" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="381" t="s">
+      <c r="D15" s="402" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="381" t="s">
+      <c r="E15" s="402" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="381" t="s">
+      <c r="F15" s="402" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="381" t="s">
+      <c r="G15" s="402" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="381" t="s">
+      <c r="H15" s="402" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="382" t="s">
+      <c r="A16" s="403" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="382" t="s">
+      <c r="B16" s="403" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="382" t="s">
+      <c r="C16" s="403" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="382" t="s">
+      <c r="D16" s="403" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="382" t="s">
+      <c r="E16" s="403" t="s">
         <v>106</v>
       </c>
-      <c r="F16" s="382" t="s">
+      <c r="F16" s="403" t="s">
         <v>107</v>
       </c>
-      <c r="G16" s="382" t="s">
+      <c r="G16" s="403" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="382" t="s">
+      <c r="H16" s="403" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="383" t="s">
+      <c r="A17" s="404" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="383" t="s">
+      <c r="B17" s="404" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="383" t="s">
+      <c r="C17" s="404" t="s">
         <v>110</v>
       </c>
-      <c r="D17" s="383" t="s">
+      <c r="D17" s="404" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="383" t="s">
+      <c r="E17" s="404" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="383" t="s">
+      <c r="F17" s="404" t="s">
         <v>113</v>
       </c>
-      <c r="G17" s="383" t="s">
+      <c r="G17" s="404" t="s">
         <v>114</v>
       </c>
-      <c r="H17" s="383" t="s">
+      <c r="H17" s="404" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="384" t="s">
+      <c r="A18" s="405" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="384" t="s">
+      <c r="B18" s="405" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="384" t="s">
+      <c r="C18" s="405" t="s">
         <v>117</v>
       </c>
-      <c r="D18" s="384" t="s">
+      <c r="D18" s="405" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="384" t="s">
+      <c r="E18" s="405" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="384" t="s">
+      <c r="F18" s="405" t="s">
         <v>120</v>
       </c>
-      <c r="G18" s="384" t="s">
+      <c r="G18" s="405" t="s">
         <v>121</v>
       </c>
-      <c r="H18" s="384" t="s">
+      <c r="H18" s="405" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="385" t="s">
+      <c r="A19" s="406" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="385" t="s">
+      <c r="B19" s="406" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="385" t="s">
+      <c r="C19" s="406" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="385" t="s">
+      <c r="D19" s="406" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="385" t="s">
+      <c r="E19" s="406" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="385" t="s">
+      <c r="F19" s="406" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="385" t="s">
+      <c r="G19" s="406" t="s">
         <v>127</v>
       </c>
-      <c r="H19" s="385" t="s">
+      <c r="H19" s="406" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="386" t="s">
+      <c r="A20" s="407" t="s">
         <v>128</v>
       </c>
-      <c r="B20" s="386" t="s">
+      <c r="B20" s="407" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="386" t="s">
+      <c r="C20" s="407" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="386" t="s">
+      <c r="D20" s="407" t="s">
         <v>130</v>
       </c>
-      <c r="E20" s="386" t="s">
+      <c r="E20" s="407" t="s">
         <v>131</v>
       </c>
-      <c r="F20" s="386" t="s">
+      <c r="F20" s="407" t="s">
         <v>132</v>
       </c>
-      <c r="G20" s="386" t="s">
+      <c r="G20" s="407" t="s">
         <v>133</v>
       </c>
-      <c r="H20" s="386" t="s">
+      <c r="H20" s="407" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="387" t="s">
+      <c r="A21" s="408" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="387" t="s">
+      <c r="B21" s="408" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="387" t="s">
+      <c r="C21" s="408" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="387" t="s">
+      <c r="D21" s="408" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="387" t="s">
+      <c r="E21" s="408" t="s">
         <v>137</v>
       </c>
-      <c r="F21" s="387" t="s">
+      <c r="F21" s="408" t="s">
         <v>138</v>
       </c>
-      <c r="G21" s="387" t="s">
+      <c r="G21" s="408" t="s">
         <v>139</v>
       </c>
-      <c r="H21" s="387" t="s">
+      <c r="H21" s="408" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed the cucumber.json generation
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3248" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3416" uniqueCount="140">
   <si>
     <t>URL</t>
   </si>
@@ -472,7 +472,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="66">
+  <fills count="67">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,8 +800,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="254">
+  <borders count="258">
     <border>
       <left/>
       <right/>
@@ -1958,11 +1963,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="409">
+  <cellXfs count="430">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3186,6 +3209,69 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="66" borderId="257" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3521,548 +3607,548 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="388" t="s">
+      <c r="A1" s="409" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="388" t="s">
+      <c r="B1" s="409" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="388" t="s">
+      <c r="C1" s="409" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="388" t="s">
+      <c r="D1" s="409" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="388" t="s">
+      <c r="E1" s="409" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="388" t="s">
+      <c r="F1" s="409" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="388" t="s">
+      <c r="G1" s="409" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="388" t="s">
+      <c r="H1" s="409" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="389" t="s">
+      <c r="A2" s="410" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="389" t="s">
+      <c r="B2" s="410" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="389" t="s">
+      <c r="C2" s="410" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="389" t="s">
+      <c r="D2" s="410" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="389" t="s">
+      <c r="E2" s="410" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="389" t="s">
+      <c r="F2" s="410" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="389" t="s">
+      <c r="G2" s="410" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="389" t="s">
+      <c r="H2" s="410" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="390" t="s">
+      <c r="A3" s="411" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="390" t="s">
+      <c r="B3" s="411" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="390" t="s">
+      <c r="C3" s="411" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="390" t="s">
+      <c r="D3" s="411" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="390" t="s">
+      <c r="E3" s="411" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="390" t="s">
+      <c r="F3" s="411" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="390" t="s">
+      <c r="G3" s="411" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="390" t="s">
+      <c r="H3" s="411" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="391" t="s">
+      <c r="A4" s="412" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="391" t="s">
+      <c r="B4" s="412" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="391" t="s">
+      <c r="C4" s="412" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="391" t="s">
+      <c r="D4" s="412" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="391" t="s">
+      <c r="E4" s="412" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="391" t="s">
+      <c r="F4" s="412" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="391" t="s">
+      <c r="G4" s="412" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="391" t="s">
+      <c r="H4" s="412" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="392" t="s">
+      <c r="A5" s="413" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="392" t="s">
+      <c r="B5" s="413" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="392" t="s">
+      <c r="C5" s="413" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="392" t="s">
+      <c r="D5" s="413" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="392" t="s">
+      <c r="E5" s="413" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="392" t="s">
+      <c r="F5" s="413" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="392" t="s">
+      <c r="G5" s="413" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="392" t="s">
+      <c r="H5" s="413" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="393" t="s">
+      <c r="A6" s="414" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="393" t="s">
+      <c r="B6" s="414" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="393" t="s">
+      <c r="C6" s="414" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="393" t="s">
+      <c r="D6" s="414" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="393" t="s">
+      <c r="E6" s="414" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="393" t="s">
+      <c r="F6" s="414" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="393" t="s">
+      <c r="G6" s="414" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="393" t="s">
+      <c r="H6" s="414" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="394" t="s">
+      <c r="A7" s="415" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="394" t="s">
+      <c r="B7" s="415" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="394" t="s">
+      <c r="C7" s="415" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="394" t="s">
+      <c r="D7" s="415" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="394" t="s">
+      <c r="E7" s="415" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="394" t="s">
+      <c r="F7" s="415" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="394" t="s">
+      <c r="G7" s="415" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="394" t="s">
+      <c r="H7" s="415" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="395" t="s">
+      <c r="A8" s="416" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="395" t="s">
+      <c r="B8" s="416" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="395" t="s">
+      <c r="C8" s="416" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="395" t="s">
+      <c r="D8" s="416" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="395" t="s">
+      <c r="E8" s="416" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="395" t="s">
+      <c r="F8" s="416" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="395" t="s">
+      <c r="G8" s="416" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="395" t="s">
+      <c r="H8" s="416" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="396" t="s">
+      <c r="A9" s="417" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="396" t="s">
+      <c r="B9" s="417" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="396" t="s">
+      <c r="C9" s="417" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="396" t="s">
+      <c r="D9" s="417" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="396" t="s">
+      <c r="E9" s="417" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="396" t="s">
+      <c r="F9" s="417" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="396" t="s">
+      <c r="G9" s="417" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="396" t="s">
+      <c r="H9" s="417" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="397" t="s">
+      <c r="A10" s="418" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="397" t="s">
+      <c r="B10" s="418" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="397" t="s">
+      <c r="C10" s="418" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="397" t="s">
+      <c r="D10" s="418" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="397" t="s">
+      <c r="E10" s="418" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="397" t="s">
+      <c r="F10" s="418" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="397" t="s">
+      <c r="G10" s="418" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="397" t="s">
+      <c r="H10" s="418" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="398" t="s">
+      <c r="A11" s="419" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="398" t="s">
+      <c r="B11" s="419" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="398" t="s">
+      <c r="C11" s="419" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="398" t="s">
+      <c r="D11" s="419" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="398" t="s">
+      <c r="E11" s="419" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="398" t="s">
+      <c r="F11" s="419" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="398" t="s">
+      <c r="G11" s="419" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="398" t="s">
+      <c r="H11" s="419" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="399" t="s">
+      <c r="A12" s="420" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="399" t="s">
+      <c r="B12" s="420" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="399" t="s">
+      <c r="C12" s="420" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="399" t="s">
+      <c r="D12" s="420" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="399" t="s">
+      <c r="E12" s="420" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="399" t="s">
+      <c r="F12" s="420" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="399" t="s">
+      <c r="G12" s="420" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="399" t="s">
+      <c r="H12" s="420" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="400" t="s">
+      <c r="A13" s="421" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="400" t="s">
+      <c r="B13" s="421" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="400" t="s">
+      <c r="C13" s="421" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="400" t="s">
+      <c r="D13" s="421" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="400" t="s">
+      <c r="E13" s="421" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="400" t="s">
+      <c r="F13" s="421" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="400" t="s">
+      <c r="G13" s="421" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="400" t="s">
+      <c r="H13" s="421" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="401" t="s">
+      <c r="A14" s="422" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="401" t="s">
+      <c r="B14" s="422" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="401" t="s">
+      <c r="C14" s="422" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="401" t="s">
+      <c r="D14" s="422" t="s">
         <v>93</v>
       </c>
-      <c r="E14" s="401" t="s">
+      <c r="E14" s="422" t="s">
         <v>94</v>
       </c>
-      <c r="F14" s="401" t="s">
+      <c r="F14" s="422" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="401" t="s">
+      <c r="G14" s="422" t="s">
         <v>95</v>
       </c>
-      <c r="H14" s="401" t="s">
+      <c r="H14" s="422" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="402" t="s">
+      <c r="A15" s="423" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="402" t="s">
+      <c r="B15" s="423" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="402" t="s">
+      <c r="C15" s="423" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="402" t="s">
+      <c r="D15" s="423" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="402" t="s">
+      <c r="E15" s="423" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="402" t="s">
+      <c r="F15" s="423" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="402" t="s">
+      <c r="G15" s="423" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="402" t="s">
+      <c r="H15" s="423" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="403" t="s">
+      <c r="A16" s="424" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="403" t="s">
+      <c r="B16" s="424" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="403" t="s">
+      <c r="C16" s="424" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="403" t="s">
+      <c r="D16" s="424" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="403" t="s">
+      <c r="E16" s="424" t="s">
         <v>106</v>
       </c>
-      <c r="F16" s="403" t="s">
+      <c r="F16" s="424" t="s">
         <v>107</v>
       </c>
-      <c r="G16" s="403" t="s">
+      <c r="G16" s="424" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="403" t="s">
+      <c r="H16" s="424" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="404" t="s">
+      <c r="A17" s="425" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="404" t="s">
+      <c r="B17" s="425" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="404" t="s">
+      <c r="C17" s="425" t="s">
         <v>110</v>
       </c>
-      <c r="D17" s="404" t="s">
+      <c r="D17" s="425" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="404" t="s">
+      <c r="E17" s="425" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="404" t="s">
+      <c r="F17" s="425" t="s">
         <v>113</v>
       </c>
-      <c r="G17" s="404" t="s">
+      <c r="G17" s="425" t="s">
         <v>114</v>
       </c>
-      <c r="H17" s="404" t="s">
+      <c r="H17" s="425" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="405" t="s">
+      <c r="A18" s="426" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="405" t="s">
+      <c r="B18" s="426" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="405" t="s">
+      <c r="C18" s="426" t="s">
         <v>117</v>
       </c>
-      <c r="D18" s="405" t="s">
+      <c r="D18" s="426" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="405" t="s">
+      <c r="E18" s="426" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="405" t="s">
+      <c r="F18" s="426" t="s">
         <v>120</v>
       </c>
-      <c r="G18" s="405" t="s">
+      <c r="G18" s="426" t="s">
         <v>121</v>
       </c>
-      <c r="H18" s="405" t="s">
+      <c r="H18" s="426" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="406" t="s">
+      <c r="A19" s="427" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="406" t="s">
+      <c r="B19" s="427" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="406" t="s">
+      <c r="C19" s="427" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="406" t="s">
+      <c r="D19" s="427" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="406" t="s">
+      <c r="E19" s="427" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="406" t="s">
+      <c r="F19" s="427" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="406" t="s">
+      <c r="G19" s="427" t="s">
         <v>127</v>
       </c>
-      <c r="H19" s="406" t="s">
+      <c r="H19" s="427" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="407" t="s">
+      <c r="A20" s="428" t="s">
         <v>128</v>
       </c>
-      <c r="B20" s="407" t="s">
+      <c r="B20" s="428" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="407" t="s">
+      <c r="C20" s="428" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="407" t="s">
+      <c r="D20" s="428" t="s">
         <v>130</v>
       </c>
-      <c r="E20" s="407" t="s">
+      <c r="E20" s="428" t="s">
         <v>131</v>
       </c>
-      <c r="F20" s="407" t="s">
+      <c r="F20" s="428" t="s">
         <v>132</v>
       </c>
-      <c r="G20" s="407" t="s">
+      <c r="G20" s="428" t="s">
         <v>133</v>
       </c>
-      <c r="H20" s="407" t="s">
+      <c r="H20" s="428" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="408" t="s">
+      <c r="A21" s="429" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="408" t="s">
+      <c r="B21" s="429" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="408" t="s">
+      <c r="C21" s="429" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="408" t="s">
+      <c r="D21" s="429" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="408" t="s">
+      <c r="E21" s="429" t="s">
         <v>137</v>
       </c>
-      <c r="F21" s="408" t="s">
+      <c r="F21" s="429" t="s">
         <v>138</v>
       </c>
-      <c r="G21" s="408" t="s">
+      <c r="G21" s="429" t="s">
         <v>139</v>
       </c>
-      <c r="H21" s="408" t="s">
+      <c r="H21" s="429" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
repositioned the features templates and the processed features folders
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3416" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3560" uniqueCount="142">
   <si>
     <t>URL</t>
   </si>
@@ -448,6 +448,19 @@
   </si>
   <si>
     <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Red Label Habano Cigars</t>
+  </si>
+  <si>
+    <t>Buy 1502 cigars online at discount prices. Famous has 1502 Emerald, 1502 Ruby, 1502 Nicaragua, and 1502 Black Gold cigars, guaranteed fresh and in stock.</t>
+  </si>
+  <si>
+    <t>1502 cigars are ready to take their place alongside many of the best Nicaraguan cigars you can buy. Presented in a variety of meticulously handcrafted blends that appeal to cigar smokers of every experience, these boutique cigars offer superb quality and taste in a limited number of box-pressed sizes in four savory selections. At the heart of the 1502 brand are the three core lines: the 1502 Emerald, 1502 Ruby, and 1502 Black Gold. Each cigar is unique in character and designed to be enjoyed morning, noon, and night, starting with the medium-bodied Emerald, followed by the more full-flavored Ruby, and concluding with the full-bodied Black Gold. Of course, the choice is yours as to when you choose to revel in their rich Nicaraguan flavor, but whichever 1502 cigar you buy, you're in for a truly satisfying and unforgettable experience.
+Launched in 2012 by native Nicaraguan, Enrique Sanchez Icaza, founder and CEO of Global Premium Cigars, 1502 Cigars were given their numerical name to commemorate the year Christopher Columbus discovered Nicaragua. Upon his arrival, Columbus also discovered a new world full of riches such as gold, silver, and precious stones for which the 1502 Emerald, Ruby, and Black Gold selections are named. But most importantly was the discovery of tobacco, which was used as a high value form of trade currency virtually equal to that of the Spanish Doubloon.
+"In our premium brand 1502, you will find three tobacco lines with the highest quality, where the sowing process, harvest, curing, aging and selection of each tobacco leaf is our major concern," says Señor Sanchez. "It takes more than five years, from the time the seeds are sown until the time you can enjoy one of our fine cigars; this is why patience is one of our greatest virtues in the art of tobacco production."
+1502 Emerald cigars yield a subtle strength and velvety smooth flavor that is achieved by a blend of long fillers from Estelí, Condega, and Mexico's San Andres valley pressed in a mouthwatering Nicaraguan Corojo Habano wrapper leaf. Delicate flavors of citrus, cedar, and roasted nut form the base, as aromas of honey, vanilla and floral notes drift amid the thick, creamy smoke.
+1502 Ruby cigars were created to delight discerning smokers who seek more body and complexity from their cigars. A lusciously dark Ecuadorian wrapper surrounds a well-balanced blend of fully-aged tobaccos from Estelí and Jalapa, for a medium-bodied, full-flavored smoke brimming with earthy elements, sweet cedar, and subtle hints of macadamia nuts and sunflower seeds.
+1502 Black Gold cigars bring on the muscle, full-tilt, for cigar smokers who enjoy extra bold tobacco flavor from end-to-end. A diverse Nicaraguan core is bound in two additional leaves, and finished in a maduro wrapper that's been nurtured by the sun to achieve the peak of flavor. Earthy-woody flavors abound as a layer of chili pepper works its way in, complemented by a delicate, chocolatey-fruity sweetness for a resounding multidimensional smoke.
+1502 Nicaragua cigars boast an "all-inclusive" Nicaraguan blend that uses tobaccos from Nicaragua's four main growing regions: Estelí, Jalapa, Condega, and Ometepe. Medium-full in body, this cigar's flavor profile fits somewhere between the 1502 Emerald and 1502 Ruby offering a velvety smoothness and amazing balance. The smoke is earthy and woody with some fruity elements, enhanced by a toasty, honeyed aroma.
+With so many wonderful blends to choose from, there's a 1502 cigar in your future. Browse the selections and find the 1502 cigar that's right for you – right now!</t>
   </si>
 </sst>
 </file>
@@ -472,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="67">
+  <fills count="70">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,8 +818,23 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="258">
+  <borders count="270">
     <border>
       <left/>
       <right/>
@@ -1981,11 +2009,65 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="430">
+  <cellXfs count="448">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3272,6 +3354,60 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="67" borderId="261" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="261" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="261" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="261" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="261" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="261" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="68" borderId="265" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="69" borderId="269" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="269" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="269" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="269" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="269" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="269" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3596,560 +3732,170 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="71.23046875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="71.23046875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="47.58203125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="145.84375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="32.0546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="126.45703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="178.8125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="409" t="s">
+      <c r="A1" s="442" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="409" t="s">
+      <c r="B1" s="442" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="409" t="s">
+      <c r="C1" s="442" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="409" t="s">
+      <c r="D1" s="442" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="409" t="s">
+      <c r="E1" s="442" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="409" t="s">
+      <c r="F1" s="442" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="409" t="s">
+      <c r="G1" s="442" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="409" t="s">
+      <c r="H1" s="442" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="410" t="s">
+      <c r="A2" s="443" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="410" t="s">
+      <c r="B2" s="443" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="410" t="s">
+      <c r="C2" s="443" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="410" t="s">
+      <c r="D2" s="443" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="410" t="s">
+      <c r="E2" s="443" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="410" t="s">
+      <c r="F2" s="443" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="410" t="s">
+      <c r="G2" s="443" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="410" t="s">
+      <c r="H2" s="443" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="411" t="s">
+      <c r="A3" s="444" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="411" t="s">
+      <c r="B3" s="444" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="411" t="s">
+      <c r="C3" s="444" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="411" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="411" t="s">
+      <c r="D3" s="444" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="444" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="411" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="411" t="s">
+      <c r="F3" s="444" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="444" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="411" t="s">
+      <c r="H3" s="444" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="412" t="s">
+      <c r="A4" s="445" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="412" t="s">
+      <c r="B4" s="445" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="412" t="s">
+      <c r="C4" s="445" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="412" t="s">
+      <c r="D4" s="445" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="412" t="s">
+      <c r="E4" s="445" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="412" t="s">
+      <c r="F4" s="445" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="412" t="s">
+      <c r="G4" s="445" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="412" t="s">
+      <c r="H4" s="445" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="413" t="s">
+      <c r="A5" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="413" t="s">
+      <c r="B5" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="413" t="s">
+      <c r="C5" s="446" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="413" t="s">
+      <c r="D5" s="446" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="413" t="s">
+      <c r="E5" s="446" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="413" t="s">
+      <c r="F5" s="446" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="413" t="s">
+      <c r="G5" s="446" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="413" t="s">
+      <c r="H5" s="446" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="414" t="s">
+      <c r="A6" s="447" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="414" t="s">
+      <c r="B6" s="447" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="414" t="s">
+      <c r="C6" s="447" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="414" t="s">
+      <c r="D6" s="447" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="414" t="s">
+      <c r="E6" s="447" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="414" t="s">
+      <c r="F6" s="447" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="414" t="s">
+      <c r="G6" s="447" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="414" t="s">
+      <c r="H6" s="447" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="415" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="415" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="415" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="415" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="415" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="415" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="415" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="415" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="416" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="416" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="416" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="416" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="416" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="416" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="416" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="416" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="417" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="417" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="417" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="417" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="417" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="417" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="417" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="417" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="418" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="418" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="418" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="418" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="418" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="418" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="418" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="418" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="419" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="419" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="419" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="419" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="419" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="419" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="419" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="419" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="420" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="420" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="420" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="420" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="420" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="420" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="420" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="420" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="421" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="421" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="421" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="421" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="421" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="421" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="421" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="421" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="422" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="422" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="422" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="422" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="422" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="422" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" s="422" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" s="422" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="423" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="423" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="423" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="423" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="423" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="423" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="423" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="423" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="424" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="424" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="424" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="424" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="424" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="424" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="424" t="s">
-        <v>108</v>
-      </c>
-      <c r="H16" s="424" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="425" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="425" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="425" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="425" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="425" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="425" t="s">
-        <v>113</v>
-      </c>
-      <c r="G17" s="425" t="s">
-        <v>114</v>
-      </c>
-      <c r="H17" s="425" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="426" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" s="426" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="426" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="426" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="426" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="426" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="426" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" s="426" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="427" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" s="427" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="427" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="427" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="427" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="427" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" s="427" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="427" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="428" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="428" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="428" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="428" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="428" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="428" t="s">
-        <v>132</v>
-      </c>
-      <c r="G20" s="428" t="s">
-        <v>133</v>
-      </c>
-      <c r="H20" s="428" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="429" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="429" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="429" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="429" t="s">
-        <v>136</v>
-      </c>
-      <c r="E21" s="429" t="s">
-        <v>137</v>
-      </c>
-      <c r="F21" s="429" t="s">
-        <v>138</v>
-      </c>
-      <c r="G21" s="429" t="s">
-        <v>139</v>
-      </c>
-      <c r="H21" s="429" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the jenkins scripts processed features path
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3560" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3608" uniqueCount="142">
   <si>
     <t>URL</t>
   </si>
@@ -485,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="70">
+  <fills count="71">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,8 +833,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="270">
+  <borders count="274">
     <border>
       <left/>
       <right/>
@@ -2063,11 +2068,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="448">
+  <cellXfs count="454">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3408,6 +3431,24 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="269" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="70" borderId="273" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="273" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="273" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="273" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="273" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="273" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3743,158 +3784,158 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="442" t="s">
+      <c r="A1" s="448" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="442" t="s">
+      <c r="B1" s="448" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="442" t="s">
+      <c r="C1" s="448" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="442" t="s">
+      <c r="D1" s="448" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="442" t="s">
+      <c r="E1" s="448" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="442" t="s">
+      <c r="F1" s="448" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="442" t="s">
+      <c r="G1" s="448" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="442" t="s">
+      <c r="H1" s="448" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="443" t="s">
+      <c r="A2" s="449" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="443" t="s">
+      <c r="B2" s="449" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="443" t="s">
+      <c r="C2" s="449" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="443" t="s">
+      <c r="D2" s="449" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="443" t="s">
+      <c r="E2" s="449" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="443" t="s">
+      <c r="F2" s="449" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="443" t="s">
+      <c r="G2" s="449" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="443" t="s">
+      <c r="H2" s="449" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="444" t="s">
+      <c r="A3" s="450" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="444" t="s">
+      <c r="B3" s="450" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="444" t="s">
+      <c r="C3" s="450" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="444" t="s">
+      <c r="D3" s="450" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="444" t="s">
+      <c r="E3" s="450" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="444" t="s">
+      <c r="F3" s="450" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="444" t="s">
+      <c r="G3" s="450" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="444" t="s">
+      <c r="H3" s="450" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="445" t="s">
+      <c r="A4" s="451" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="445" t="s">
+      <c r="B4" s="451" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="445" t="s">
+      <c r="C4" s="451" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="445" t="s">
+      <c r="D4" s="451" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="445" t="s">
+      <c r="E4" s="451" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="445" t="s">
+      <c r="F4" s="451" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="445" t="s">
+      <c r="G4" s="451" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="445" t="s">
+      <c r="H4" s="451" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="446" t="s">
+      <c r="A5" s="452" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="446" t="s">
+      <c r="B5" s="452" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="446" t="s">
+      <c r="C5" s="452" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="446" t="s">
+      <c r="D5" s="452" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="446" t="s">
+      <c r="E5" s="452" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="446" t="s">
+      <c r="F5" s="452" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="446" t="s">
+      <c r="G5" s="452" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="446" t="s">
+      <c r="H5" s="452" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="447" t="s">
+      <c r="A6" s="453" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="447" t="s">
+      <c r="B6" s="453" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="447" t="s">
+      <c r="C6" s="453" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="447" t="s">
+      <c r="D6" s="453" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="447" t="s">
+      <c r="E6" s="453" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="447" t="s">
+      <c r="F6" s="453" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="447" t="s">
+      <c r="G6" s="453" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="447" t="s">
+      <c r="H6" s="453" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
segmented the tests in different runners
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3608" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3704" uniqueCount="142">
   <si>
     <t>URL</t>
   </si>
@@ -485,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="71">
+  <fills count="74">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,8 +838,23 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="274">
+  <borders count="286">
     <border>
       <left/>
       <right/>
@@ -2086,11 +2101,65 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="454">
+  <cellXfs count="466">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3449,6 +3518,42 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="273" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="71" borderId="277" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="277" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="277" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="277" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="277" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="277" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="72" borderId="281" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="73" borderId="285" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="285" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="285" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3773,170 +3878,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="54.546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="54.546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="31.0078125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.48046875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="81.71875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="114.3515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="448" t="s">
+      <c r="A1" s="463" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="448" t="s">
+      <c r="B1" s="463" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="448" t="s">
+      <c r="C1" s="463" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="448" t="s">
+      <c r="D1" s="463" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="448" t="s">
+      <c r="E1" s="463" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="448" t="s">
+      <c r="F1" s="463" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="448" t="s">
+      <c r="G1" s="463" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="448" t="s">
+      <c r="H1" s="463" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="449" t="s">
+      <c r="A2" s="464" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="449" t="s">
+      <c r="B2" s="464" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="449" t="s">
+      <c r="C2" s="464" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="449" t="s">
+      <c r="D2" s="464" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="449" t="s">
+      <c r="E2" s="464" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="449" t="s">
+      <c r="F2" s="464" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="449" t="s">
+      <c r="G2" s="464" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="449" t="s">
+      <c r="H2" s="464" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="450" t="s">
+      <c r="A3" s="465" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="450" t="s">
+      <c r="B3" s="465" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="450" t="s">
+      <c r="C3" s="465" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="450" t="s">
+      <c r="D3" s="465" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="450" t="s">
+      <c r="E3" s="465" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="450" t="s">
+      <c r="F3" s="465" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="450" t="s">
+      <c r="G3" s="465" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="450" t="s">
+      <c r="H3" s="465" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="451" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="451" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="451" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="451" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="451" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="451" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="451" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="451" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="452" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="452" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="452" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="452" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="452" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="452" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="452" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="452" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="453" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="453" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="453" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="453" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="453" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="453" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="453" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="453" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the pretty html cucumber report
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3704" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3728" uniqueCount="142">
   <si>
     <t>URL</t>
   </si>
@@ -485,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="74">
+  <fills count="75">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -853,8 +853,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="286">
+  <borders count="290">
     <border>
       <left/>
       <right/>
@@ -2155,11 +2160,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="466">
+  <cellXfs count="469">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3554,6 +3577,15 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="285" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="74" borderId="289" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="289" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="289" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3889,80 +3921,80 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="463" t="s">
+      <c r="A1" s="466" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="463" t="s">
+      <c r="B1" s="466" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="463" t="s">
+      <c r="C1" s="466" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="463" t="s">
+      <c r="D1" s="466" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="463" t="s">
+      <c r="E1" s="466" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="463" t="s">
+      <c r="F1" s="466" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="463" t="s">
+      <c r="G1" s="466" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="463" t="s">
+      <c r="H1" s="466" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="464" t="s">
+      <c r="A2" s="467" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="464" t="s">
+      <c r="B2" s="467" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="464" t="s">
+      <c r="C2" s="467" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="464" t="s">
+      <c r="D2" s="467" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="464" t="s">
+      <c r="E2" s="467" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="464" t="s">
+      <c r="F2" s="467" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="464" t="s">
+      <c r="G2" s="467" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="464" t="s">
+      <c r="H2" s="467" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="465" t="s">
+      <c r="A3" s="468" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="465" t="s">
+      <c r="B3" s="468" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="465" t="s">
+      <c r="C3" s="468" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="465" t="s">
+      <c r="D3" s="468" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="465" t="s">
+      <c r="E3" s="468" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="465" t="s">
+      <c r="F3" s="468" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="465" t="s">
+      <c r="G3" s="468" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="465" t="s">
+      <c r="H3" s="468" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made collections even more generalized
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3728" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3776" uniqueCount="142">
   <si>
     <t>URL</t>
   </si>
@@ -485,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="75">
+  <fills count="77">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -858,8 +858,18 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="290">
+  <borders count="298">
     <border>
       <left/>
       <right/>
@@ -2178,11 +2188,47 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="469">
+  <cellXfs count="475">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3586,6 +3632,24 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="289" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="75" borderId="293" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="76" borderId="297" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="297" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="297" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3921,80 +3985,80 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="466" t="s">
+      <c r="A1" s="472" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="466" t="s">
+      <c r="B1" s="472" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="466" t="s">
+      <c r="C1" s="472" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="466" t="s">
+      <c r="D1" s="472" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="466" t="s">
+      <c r="E1" s="472" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="466" t="s">
+      <c r="F1" s="472" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="466" t="s">
+      <c r="G1" s="472" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="466" t="s">
+      <c r="H1" s="472" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="467" t="s">
+      <c r="A2" s="473" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="467" t="s">
+      <c r="B2" s="473" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="467" t="s">
+      <c r="C2" s="473" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="467" t="s">
+      <c r="D2" s="473" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="467" t="s">
+      <c r="E2" s="473" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="467" t="s">
+      <c r="F2" s="473" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="467" t="s">
+      <c r="G2" s="473" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="467" t="s">
+      <c r="H2" s="473" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="468" t="s">
+      <c r="A3" s="474" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="468" t="s">
+      <c r="B3" s="474" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="468" t="s">
+      <c r="C3" s="474" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="468" t="s">
+      <c r="D3" s="474" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="468" t="s">
+      <c r="E3" s="474" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="468" t="s">
+      <c r="F3" s="474" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="468" t="s">
+      <c r="G3" s="474" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="468" t="s">
+      <c r="H3" s="474" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the scenarioid field in the examples to fix the allure reporting
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3776" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4016" uniqueCount="142">
   <si>
     <t>URL</t>
   </si>
@@ -485,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="77">
+  <fills count="82">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -868,8 +868,33 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="298">
+  <borders count="318">
     <border>
       <left/>
       <right/>
@@ -2224,11 +2249,101 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="475">
+  <cellXfs count="505">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3650,6 +3765,96 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="297" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="77" borderId="301" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="301" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="301" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="301" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="301" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="301" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="78" borderId="305" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="305" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="305" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="305" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="305" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="305" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="79" borderId="309" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="80" borderId="313" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="313" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="313" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="313" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="313" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="313" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="81" borderId="317" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="317" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="317" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="317" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="317" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="317" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -3974,92 +4179,170 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="54.546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="54.546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="31.0078125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.48046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="81.71875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="114.3515625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="472" t="s">
+      <c r="A1" s="499" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="472" t="s">
+      <c r="B1" s="499" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="472" t="s">
+      <c r="C1" s="499" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="472" t="s">
+      <c r="D1" s="499" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="472" t="s">
+      <c r="E1" s="499" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="472" t="s">
+      <c r="F1" s="499" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="472" t="s">
+      <c r="G1" s="499" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="472" t="s">
+      <c r="H1" s="499" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="473" t="s">
+      <c r="A2" s="500" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="473" t="s">
+      <c r="B2" s="500" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="473" t="s">
+      <c r="C2" s="500" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="473" t="s">
+      <c r="D2" s="500" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="473" t="s">
+      <c r="E2" s="500" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="473" t="s">
+      <c r="F2" s="500" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="473" t="s">
+      <c r="G2" s="500" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="473" t="s">
+      <c r="H2" s="500" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="474" t="s">
+      <c r="A3" s="501" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="474" t="s">
+      <c r="B3" s="501" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="474" t="s">
+      <c r="C3" s="501" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="474" t="s">
+      <c r="D3" s="501" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="474" t="s">
+      <c r="E3" s="501" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="474" t="s">
+      <c r="F3" s="501" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="474" t="s">
+      <c r="G3" s="501" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="474" t="s">
+      <c r="H3" s="501" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="502" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="502" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="502" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="502" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="502" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="502" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="502" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="502" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="503" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="503" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="503" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="503" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="503" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="503" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="503" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="503" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="504" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="504" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="504" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="504" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="504" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="504" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="504" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="504" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added custom assertions and the brand logo and video validation
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4016" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4104" uniqueCount="142">
   <si>
     <t>URL</t>
   </si>
@@ -485,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="82">
+  <fills count="83">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,8 +893,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="318">
+  <borders count="322">
     <border>
       <left/>
       <right/>
@@ -2339,11 +2344,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="505">
+  <cellXfs count="516">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3855,6 +3878,39 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="317" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="82" borderId="321" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -4179,170 +4235,300 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="70.01171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="70.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="46.9609375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="31.43359375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="126.45703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="178.8125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="499" t="s">
+      <c r="A1" s="505" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="499" t="s">
+      <c r="B1" s="505" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="499" t="s">
+      <c r="C1" s="505" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="499" t="s">
+      <c r="D1" s="505" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="499" t="s">
+      <c r="E1" s="505" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="499" t="s">
+      <c r="F1" s="505" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="499" t="s">
+      <c r="G1" s="505" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="499" t="s">
+      <c r="H1" s="505" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="500" t="s">
+      <c r="A2" s="506" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="500" t="s">
+      <c r="B2" s="506" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="500" t="s">
+      <c r="C2" s="506" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="500" t="s">
+      <c r="D2" s="506" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="500" t="s">
+      <c r="E2" s="506" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="500" t="s">
+      <c r="F2" s="506" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="500" t="s">
+      <c r="G2" s="506" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="500" t="s">
+      <c r="H2" s="506" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="501" t="s">
+      <c r="A3" s="507" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="501" t="s">
+      <c r="B3" s="507" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="501" t="s">
+      <c r="C3" s="507" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="501" t="s">
+      <c r="D3" s="507" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="501" t="s">
+      <c r="E3" s="507" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="501" t="s">
+      <c r="F3" s="507" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="501" t="s">
+      <c r="G3" s="507" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="501" t="s">
+      <c r="H3" s="507" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="502" t="s">
+      <c r="A4" s="508" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="502" t="s">
+      <c r="B4" s="508" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="502" t="s">
+      <c r="C4" s="508" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="502" t="s">
+      <c r="D4" s="508" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="502" t="s">
+      <c r="E4" s="508" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="502" t="s">
+      <c r="F4" s="508" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="502" t="s">
+      <c r="G4" s="508" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="502" t="s">
+      <c r="H4" s="508" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="503" t="s">
+      <c r="A5" s="509" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="503" t="s">
+      <c r="B5" s="509" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="503" t="s">
+      <c r="C5" s="509" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="503" t="s">
+      <c r="D5" s="509" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="503" t="s">
+      <c r="E5" s="509" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="503" t="s">
+      <c r="F5" s="509" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="503" t="s">
+      <c r="G5" s="509" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="503" t="s">
+      <c r="H5" s="509" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="504" t="s">
+      <c r="A6" s="510" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="504" t="s">
+      <c r="B6" s="510" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="504" t="s">
+      <c r="C6" s="510" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="504" t="s">
+      <c r="D6" s="510" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="504" t="s">
+      <c r="E6" s="510" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="504" t="s">
+      <c r="F6" s="510" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="504" t="s">
+      <c r="G6" s="510" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="504" t="s">
+      <c r="H6" s="510" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="511" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="511" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="511" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="511" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="511" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="511" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="511" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="511" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="512" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="512" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="512" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="512" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="512" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="512" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="512" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="512" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="513" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="513" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="513" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="513" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="513" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="513" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="513" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="513" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="514" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="514" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="514" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="514" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="514" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="514" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="514" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="514" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="515" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="515" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="515" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="515" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="515" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="515" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="515" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="515" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code cleanup and packaging redefinition
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4104" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4781" uniqueCount="342">
   <si>
     <t>URL</t>
   </si>
@@ -461,6 +461,645 @@
 1502 Black Gold cigars bring on the muscle, full-tilt, for cigar smokers who enjoy extra bold tobacco flavor from end-to-end. A diverse Nicaraguan core is bound in two additional leaves, and finished in a maduro wrapper that's been nurtured by the sun to achieve the peak of flavor. Earthy-woody flavors abound as a layer of chili pepper works its way in, complemented by a delicate, chocolatey-fruity sweetness for a resounding multidimensional smoke.
 1502 Nicaragua cigars boast an "all-inclusive" Nicaraguan blend that uses tobaccos from Nicaragua's four main growing regions: Estelí, Jalapa, Condega, and Ometepe. Medium-full in body, this cigar's flavor profile fits somewhere between the 1502 Emerald and 1502 Ruby offering a velvety smoothness and amazing balance. The smoke is earthy and woody with some fruity elements, enhanced by a toasty, honeyed aroma.
 With so many wonderful blends to choose from, there's a 1502 cigar in your future. Browse the selections and find the 1502 cigar that's right for you – right now!</t>
+  </si>
+  <si>
+    <t>CANONICAL URL</t>
+  </si>
+  <si>
+    <t>HEADER 1</t>
+  </si>
+  <si>
+    <t>SEO PARAGRAPH</t>
+  </si>
+  <si>
+    <t>1502 cigars are ready to take their place alongside many of the best Nicaraguan cigars you can buy. Presented in a variety of meticulously handcrafted blends that appeal to cigar smokers of every experience, these boutique cigars offer superb quality and taste in a limited number of box-pressed sizes in four savory selections. At the heart of the 1502 brand are the three core lines: the 1502 Emerald, 1502 Ruby, and 1502 Black Gold. Each cigar is unique in character and designed to be enjoyed morning, noon, and night, starting with the medium-bodied Emerald, followed by the more full-flavored Ruby, and concluding with the full-bodied Black Gold. Of course, the choice is yours as to when you choose to revel in their rich Nicaraguan flavor, but whichever 1502 cigar you buy, you're in for a truly satisfying and unforgettable experience.
+Launched in 2012 by native Nicaraguan, Enrique Sanchez Icaza, founder and CEO of Global Premium Cigars, 1502 Cigars were given their numerical name to commemorate the year Christopher Columbus discovered Nicaragua. Upon his arrival, Columbus also discovered a new world full of riches such as gold, silver, and precious stones for which the 1502 Emerald, Ruby, and Black Gold selections are named. But most importantly was the discovery of tobacco, which was used as a high value form of trade currency virtually equal to that of the Spanish Doubloon.
+"In our premium brand 1502, you will find three tobacco lines with the highest quality, where the sowing process, harvest, curing, aging and selection of each tobacco leaf is our major concern," says Señor Sanchez. "It takes more than five years, from the time the seeds are sown until the time you can enjoy one of our fine cigars; this is why patience is one of our greatest virtues in the art of tobacco production."
+1502 Emerald cigars yield a subtle strength and velvety smooth flavor that is achieved by a blend of long fillers from Estelí, Condega, and Mexico's San Andres valley pressed in a mouthwatering Nicaraguan Corojo Habano wrapper leaf. Delicate flavors of citrus, cedar, and roasted nut form the base, as aromas of honey, vanilla and floral notes drift amid the thick, creamy smoke.
+1502 Ruby cigars were created to delight discerning smokers who seek more body and complexity from their cigars. A lusciously dark Ecuadorian wrapper surrounds a well-balanced blend of fully-aged tobaccos from Estelí and Jalapa, for a medium-bodied, full-flavored smoke brimming with earthy elements, sweet cedar, and subtle hints of macadamia nuts and sunflower seeds.
+1502 Black Gold cigars bring on the muscle, full-tilt, for cigar smokers who enjoy extra bold tobacco flavor from end-to-end. A diverse Nicaraguan core is bound in two additional leaves, and finished in a maduro wrapper that's been nurtured by the sun to achieve the peak of flavor. Earthy-woody flavors abound as a layer of chili pepper works its way in, complemented by a delicate, chocolatey-fruity sweetness for a resounding multidimensional smoke.
+1502 Nicaragua cigars boast an "all-inclusive" Nicaraguan blend that uses tobaccos from Nicaragua's four main growing regions: Estelí, Jalapa, Condega, and Ometepe. Medium-full in body, this cigar's flavor profile fits somewhere between the 1502 Emerald and 1502 Ruby offering a velvety smoothness and amazing balance. The smoke is earthy and woody with some fruity elements, enhanced by a toasty, honeyed aroma.
+With so many wonderful blends to choose from, there's a 1502 cigar in your future. Browse the selections and find the 1502 cigar that's right for you – right now!</t>
+  </si>
+  <si>
+    <t>1502 BLACK GOLD CIGARS</t>
+  </si>
+  <si>
+    <t>IDENTIFIED</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>1502 EMERALD CIGARS</t>
+  </si>
+  <si>
+    <t>1502 NICARAGUA CIGARS</t>
+  </si>
+  <si>
+    <t>4th Generation pipe accessories and tobacco say Stokkebye, so you know they’re good. Order now and treat your pipe to a rich selection of their best blends!</t>
+  </si>
+  <si>
+    <t>4th Generation pipe accessories and tobacco celebrate the rich history of Stokkebye tobacco – and fourth generation family head Erik Stokkebye has done the family proud with this rich variety of pipe tobaccos. Based on decades of his clan’s expertise that started with founding father Erik Peter, who began the tobacco journey in 1882 - this 4th Generation Stokkebye channels the legacy to offer to you a wide array of tastes, ranging from the mild and aromatic to mature Virginia. Order yours now!</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/601+steel+cigars</t>
+  </si>
+  <si>
+    <t>601 Steel Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Nestled in the foothills of Esteli, Nicaragua, sits the La Zona factory. A strikingly beautiful 2-story building that was once used as an Inn, is now the...</t>
+  </si>
+  <si>
+    <t>601 Steel Cigars</t>
+  </si>
+  <si>
+    <t>Nestled in the foothills of Esteli, Nicaragua, sits the La Zona factory. A strikingly beautiful 2-story building that was once used as an Inn, is now the centerpiece of Erik Espinosa's cigar domain, and where you'll find his excellent staff of torcedores rolling 601 Steel cigars. This bold new blend features a gorgeous and extra dark Habano oscuro wrapper for a smoke that's tough as nails, yet easy on the palate. Order a box, a 10-pack, or start with a 5-pack now. You'll be back for more!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 601 Brands » 601 Steel Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/7+20+4+cigars</t>
+  </si>
+  <si>
+    <t>7 20 4 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Looking for 7-20-4 cigars? Founded in 1874, today, this former Cuban tobacco blend has re-emerged, post Cuban embargo, as one of the best boutique cigars.</t>
+  </si>
+  <si>
+    <t>7 20 4 Cigars</t>
+  </si>
+  <si>
+    <t>Urban legend has it that 7-20-4 cigars were so-named, because R.G. Sullivan, who founded the brand in 1874, got his start in business with the winnings from a lottery ticket with the numbers 7, 20, and 4. However, writer George Franklyn Willey, offered a more plausible explanation in his book, Willey's semi-centennial book of Manchester, 1846-1896, that Sullivan changed the brand's original name, "New Gold Dust Cigars" to "7-20-4," the address of his Manchester, NH cigar factory at 724 Elm Street. The cigars, which sold for 10¢, were hand-made with Cuban tobacco fillers and Sumatra wrappers. The brand was so successful that Sullivan's factory became one of the world's largest manufacturers of handmade cigars.
+Today, Kurt A. Kendall, an entrepreneur and owner of two New Hampshire cigar stores, always had a fascination for vintage cigar memorabilia. Over the years he built-up an extensive collection of artifacts, and one of his passions was to revive the 7-20-4 cigars brand. So, Kendall acquired the then-defunct trademark, and began reproducing the historic cigars that now rank as one of the best boutique cigars on the market.
+K.A. Kendall's 7-20-4 core line is blended with a highly diverse blend of Nicaraguan, Honduran, Mexican and Columbian long-fillers, a Costa Rican binder, and a Brazilian Mata Fina wrapper, then cedar-aged for 120 days. The smoke is smooth, well-balanced, earthy, and naturally sweet, making it an ideal selection if you prefer a medium-full cigar with plenty of flavor at a very reasonable price.
+In another nostalgic presentation, 7-20-4 Hustler cigars are rolled "barber pole" style using alternating dark Brazilian and light Ecuadorian Connecticut wrappers that conceal a full-flavored blend of Nicaraguan long-fillers and a Brazilian binder. Brimming with creamy smoke underpinned by subtle sweet and spicy flavors, the cigar mixes it up along the way, making the 7-20-4 Hustler a satisfyingly complex buffet for the palate.
+If vintage cigar tobaccos make your mouth water, Erte cigars offer you a rare opportunity to taste the incomparable flavor a cigar that was rolled in 1996! The cigars were handmade in Costa Rica with Costa Rican, Nicaraguan, and Ecuadorian tobaccos that have mellowed beautifully over time. The smoke is ultra-smooth, laced with creamy flavors of sweet cedar, some earthiness, and a subtle sweetness on the finish. Presented with Erte's famed deco artwork on the boxes, and signature on the bands, Erté cigars are one of those rare finds. Just remember that once they're gone, they're gone forever.
+If you like a more full-flavored cigar blended with a variety of different tobaccos, 7-20-4 Factory 57 cigars are made with high-priming tobaccos from Honduras, Nicaragua, Mexico, Colombia, and Costa Rica rolled in a high-priming, triple-fermented Nicaraguan Jalapa Habano wrapper, all aged for three years, plus an additional six months before shipping.
+According to 7-20-4 Cigars owner, Kurt A. Kendall, the "Factory 57" name refers to the U.S. government's official designation of 7-20-4 as a licensed and taxed manufacturer of premium cigars. Medium to full in body, Kendall, describes the smoke as "bold, full, yet very smooth, with a distinct creaminess." Here again, 7-20-4 delivers a uniquely original flavor profile that must be smoked to be fully appreciated."</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » 7 20 4 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/7+20+4+1+cigars</t>
+  </si>
+  <si>
+    <t>7-20-4 Brand Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>7-20-4 cigars are one of those rare boutique brands that you just have to taste to fully appreciate. Their complex blend is handcrafted with Nicaraguan,...</t>
+  </si>
+  <si>
+    <t>7-20-4 Brand Cigars</t>
+  </si>
+  <si>
+    <t>7-20-4 cigars are one of those rare boutique brands that you just have to taste to fully appreciate. Their complex blend is handcrafted with Nicaraguan, Honduran, Mexican and Colombian, long-fillers, Costa Rican binder, and Brazilian Mata Fina wrappers. After curing &amp; aging, the cigars are aged again in Spanish cedar boxes for 120 days to mellow. The body is upper-to-medium, and very smooth with an amazing flavor and aroma, says 7-20-4 creator, K.A. Kendall. Try a box today and say WOW!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 7-20-4 Brands » 7-20-4 Brand Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/7+20+4+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/7+20+4+hustler+cigars</t>
+  </si>
+  <si>
+    <t>7-20-4 Hustler Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>7-20-4 Hustler Cigars are a medium-bodied barber pole selection from Kurt A. Kendall. Presented with bright blue neck and foot bands, a well-packed...</t>
+  </si>
+  <si>
+    <t>7-20-4 Hustler Cigars</t>
+  </si>
+  <si>
+    <t>7-20-4 Hustler Cigars are a medium-bodied barber pole selection from Kurt A. Kendall. Presented with bright blue neck and foot bands, a well-packed 3-nation core is seamlessly rolled in alternating Brazilian Mata Fina &amp; Ecuadorian Connecticut wrappers. The smoke is smooth, creamy and shifts gears during the flight for an impressively complex adventure. If you want to buy a barber pole cigar with lots of flavor, yet won't make your hair stand on end like Guy Fieri, order some Hustlers NOW.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All 7-20-4 Brands » 7-20-4 Hustler Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/90+miles+1980+cigars</t>
+  </si>
+  <si>
+    <t>90 Miles 1980 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>90 Miles 1980 cigars are the 3rd release in this award-winning brand by Flor De Gonzalez. Made with a blend of Nicaraguan &amp; Dominican Ligero, a rare,...</t>
+  </si>
+  <si>
+    <t>90 Miles 1980 Cigars</t>
+  </si>
+  <si>
+    <t>90 Miles 1980 cigars are the 3rd release in this award-winning brand by Flor De Gonzalez. Made with a blend of Nicaraguan &amp; Dominican Ligero, a rare, Ecuadorian-grown, Connecticut seed Broadleaf binder, and a flawless Mexican San Andres capa. The smoke is medium-full and ultra-creamy. Opening with notes of caramel, the cigar builds to a perfectly balanced mix of earthy, nutty and sweet tobacco flavors. The ash and burn are equally outstanding. Maybe the best 90 Miles yet! Order your box now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Flor De Gonzalez Brands » 90 Miles 1980 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/flor+de+gonzalez+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/90+miles+by+flor+de+gonzalez+1+cigars</t>
+  </si>
+  <si>
+    <t>90 Miles by Flor De Gonzalez Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>90 Miles cigars are among the finest editions from good folks at Flor De Gonzalez. An all-Nicaraguan longfiller core rolled in reddish Ecuadorian Habano...</t>
+  </si>
+  <si>
+    <t>90 Miles by Flor De Gonzalez Cigars</t>
+  </si>
+  <si>
+    <t>90 Miles cigars are among the finest editions from good folks at Flor De Gonzalez. An all-Nicaraguan longfiller core rolled in reddish Ecuadorian Habano wrappers offers a medium-bodied smoke that starts out with sweet spice notes, then shifts to an earthier, creamier smoke with flavors of sweet wood and white pepper. The cigars burn beautifully, and stay in character right down to the nub, making the final act a full-flavored treat. A lot of love went into making these. Order your box now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Flor De Gonzalez Brands » 90 Miles by Flor De Gonzalez Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/90+miles+reserva+selecta+cigars</t>
+  </si>
+  <si>
+    <t>90 Miles Reserva Selecta Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>90 Miles Reserva Selecta cigars take the highly-rated 90 Miles selection to new heights of flavor and complexity. Medium to full in body, each cigar is...</t>
+  </si>
+  <si>
+    <t>90 Miles Reserva Selecta Cigars</t>
+  </si>
+  <si>
+    <t>90 Miles Reserva Selecta cigars take the highly-rated 90 Miles selection to new heights of flavor and complexity. Medium to full in body, each cigar is wrapped in a dark, shimmering Habano 2000 wrapper grown in Ecuador that surrounds the finest, most select Dominican and Nicaraguan longfillers slowly aged 3-5 years for a luxurious, well-rounded, and perfectly-balanced smoke with a seductive aroma. Arguably the best cigars yet from the Gonzalez family. Tasting is believing! Order some now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Flor De Gonzalez Brands » 90 Miles Reserva Selecta Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/a+flores+cigars</t>
+  </si>
+  <si>
+    <t>A Flores Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Shop for A. Flores 1975 cigars online at Famous Smoke Shop. Gran Reserva, Serie Privada, AFR-75, Flores y Rodriguez 10th, now in stock at discount prices.</t>
+  </si>
+  <si>
+    <t>A Flores Cigars</t>
+  </si>
+  <si>
+    <t>A. Flores Cigars are named for Abe Flores, president and blending mastermind behind PDR Cigars, producers of some of the best Dominican premium cigars, and the fastest growing Dominican-owned cigar factory in the Dominican Republic. Founded in 2004 and based in Tamboril, under Abe's direction the company has gone from a small boutique cigar business to a leading manufacturer that has also made cigars for some of the world's best cigar brands, as well as exclusive selections for several online cigar stores, including Famous Smoke Shop. Some people just have the knack for tobac' and Abe Flores is one of them. Moreover, the A. Flores 1975 lines are distinguished from the PDR 1878 brands (most of which are Dominican puros), by their singular blends and complex flavor characteristics. These include the A. Flores Gran Reserva, A. Flores Serie Privada, AFR-75 San Andrés Maduro, and the Flores y Rodriguez 10th Anniversary cigars.
+In 2011, the company moved to a much larger facility which allowed Abe to begin processing his own tobacco and gave him access to the highest quality tobacco leaves.
+"The Cuban seed tobaccos, that’s my spice rack," said Abe in a 2013 Cigar Journal article. The article also went on to say that Abe's "new-age Cuban designs are classic and familiar, inspired by the old but not out of date. We can see why [he] is moving ahead so fast. His designs are fresh, his blends are great. He is a cigar-maker to watch, closely."
+Notice that A. Flores cigars have the year 1975 on their bands; that signifies the year Flores was born. In addition to his acumen for blending, A. Flores 1975 cigars are rolled in a traditional Cuban method known as "entubado" wherein the tobaccos are bunched around each other in a circular fashion, like the rings of a tree, rather than folding them inside each other. The process is more time consuming and costly, but the upside is that it yields a much more complex smoke, while providing an effortless draw and a more even burn.
+A. Flores Gran Reserva cigars are a medium-bodied selection released in 2013. Described as "a delightful symphony of flavors," each A. Flores Gran Reserva cigar is handcrafted with a mass of diverse Nicaraguan Habano &amp; Dominican Corojo long fillers, and a Dominican Olor binder seamlessly rolled in an extra-long-aged 2006 Dominican Corojo wrapper. The result is a full-flavored smoke that's rich, creamy and well-balanced with a fragrant aroma.
+A. Flores 1975 Serie Privada cigars are presented in a choice of Ecuadorian Habano natural or richer-tasting maduro wrappers. These savory leaves encase a Nicaraguan Habano and Dominican Corojo filler &amp; binder blend, then are neatly box-pressed to perfection. The result is a medium-bodied masterpiece that reveals hints of vanilla, coffee bean and cocoa in perfect harmony. This selection has been so well-received it earned an "outstanding" 93 rating from Cigar Aficionado, and took the #10 spot for "Cigar of the Year" 2014.
+AFR-75 San Andrés Maduro cigars are made in extremely limited release, and named in honor of Abraham Flores Rosario (the initials of Abe's full name and the year he was born, 1975). "This is our 'factory' super premium," says Abe. A gorgeous and inherently sweet Mexican San Andres maduro wrapper caps a complex blend of Dominican Habano, Connecticut Broadleaf and Nicaraguan Criollo '98 with a Nicaraguan Criollo '98 binder, completed with a classy-looking band. The smoke is bold and spicy, yet incredibly smooth and well-balanced revealing dark, earthy, semi-sweet chocolate flavors laced with red pepper, making it a great selection for cigar smokers who already have a few notches on their gun belts.
+Flores y Rodriguez 10th Anniversary cigars celebrate a decade of making some of the best cigars in the Dominican Republic, or anywhere, for that matter. Using Nicaraguan long-fillers with 7-year-aged Dominican Piloto Cubano, a Dominican Olor binder, and an Ecuadorian Habano wrapper, the goal for this blend was to create something different that paid tribute to all of the people at PDR Cigars who have helped make the company a huge success. The result is a mild to medium-bodied cigar with a lot happening in terms of flavor and aroma, including earthiness, sweetness, spice, some woody-leathery notes and herbal elements, making it a great cigar for introducing yourself to the PDR cigar family.
+"I am extremely proud to have the opportunity to build on the legacy of the exceptional cigar makers that have been making cigars here in the Dominican Republic for decades," says Abe, "and very excited about bringing these A. Flores cigars to the market. We’ve taken special care to select the finest tobacco and create exceptional blend profiles that we feel today’s cigar enthusiast will truly appreciate."
+Now it's your turn. Browse through the selections featured here and find the A. Flores cigar that's right for you.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » A Flores Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/a+flores+gran+reserva+cigars</t>
+  </si>
+  <si>
+    <t>A Flores Gran Reserva Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>A Flores Gran Reserva cigars were released at 2013's IPCPR as Pinar Del Rio's premier cigar launch of the year. The cigar is a tribute to PDR's master...</t>
+  </si>
+  <si>
+    <t>A Flores Gran Reserva Cigars</t>
+  </si>
+  <si>
+    <t>A Flores Gran Reserva cigars were released at 2013's IPCPR as Pinar Del Rio's premier cigar launch of the year. The cigar is a tribute to PDR's master blender Abe Flores, creator of some of the best cigars on the market. The blend has a Dominican Corojo and Nicaraguan Habano filler, Dominican binder, and a well-aged 2006 Dominican Corojo wrapper. This is a limited run cigar with only 500 boxes of 24 cigars being made this year so make sure you pick up this amazing cigar while you still can!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All A Flores Brands » A Flores Gran Reserva Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/a+flores+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/a+flores+serie+privada+cigars</t>
+  </si>
+  <si>
+    <t>A Flores Serie Privada Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>A Flores Serie Privada cigars are one of the new offerings by Pinar Del Rio. This cigar is a tribute to master blender Abe Flores who has come out with a...</t>
+  </si>
+  <si>
+    <t>A Flores Serie Privada Cigars</t>
+  </si>
+  <si>
+    <t>A Flores Serie Privada cigars are one of the new offerings by Pinar Del Rio. This cigar is a tribute to master blender Abe Flores who has come out with a myriad of cigars that have time after time been rated 90+. These cigars are no different whether you get the Ecuadorian Habano wrapper for a creamy smoke, or the Ecuadorian Maduro wrapper which gives off a little more spice and sweetness. Whatever your taste may be, these are sure to please the pickiest of aficionados. Pick yours up now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All A Flores Brands » A Flores Serie Privada Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/a+crop+cigars</t>
+  </si>
+  <si>
+    <t>A-Crop Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>A-Crop cigars by PDR feature surplus leaf from their most premium cigars; rolled together, satisfaction is yours for a fraction of the price. Order now!</t>
+  </si>
+  <si>
+    <t>A-Crop Cigars</t>
+  </si>
+  <si>
+    <t>A-Crop cigars by PDR beg the question: when an artist paints his finest work, does he throw away his unused paint? No – they are used to create something else great. And in the case of A-Crop, it is a whole new PDR cigar brand crafted from excess tobacco purchased for use in Abe Flores pricier premium lines. Yes: PDR A-Crop cigars are the exact same scrumptious all-longfiller leaves that grace Abe’s finest sticks, now offered in 3 budget-friendly bundle sizes for your consumption. Try them all!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All PDR Brands » A-Crop Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/pdr+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/acid+cigars</t>
+  </si>
+  <si>
+    <t>ACID Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Looking for ACID Cigars at the best prices? For an awesomely aromatic smoking experience that's unequaled, save on ACID cigars today at Famous Smoke Shop.</t>
+  </si>
+  <si>
+    <t>ACID Cigars</t>
+  </si>
+  <si>
+    <t>The Rebirth of Cigars started in 1998. Long Island native Jonathan Drew employed a handful of cigar rollers in Nicaragua, while back in New York, Drew Estate partner and co-founder Marvin Samel led operations from a warehouse office in Brooklyn's DUMBO neighborhood. The “ACID” name was inspired by Scott "ACID" Chester, a neighborhood artist whose work mixed industrial, urban, graffiti, and motorcycle art – and provided an ideal marketing vehicle for ACID Cigars. This "sub-culture" aesthetic has become a dominant aspect of Drew Estate's culture and vibe.
+ACID cigars are all-handcrafted at Drew Estate's Esteli, Nicaragua factory. The cigars are rolled with some of the world's most select tobaccos, and have developed an almost cult-like following among cigar lovers who like a little extra something to their smoke. That something extra is Drew Estate's secret infusion process: unlike flavored cigars, the method involves various combinations of nearly 150 herbs, spices, botanicals and essences - making ACIDs a cigar smoking experience simply unlike anything else on the market. That means the only way to truly understand ACID cigars is to experience them.
+There are 4 distinctly different formulas at work here; so it’s helpful to look at each color band as an indicator of the strength and body of that particular infusion, as opposed to the strength or body of the cigar’s tobacco blend. First is ACID Blue band cigars, like the highly sought-after Kuba Kuba and Blondie, which are mild to medium cigars – but are blended to be very aromatic and sweet. You’ll also see this metallic blue band on 1400cc and ACID Wafe cigars, which are very different shapes of cigars – but smoke with the same aroma.
+ACID Red band cigars are a potent mix of ripe black tobaccos and the heaviest aromas; strength and body hover around medium, but the aromatics in Red bands like Liquid and Nasty are intense.
+The Gold band ACIDs – such as Cold Infusion – are lighter and more refreshing. They’re also very distinct, relying more on the natural cigar tobacco aromas to produce a sensation that’s somewhat more complex.
+The Purple band blends, like ACID Roam, feature creamier and super-complex aromatic hybrids that focus on flavor.
+The flavor experience in each cigar is unique, and that’s why people love them – find the infusion you like best and buy ACID cigars online at discount prices here at Famous Smoke Shop.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » ACID Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/acid+1+cigars</t>
+  </si>
+  <si>
+    <t>ACID Brand Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>All the ACID cigars are carefully handcrafted using some of the world's finest tobacco with more than one hundred and forty herbs, botanicals and other...</t>
+  </si>
+  <si>
+    <t>ACID Brand Cigars</t>
+  </si>
+  <si>
+    <t>All the ACID cigars are carefully handcrafted using some of the world's finest tobacco with more than one hundred and forty herbs, botanicals and other essential oils to get their unique aroma and flavor. Experiencing ACID cigars is the only way to understand them. Similar to all Drew Estate cigars, their construction is flawless since they are rolled in Sumatra, Maduro, Connecticut and African wrappers.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Acid Brands » ACID Brand Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/acid+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/acid+cigarillos+cigars</t>
+  </si>
+  <si>
+    <t>ACID Cigarillos | Famous Smoke</t>
+  </si>
+  <si>
+    <t>ACID Cigarillos are a more time-friendly expression of Drew Estate's secret infusion method used in ACID cigars. Each marries premium cigar tobaccos to a...</t>
+  </si>
+  <si>
+    <t>ACID Cigarillos</t>
+  </si>
+  <si>
+    <t>ACID Cigarillos are a more time-friendly expression of Drew Estate's secret infusion method used in ACID cigars. Each marries premium cigar tobaccos to a medley of 150 unique and flavorful herbs, spices and botanicals - and is finished in an array of choice, natural wrappers. As with their bigger brethren, an ACID cigarillo is a bona fide flavor machine. Prepare your senses for an intense encounter with the mellow Blue, bold Red, or the untamed flavor and aroma of Green - and get yours today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Acid Brands » ACID Cigarillos</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/acid+g+fresh+cigars</t>
+  </si>
+  <si>
+    <t>ACID G-Fresh Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Acid cigars were the first are still the best-selling cigar infused cigars in the industry. Each cigar is masterfully blended and infused with hundreds of...</t>
+  </si>
+  <si>
+    <t>ACID G-Fresh Cigars</t>
+  </si>
+  <si>
+    <t>Acid cigars were the first are still the best-selling cigar infused cigars in the industry. Each cigar is masterfully blended and infused with hundreds of botanicals for a smooth, flavorful, and aromatic smoke. Every cigar employs your senses for an all encompassing smoke, and now the G-Fresh packs ensure each cigar is as fresh as the last. Each is sealed in a fresh pack with a humidifying device so they stay fresh during shipping and at home without the need for a humidor. Buy yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Acid Brands » ACID G-Fresh Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/acid+subculture+cigars</t>
+  </si>
+  <si>
+    <t>ACID Subculture Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>ACID cigars are lurking just below the surface, flying under the radar of mainstream tastes and accepted cigar smoking traditions. Subculture is for the...</t>
+  </si>
+  <si>
+    <t>ACID Subculture Cigars</t>
+  </si>
+  <si>
+    <t>ACID cigars are lurking just below the surface, flying under the radar of mainstream tastes and accepted cigar smoking traditions. Subculture is for the hardcore only, boasting an extra-rich infusion of herbs, botanicals, and essential oils. Each entry in the Subculture series is aged an extra year to ensure a truly one-of-a-kind smoking experience. If you're ready to go to the next level in infused cigars, try a box today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Acid Brands » ACID Subculture Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/adorini+accessories</t>
+  </si>
+  <si>
+    <t>Adorini | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Adorini accessories and humidors are made to standards of the highest quality, while being sold at fair pricing. Order yours today from Famous and save!</t>
+  </si>
+  <si>
+    <t>Adorini</t>
+  </si>
+  <si>
+    <t>Adorini accessories and humidors are made of the highest quality while being sold at fair prices. They use the latest technology to create products work amazingly well and hold up to every day usage. Hours of manual labor go into every humidor they make, utilizing premium cedar and giving each box up to twenty individual layers of lacquer. All Adorini products go through a rigorous QC check before being sent out, and are the first brand to offer a lifetime warranty on all of their humidors. Your cigars deserve it – order one today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Accessories » Accessories » Humidification Brand List » Adorini</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/accessories,https://www.famous-smoke.com/cigar-humidification-brand-list</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/afr+75+san+andres+maduro+cigars</t>
+  </si>
+  <si>
+    <t>AFR-75 San Andres Maduro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>PDR AFR-75 cigars were introduced to the cigar world at IPCPR in 2013 as a tribute to the master blender great Abe Flores. The name AFR-75 represents...</t>
+  </si>
+  <si>
+    <t>AFR-75 San Andres Maduro Cigars</t>
+  </si>
+  <si>
+    <t>PDR AFR-75 cigars were introduced to the cigar world at IPCPR in 2013 as a tribute to the master blender great Abe Flores. The name AFR-75 represents Abraham Flores Rosario who was born in 1975. Each cigar is is made using a blend of Dominican, Connecticut Broadleaf, and a rare Nicaraguan Criollo 1998 filler. The same Nicaraguan Criollo 1998 tobacco is used for the binder, and it is all wrapped in a smooth and creamy San Andreas Maduro wrapper. Get your AFR-75 cigars today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All A Flores Brands » AFR-75 San Andres Maduro Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/aging+room+boutique+blends+cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Boutique Blends Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Aging Room &amp; Boutique Blends cigars offer small batch quality cigars in both traditional and flavored form. Add these delicious smokes to your humidor now!</t>
+  </si>
+  <si>
+    <t>Aging Room Boutique Blends Cigars</t>
+  </si>
+  <si>
+    <t>Aging Room &amp; Boutique Blends Cigars is the company responsible for the well-rated, highly-acclaimed SWAG and Aging Room cigars; and while these brands put Cuban-born Rafael Nodal on the map, his role in the company’s success runs much deeper than churning out delicious small batch after small batch of smokes.
+Boutique Blends wasn’t the name of Rafael &amp; Co.’s operation until 2012 – it was known as the Habana Cuba Cigar Company. HCCC was founded in 1996, and made premium hand rolled cigars during the boom – most notably reestablishing the Cuban Oliveros brand of cigars.
+Oliveros cigars was their first brand to debut, launching as a flavored cigar that was being manufactured in the Dominican Republic. But within a year, the Cigar Boom went bust…and with America turning its collective attention away from cigars, Habana Cuba Cigar had to find a new way to sell their smokes. It was then that the owners turned to an internet marketing operation that specialized in selling boutique blends made in and around the Miami area, operated by…Rafael Nodal and Hank Bischoff. As Habana Cigars’ most successful marketers, Rafael and Hank were brought on staff to advise the company; not long after, Habana’s owners wanted out of the tobacco market, and sold their lines of flavored and premium Oliveros lines to Nodal, his wife Alina and Bischoff in 2002.
+The new owners decided that it was time to focus on premium hand made cigars, and turned to Nick Perdomo for help. Perdomo manufactured high-quality Nicaraguan smokes under contract for HCCC, and the company was able to build its portfolio beyond the Oliveros label. Partnerships like these would continue over the next few years, involving Nick, Nestor Plasencia and other talented cigar makers – including José "Jochi" Blanco and his Dominican Tabacalera La Palma. As Nodal &amp; Bischoff began specializing in these more limited batch cigars, they worked with Blanco on the Dominican puro blend that would become SWAG. With Jochi’s stocks of well-aged, premium DR leaf, the Aging Room cigar line would follow – and the company rebranded itself as Boutique Blends Cigars in 2012.
+Though the flavored cigar market is dominated by machine-made offerings, Oliveros flavored cigars have carved out a nice spot for themselves by doing it differently: they’re hand made in the DR, and feature 100% premium aged Dominican tobaccos in their Long Lady line of smokes. And keeping true to Rafael &amp; Hank’s vision for a true boutique premium produced in limited fashion, La Boheme cigars were released in 2014 as a flavorful, medium-to-full bodied Dominican premium sporting a Habano wrapper – and definitely different than the SWAG and Aging Room you may have had the pleasure of smoking.
+All of the cigar selections under both the Aging Room cigar line and the Boutique Blends banner are handmade treats, whether it’s the flavored Oliveros or the premium La Boheme – and well worth the smoking time. Buy Aging Room &amp; Boutique Blends cigars at Famous Smoke Shop, and smoke them for less!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » Aging Room Boutique Blends Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/aging+room+bin+no.+1+cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Bin #1 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Aging Room Bin No. 1 comes to you from a special place. See, there's actually a spot in the factory called Bin #1, where Cuban-seed Dominican tobaccos have...</t>
+  </si>
+  <si>
+    <t>Aging Room Bin #1 Cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Bin No. 1 comes to you from a special place. See, there's actually a spot in the factory called Bin #1, where Cuban-seed Dominican tobaccos have been resting for over 15 years, making this leaf so well-aged, we can actually call it grown up. That extra rest reveals a VERY FULL-body smoke that, wrapped in Ecuadorian Habano, well...your taste buds will have a field day. Good things truly come to those who wait - now that Aging Room Bin No.1 has arrived, grab your box without delay!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Aging Room - Boutique Blends Brands » Aging Room Bin #1 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/aging+room+boutique+blends+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/aging+room+havao+cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Havao Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>The Aging Room Havao is a limited batch cigar, using only the finest and rarest tobaccos today incorporating an Ecuadorian Connecticut shade with Dominican...</t>
+  </si>
+  <si>
+    <t>Aging Room Havao Cigars</t>
+  </si>
+  <si>
+    <t>The Aging Room Havao is a limited batch cigar, using only the finest and rarest tobaccos today incorporating an Ecuadorian Connecticut shade with Dominican Havano Criollo filler and binder which releases a complex blend of exquisite flavor and aroma. This is the first cigar manufactured under Rafael Nodal's Boutique Blends Cigars, and what a cigar to start with. A true boutique cigar, this is sure to please anyone from a new cigar smoker, to the veterans. Order yours now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Aging Room - Boutique Blends Brands » Aging Room Havao Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/aging+room+maduro+cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Maduro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Aging Room Maduro cigars are another great offering by Rafael Nodal. Aging Room cigars are known for their small batch offerings with the philosophy that...</t>
+  </si>
+  <si>
+    <t>Aging Room Maduro Cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Maduro cigars are another great offering by Rafael Nodal. Aging Room cigars are known for their small batch offerings with the philosophy that each cigar should be made using the best tobaccos making each one, in a sense, perfect. The Aging Room Maduro is just that. Perfect. Each cigar is composed of Dominican binders and fillers all wrapped up in a dark Nicaraguan Maduro wrapper for ultimate complexity and flavor. This is a cigar smoker's dream. Pick yours up now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Aging Room - Boutique Blends Brands » Aging Room Maduro Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/aging+room+quattro+f55+cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Quattro F55 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Aging Room Quattro cigars are made with the most select Dominican Habano long-fillers and binders, BOX-PRESSED in gorgeous, buttery-smooth, 2003-vintage...</t>
+  </si>
+  <si>
+    <t>Aging Room Quattro F55 Cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Quattro cigars are made with the most select Dominican Habano long-fillers and binders, BOX-PRESSED in gorgeous, buttery-smooth, 2003-vintage Sumatra (on the F55) and Dominican Habano wrappers (on the F59). These medium-full smokes are robust, earthy, and stealthily heady with an excellent balance, burn and draw. Perfect for the cigar enthusiast who appreciates an opulent, high-quality cigar riddled with savory nuances. Discover these award-winning cigars by ordering some today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Aging Room - Boutique Blends Brands » Aging Room Quattro F55 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/aging+room+small+batch+1+cigars</t>
+  </si>
+  <si>
+    <t>Aging Room Small Batch Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Aging Room M356 cigars are made by Rafael Nodal, of Boutique Blends, using rare Dominican tobaccos encased in Habano-seed wrappers. The tobaccos were...</t>
+  </si>
+  <si>
+    <t>Aging Room Small Batch Cigars</t>
+  </si>
+  <si>
+    <t>Aging Room M356 cigars are made by Rafael Nodal, of Boutique Blends, using rare Dominican tobaccos encased in Habano-seed wrappers. The tobaccos were originally intended for use in another line, but there simply wasn't enough of it to meet production demand.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Aging Room - Boutique Blends Brands » Aging Room Small Batch Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/agio+meharis+1+cigars</t>
+  </si>
+  <si>
+    <t>Agio Meharis Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Since 1976, Agio Mehari's cigars have been appreciated for their unique flavor, authenticity, and their handy cigarillo size. Ever since, Mehari's has...</t>
+  </si>
+  <si>
+    <t>Agio Meharis Cigars</t>
+  </si>
+  <si>
+    <t>Since 1976, Agio Mehari's cigars have been appreciated for their unique flavor, authenticity, and their handy cigarillo size. Ever since, Mehari's has constantly reinvented itself without losing its identity. Mehari's take you on a unique voyage of discovery to places that appeal to the imagination. Places that are rarely visited and filled with mystery for a journey brimming with enigma, adventure, and satisfying tobacco flavor and aroma. That's Mehari's. Try some Agio Mehari's today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » Agio Meharis Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/al+capone+cigars</t>
+  </si>
+  <si>
+    <t>Al Capone Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Al Capone cigars are so deliciously sweet and petite they're downright habit forming! Hand rolled and presented in several flavors, including a filtered...</t>
+  </si>
+  <si>
+    <t>Al Capone Cigars</t>
+  </si>
+  <si>
+    <t>Al Capone cigars are so deliciously sweet and petite they're downright habit forming! Hand rolled and presented in several flavors, including a filtered version, they're perfect for those times when you just HAVE to have a cigar, but don't have time for a full-size smoke. Priced affordably, find the Al Capone cigars that are right for you and toss 'em in your cart. Make sure you have enough, too. (If you run short, don't say we didn't warn 'ya about them being habit forming.)</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » Al Capone Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/alec+bradley+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley cigars are about as high class and scrumptious as you can find. We carry the complete line of Alec Bradley at prices that won't bust your budget!</t>
+  </si>
+  <si>
+    <t>Alec Bradley Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley cigars are to the smoking world as Rolex is to the word of timepieces. Both make a wide variety of items, but both have one thing in common: quality. Alec Bradley stogies are about as high class and scrumptious as you can find, all at a price that not only a prince, but a pauper can afford. Famous Smoke Shop and Alec Bradley have built a long standing relationship to help provide you with these cigars at damn good prices. The reason we keep good relations with them is simple. Aside from being awesome people in general, and pretty damn good at flip cup, they have developed a rich history in their short time on the market.
+It all started in 1996 with Alan Rubin taking part of the proceeds of his father's hardware import company to create Alec Bradley cigars, named after his two children (dawwww). It was at the Retail Tobacco Dealers of America trade show where he eventually found a small manufacturer in Honduras to make his first creation, but those crafty Honduran thieves took him for a ride. He paid them but barely received the cigars he asked for. Eventually he received some cigars, and the first Alec Bradley cigars ever banded, called Bogey's Stogies, were meant to be sold at golf courses locally, but ended up failing miserably after only 2 years. Of course, with a cigar including bogey in the name, it's easy to see why golfers wouldn't want this bogus cigar.
+Mind you, Alan was starting Alec Bradley cigars right at the tail end of the cigar boom of the 1990s which meant prominent cigar companies had already formed and secured a foothold in the industry. Breaking in to a newly established market was no easy feat at the time, but persistence paid off in the year 2000 when he teamed up with Ralph Montero, a prominent cigar professional. That year they employed Davidoff's master blender, Henke Kelner, to create the Occidental Reserve, and samples were sent to brick and mortar shops around the nation, garnering them 300 customers. Alec Bradley followed up shortly thereafter with the Trilogy, a triangular box-pressed cigar.
+However, Alan Rubin and Ralph Montero hit their stride as late as 2007 with their first full-bodied cigar called the Tempus. No other Alec Bradley cigar offered a strength profile as powerful and perfectly balanced as the Alec Bradley Tempus. It was an instant success, which sent the company into overdrive. And what does a company do when the profits roll in and they want to be a contender? They throw down the knockout punch.
+Two years later, in the spirit of going all-out for the sake of premium hand rolled goodness, the Alec Bradley Prensado was released, which immediately drew cigar collectors to retail counters across the globe. Immediately the ratings started flowing in - 91, 94, 96, hardly any marks below the 90 mark, leading to Alec Bradley's biggest honor. They had made the number one cigar in the world. Sure, it took two years before it won the prestigious award, but the Alec Bradley Prensado had beat out the competition, and in just over a decade, Alan Rubin went from selling an import company to receiving top honors.
+Since then, Alec Bradley has been pumping out stellar blends non-stop. The Alec Bradley Sun Grown has been making its way into everyone's humidor; the Alec Bradley Nica Puro is perhaps the best Nicaraguan Puro to ever hit the shelves; and the Black Market should honestly be illegal it's so good. They might actually need to start selling it on the black market.
+It's unheard of to have the kind of success Alan Rubin had while making every Alec Bradley cigar, well, aside from the Bogey Stogie fiasco. To go from nobody to top dog after failing with his first product in just over a decade is unheard of. But if Alan Rubin proved one thing, it's that he knows how to make a damn good stogie."</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » Alec Bradley Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+1600+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley 1600 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley 1600 cigars continue AB's award-winning rep for producing premium cigars with superb quality, flavor and balance. Their numerical moniker...</t>
+  </si>
+  <si>
+    <t>Alec Bradley 1600 Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley 1600 cigars continue AB's award-winning rep for producing premium cigars with superb quality, flavor and balance. Their numerical moniker comes from the year 1600, when tobacco was first grown in Brazil, and the source of their dark, lustrous Habano wrappers. When added to the Honduran, Nicaraguan &amp; Costa Rican filler core, they reveal a full-bodied smoke rippling with flavors of earth, wood, some sweetness, and a spicy aroma. Priced affordably, add some to your cart right now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley 1600 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/alec+bradley+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+1633+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley 1633 Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley 1633 cigars are going to be your new every day smoke! Using a master blend of Panamanian, Honduran, and Nicaraguan longfillers, a Costa Rican...</t>
+  </si>
+  <si>
+    <t>Alec Bradley 1633 Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley 1633 cigars are going to be your new every day smoke! Using a master blend of Panamanian, Honduran, and Nicaraguan longfillers, a Costa Rican binder, and smooth Connecticut wrapper, this cigar is a 5 nation coalition that'll lay down some serious flavor. Made to pay homage to the year tobacco was grown in CT for the first time (1633), this cigar embodies everything a true full-flavored CT wrapped cigar should be. Get your hands on this exquisite cigar today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley 1633 Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+accessories+and+samplers+1+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Accessories And Cigar Samplers | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley cigars represent some of the finest premium cigar selections available today. With their passion for excellence, Alec Bradley premium cigars...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Accessories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>Alec Bradley cigars represent some of the finest premium cigar selections available today. With their passion for excellence, Alec Bradley premium cigars are expertly handmade using only the most select tobaccos from all over the world, and have achieved some of the highest cigar tasting scores. When you light-up an Alec Bradley cigar you can expect a cigar made to the highest standards of quality for a smoke that's consistently rich in flavor and aroma. Try some today and taste for yourself!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Accessories And Cigar Samplers</t>
   </si>
 </sst>
 </file>
@@ -485,7 +1124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="83">
+  <fills count="90">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -898,8 +1537,43 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="322">
+  <borders count="350">
     <border>
       <left/>
       <right/>
@@ -2362,11 +3036,137 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="516">
+  <cellXfs count="593">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3911,6 +4711,237 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="83" borderId="325" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="325" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="325" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="325" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="84" borderId="329" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="329" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="329" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="329" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="85" borderId="333" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="333" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="333" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="333" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="86" borderId="337" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="337" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="337" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="337" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="87" borderId="341" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="341" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="341" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="341" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="88" borderId="345" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="345" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="345" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="345" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="345" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="345" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="89" borderId="349" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -4235,300 +5266,1494 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="70.01171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="70.01171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="46.9609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="145.83984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="31.43359375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="82.36328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="82.36328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="56.2421875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="145.84375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="40.71484375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="126.45703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="178.8125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="133.88671875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="188.4921875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.87109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="505" t="s">
+      <c r="A1" s="542" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="505" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="505" t="s">
+      <c r="B1" s="542" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="505" t="s">
+      <c r="D1" s="542" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="505" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="505" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="505" t="s">
+      <c r="E1" s="542" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="542" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="542" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="505" t="s">
+      <c r="H1" s="542" t="s">
         <v>10</v>
+      </c>
+      <c r="I1" s="542" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="506" t="s">
+      <c r="A2" s="543" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="506" t="s">
+      <c r="B2" s="543" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="506" t="s">
+      <c r="C2" s="543" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="506" t="s">
+      <c r="D2" s="543" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="506" t="s">
+      <c r="E2" s="543" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="506" t="s">
+      <c r="F2" s="543" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="506" t="s">
+      <c r="G2" s="543" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="506" t="s">
+      <c r="H2" s="543" t="s">
         <v>17</v>
+      </c>
+      <c r="I2" s="543" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="507" t="s">
+      <c r="A3" s="544" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="544" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="507" t="s">
+      <c r="C3" s="544" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="507" t="s">
+      <c r="D3" s="544" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="507" t="s">
+      <c r="E3" s="544" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="507" t="s">
+      <c r="F3" s="544" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="507" t="s">
+      <c r="G3" s="544" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="507" t="s">
+      <c r="H3" s="544" t="s">
         <v>24</v>
+      </c>
+      <c r="I3" s="544" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="508" t="s">
+      <c r="A4" s="545" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="508" t="s">
+      <c r="B4" s="545" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="508" t="s">
+      <c r="C4" s="545" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="508" t="s">
+      <c r="D4" s="545" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="508" t="s">
+      <c r="E4" s="545" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="508" t="s">
+      <c r="F4" s="545" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="508" t="s">
+      <c r="G4" s="545" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="508" t="s">
+      <c r="H4" s="545" t="s">
         <v>31</v>
+      </c>
+      <c r="I4" s="545" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="509" t="s">
+      <c r="A5" s="546" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="509" t="s">
+      <c r="B5" s="546" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="509" t="s">
+      <c r="C5" s="546" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="509" t="s">
+      <c r="D5" s="546" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="509" t="s">
+      <c r="E5" s="546" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="509" t="s">
+      <c r="F5" s="546" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="509" t="s">
+      <c r="G5" s="546" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="509" t="s">
+      <c r="H5" s="546" t="s">
         <v>31</v>
+      </c>
+      <c r="I5" s="546" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="510" t="s">
+      <c r="A6" s="547" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="510" t="s">
+      <c r="B6" s="547" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="510" t="s">
+      <c r="C6" s="547" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="510" t="s">
+      <c r="D6" s="547" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="510" t="s">
+      <c r="E6" s="547" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="510" t="s">
+      <c r="F6" s="547" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="510" t="s">
+      <c r="G6" s="547" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="510" t="s">
+      <c r="H6" s="547" t="s">
         <v>31</v>
+      </c>
+      <c r="I6" s="547" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="511" t="s">
+      <c r="A7" s="548" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="511" t="s">
+      <c r="B7" s="548" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="511" t="s">
+      <c r="C7" s="548" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="511" t="s">
+      <c r="D7" s="548" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="511" t="s">
+      <c r="E7" s="548" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="511" t="s">
+      <c r="F7" s="548" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="511" t="s">
+      <c r="G7" s="548" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="511" t="s">
+      <c r="H7" s="548" t="s">
         <v>31</v>
+      </c>
+      <c r="I7" s="548" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="512" t="s">
+      <c r="A8" s="549" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="512" t="s">
+      <c r="B8" s="549" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="512" t="s">
+      <c r="C8" s="549" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="512" t="s">
+      <c r="D8" s="549" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="512" t="s">
+      <c r="E8" s="549" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="512" t="s">
+      <c r="F8" s="549" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="512" t="s">
+      <c r="G8" s="549" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="512" t="s">
+      <c r="H8" s="549" t="s">
         <v>59</v>
+      </c>
+      <c r="I8" s="549" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="513" t="s">
+      <c r="A9" s="550" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="513" t="s">
+      <c r="B9" s="550" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="513" t="s">
+      <c r="C9" s="550" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="513" t="s">
+      <c r="D9" s="550" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="513" t="s">
+      <c r="E9" s="550" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="513" t="s">
+      <c r="F9" s="550" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="513" t="s">
+      <c r="G9" s="550" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="513" t="s">
+      <c r="H9" s="550" t="s">
         <v>24</v>
+      </c>
+      <c r="I9" s="550" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="514" t="s">
+      <c r="A10" s="551" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="514" t="s">
+      <c r="B10" s="551" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="514" t="s">
+      <c r="C10" s="551" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="514" t="s">
+      <c r="D10" s="551" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="514" t="s">
+      <c r="E10" s="551" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="514" t="s">
+      <c r="F10" s="551" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="514" t="s">
+      <c r="G10" s="551" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="514" t="s">
+      <c r="H10" s="551" t="s">
         <v>72</v>
+      </c>
+      <c r="I10" s="551" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="515" t="s">
+      <c r="A11" s="552" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="515" t="s">
+      <c r="B11" s="552" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="515" t="s">
+      <c r="C11" s="552" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="515" t="s">
+      <c r="D11" s="552" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="515" t="s">
+      <c r="E11" s="552" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="515" t="s">
+      <c r="F11" s="552" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="515" t="s">
+      <c r="G11" s="552" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="515" t="s">
+      <c r="H11" s="552" t="s">
         <v>72</v>
+      </c>
+      <c r="I11" s="552" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="553" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="553" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="553" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="553" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="553" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="553" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="553" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="553" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="553" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="554" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="554" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="554" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="554" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="554" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="554" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="554" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="554" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="554" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="555" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="555" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="555" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="555" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="555" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="555" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="555" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="555" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="555" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="556" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="556" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="556" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="556" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="556" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="556" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="556" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="556" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="556" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="557" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="557" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="557" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="557" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="557" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="557" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="557" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" s="557" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="557" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="558" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="558" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="558" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="558" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="558" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="558" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="558" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" s="558" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" s="558" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="559" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="559" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="559" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="559" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="559" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="559" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="559" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" s="559" t="s">
+        <v>115</v>
+      </c>
+      <c r="I18" s="559" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="560" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="560" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="560" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="560" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="560" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="560" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" s="560" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="560" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" s="560" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="561" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="561" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="561" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="561" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="561" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="561" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="561" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="561" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" s="561" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="562" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="562" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="562" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="562" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="562" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="562" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="562" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="562" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="562" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="563" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" s="563" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="563" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="563" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="563" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="563" t="s">
+        <v>158</v>
+      </c>
+      <c r="G22" s="563" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" s="563" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" s="563" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="564" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="564" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="564" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="564" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" s="564" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" s="564" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" s="564" t="s">
+        <v>165</v>
+      </c>
+      <c r="H23" s="564" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="564" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="565" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="565" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="565" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" s="565" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" s="565" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24" s="565" t="s">
+        <v>170</v>
+      </c>
+      <c r="G24" s="565" t="s">
+        <v>171</v>
+      </c>
+      <c r="H24" s="565" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24" s="565" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="566" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25" s="566" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="566" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="566" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" s="566" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" s="566" t="s">
+        <v>177</v>
+      </c>
+      <c r="G25" s="566" t="s">
+        <v>178</v>
+      </c>
+      <c r="H25" s="566" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" s="566" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="567" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="567" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="567" t="s">
+        <v>180</v>
+      </c>
+      <c r="D26" s="567" t="s">
+        <v>181</v>
+      </c>
+      <c r="E26" s="567" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26" s="567" t="s">
+        <v>183</v>
+      </c>
+      <c r="G26" s="567" t="s">
+        <v>184</v>
+      </c>
+      <c r="H26" s="567" t="s">
+        <v>185</v>
+      </c>
+      <c r="I26" s="567" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="568" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="568" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="568" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="568" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="568" t="s">
+        <v>189</v>
+      </c>
+      <c r="F27" s="568" t="s">
+        <v>190</v>
+      </c>
+      <c r="G27" s="568" t="s">
+        <v>191</v>
+      </c>
+      <c r="H27" s="568" t="s">
+        <v>185</v>
+      </c>
+      <c r="I27" s="568" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="569" t="s">
+        <v>192</v>
+      </c>
+      <c r="B28" s="569" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" s="569" t="s">
+        <v>193</v>
+      </c>
+      <c r="D28" s="569" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="569" t="s">
+        <v>195</v>
+      </c>
+      <c r="F28" s="569" t="s">
+        <v>196</v>
+      </c>
+      <c r="G28" s="569" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" s="569" t="s">
+        <v>185</v>
+      </c>
+      <c r="I28" s="569" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="570" t="s">
+        <v>198</v>
+      </c>
+      <c r="B29" s="570" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="570" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" s="570" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="570" t="s">
+        <v>201</v>
+      </c>
+      <c r="F29" s="570" t="s">
+        <v>202</v>
+      </c>
+      <c r="G29" s="570" t="s">
+        <v>203</v>
+      </c>
+      <c r="H29" s="570" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="570" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="571" t="s">
+        <v>204</v>
+      </c>
+      <c r="B30" s="571" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" s="571" t="s">
+        <v>205</v>
+      </c>
+      <c r="D30" s="571" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="571" t="s">
+        <v>207</v>
+      </c>
+      <c r="F30" s="571" t="s">
+        <v>208</v>
+      </c>
+      <c r="G30" s="571" t="s">
+        <v>209</v>
+      </c>
+      <c r="H30" s="571" t="s">
+        <v>210</v>
+      </c>
+      <c r="I30" s="571" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="572" t="s">
+        <v>211</v>
+      </c>
+      <c r="B31" s="572" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" s="572" t="s">
+        <v>212</v>
+      </c>
+      <c r="D31" s="572" t="s">
+        <v>213</v>
+      </c>
+      <c r="E31" s="572" t="s">
+        <v>214</v>
+      </c>
+      <c r="F31" s="572" t="s">
+        <v>215</v>
+      </c>
+      <c r="G31" s="572" t="s">
+        <v>216</v>
+      </c>
+      <c r="H31" s="572" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="572" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="573" t="s">
+        <v>217</v>
+      </c>
+      <c r="B32" s="573" t="s">
+        <v>217</v>
+      </c>
+      <c r="C32" s="573" t="s">
+        <v>218</v>
+      </c>
+      <c r="D32" s="573" t="s">
+        <v>219</v>
+      </c>
+      <c r="E32" s="573" t="s">
+        <v>220</v>
+      </c>
+      <c r="F32" s="573" t="s">
+        <v>221</v>
+      </c>
+      <c r="G32" s="573" t="s">
+        <v>222</v>
+      </c>
+      <c r="H32" s="573" t="s">
+        <v>223</v>
+      </c>
+      <c r="I32" s="573" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="574" t="s">
+        <v>224</v>
+      </c>
+      <c r="B33" s="574" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" s="574" t="s">
+        <v>225</v>
+      </c>
+      <c r="D33" s="574" t="s">
+        <v>226</v>
+      </c>
+      <c r="E33" s="574" t="s">
+        <v>227</v>
+      </c>
+      <c r="F33" s="574" t="s">
+        <v>228</v>
+      </c>
+      <c r="G33" s="574" t="s">
+        <v>229</v>
+      </c>
+      <c r="H33" s="574" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="574" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="575" t="s">
+        <v>230</v>
+      </c>
+      <c r="B34" s="575" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="575" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="575" t="s">
+        <v>232</v>
+      </c>
+      <c r="E34" s="575" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" s="575" t="s">
+        <v>234</v>
+      </c>
+      <c r="G34" s="575" t="s">
+        <v>235</v>
+      </c>
+      <c r="H34" s="575" t="s">
+        <v>236</v>
+      </c>
+      <c r="I34" s="575" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="576" t="s">
+        <v>237</v>
+      </c>
+      <c r="B35" s="576" t="s">
+        <v>237</v>
+      </c>
+      <c r="C35" s="576" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" s="576" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" s="576" t="s">
+        <v>240</v>
+      </c>
+      <c r="F35" s="576" t="s">
+        <v>241</v>
+      </c>
+      <c r="G35" s="576" t="s">
+        <v>242</v>
+      </c>
+      <c r="H35" s="576" t="s">
+        <v>236</v>
+      </c>
+      <c r="I35" s="576" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="577" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="577" t="s">
+        <v>243</v>
+      </c>
+      <c r="C36" s="577" t="s">
+        <v>244</v>
+      </c>
+      <c r="D36" s="577" t="s">
+        <v>245</v>
+      </c>
+      <c r="E36" s="577" t="s">
+        <v>246</v>
+      </c>
+      <c r="F36" s="577" t="s">
+        <v>247</v>
+      </c>
+      <c r="G36" s="577" t="s">
+        <v>248</v>
+      </c>
+      <c r="H36" s="577" t="s">
+        <v>236</v>
+      </c>
+      <c r="I36" s="577" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="578" t="s">
+        <v>249</v>
+      </c>
+      <c r="B37" s="578" t="s">
+        <v>249</v>
+      </c>
+      <c r="C37" s="578" t="s">
+        <v>250</v>
+      </c>
+      <c r="D37" s="578" t="s">
+        <v>251</v>
+      </c>
+      <c r="E37" s="578" t="s">
+        <v>252</v>
+      </c>
+      <c r="F37" s="578" t="s">
+        <v>253</v>
+      </c>
+      <c r="G37" s="578" t="s">
+        <v>254</v>
+      </c>
+      <c r="H37" s="578" t="s">
+        <v>236</v>
+      </c>
+      <c r="I37" s="578" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="579" t="s">
+        <v>255</v>
+      </c>
+      <c r="B38" s="579" t="s">
+        <v>255</v>
+      </c>
+      <c r="C38" s="579" t="s">
+        <v>256</v>
+      </c>
+      <c r="D38" s="579" t="s">
+        <v>257</v>
+      </c>
+      <c r="E38" s="579" t="s">
+        <v>258</v>
+      </c>
+      <c r="F38" s="579" t="s">
+        <v>259</v>
+      </c>
+      <c r="G38" s="579" t="s">
+        <v>260</v>
+      </c>
+      <c r="H38" s="579" t="s">
+        <v>261</v>
+      </c>
+      <c r="I38" s="579" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="580" t="s">
+        <v>262</v>
+      </c>
+      <c r="B39" s="580" t="s">
+        <v>262</v>
+      </c>
+      <c r="C39" s="580" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" s="580" t="s">
+        <v>264</v>
+      </c>
+      <c r="E39" s="580" t="s">
+        <v>265</v>
+      </c>
+      <c r="F39" s="580" t="s">
+        <v>266</v>
+      </c>
+      <c r="G39" s="580" t="s">
+        <v>267</v>
+      </c>
+      <c r="H39" s="580" t="s">
+        <v>210</v>
+      </c>
+      <c r="I39" s="580" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="581" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" s="581" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" s="581" t="s">
+        <v>269</v>
+      </c>
+      <c r="D40" s="581" t="s">
+        <v>270</v>
+      </c>
+      <c r="E40" s="581" t="s">
+        <v>271</v>
+      </c>
+      <c r="F40" s="581" t="s">
+        <v>272</v>
+      </c>
+      <c r="G40" s="581" t="s">
+        <v>273</v>
+      </c>
+      <c r="H40" s="581" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="581" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="582" t="s">
+        <v>274</v>
+      </c>
+      <c r="B41" s="582" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" s="582" t="s">
+        <v>275</v>
+      </c>
+      <c r="D41" s="582" t="s">
+        <v>276</v>
+      </c>
+      <c r="E41" s="582" t="s">
+        <v>277</v>
+      </c>
+      <c r="F41" s="582" t="s">
+        <v>278</v>
+      </c>
+      <c r="G41" s="582" t="s">
+        <v>279</v>
+      </c>
+      <c r="H41" s="582" t="s">
+        <v>280</v>
+      </c>
+      <c r="I41" s="582" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="583" t="s">
+        <v>281</v>
+      </c>
+      <c r="B42" s="583" t="s">
+        <v>281</v>
+      </c>
+      <c r="C42" s="583" t="s">
+        <v>282</v>
+      </c>
+      <c r="D42" s="583" t="s">
+        <v>283</v>
+      </c>
+      <c r="E42" s="583" t="s">
+        <v>284</v>
+      </c>
+      <c r="F42" s="583" t="s">
+        <v>285</v>
+      </c>
+      <c r="G42" s="583" t="s">
+        <v>286</v>
+      </c>
+      <c r="H42" s="583" t="s">
+        <v>280</v>
+      </c>
+      <c r="I42" s="583" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="584" t="s">
+        <v>287</v>
+      </c>
+      <c r="B43" s="584" t="s">
+        <v>287</v>
+      </c>
+      <c r="C43" s="584" t="s">
+        <v>288</v>
+      </c>
+      <c r="D43" s="584" t="s">
+        <v>289</v>
+      </c>
+      <c r="E43" s="584" t="s">
+        <v>290</v>
+      </c>
+      <c r="F43" s="584" t="s">
+        <v>291</v>
+      </c>
+      <c r="G43" s="584" t="s">
+        <v>292</v>
+      </c>
+      <c r="H43" s="584" t="s">
+        <v>280</v>
+      </c>
+      <c r="I43" s="584" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="585" t="s">
+        <v>293</v>
+      </c>
+      <c r="B44" s="585" t="s">
+        <v>293</v>
+      </c>
+      <c r="C44" s="585" t="s">
+        <v>294</v>
+      </c>
+      <c r="D44" s="585" t="s">
+        <v>295</v>
+      </c>
+      <c r="E44" s="585" t="s">
+        <v>296</v>
+      </c>
+      <c r="F44" s="585" t="s">
+        <v>297</v>
+      </c>
+      <c r="G44" s="585" t="s">
+        <v>298</v>
+      </c>
+      <c r="H44" s="585" t="s">
+        <v>280</v>
+      </c>
+      <c r="I44" s="585" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="586" t="s">
+        <v>299</v>
+      </c>
+      <c r="B45" s="586" t="s">
+        <v>299</v>
+      </c>
+      <c r="C45" s="586" t="s">
+        <v>300</v>
+      </c>
+      <c r="D45" s="586" t="s">
+        <v>301</v>
+      </c>
+      <c r="E45" s="586" t="s">
+        <v>302</v>
+      </c>
+      <c r="F45" s="586" t="s">
+        <v>303</v>
+      </c>
+      <c r="G45" s="586" t="s">
+        <v>304</v>
+      </c>
+      <c r="H45" s="586" t="s">
+        <v>280</v>
+      </c>
+      <c r="I45" s="586" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="587" t="s">
+        <v>305</v>
+      </c>
+      <c r="B46" s="587" t="s">
+        <v>305</v>
+      </c>
+      <c r="C46" s="587" t="s">
+        <v>306</v>
+      </c>
+      <c r="D46" s="587" t="s">
+        <v>307</v>
+      </c>
+      <c r="E46" s="587" t="s">
+        <v>308</v>
+      </c>
+      <c r="F46" s="587" t="s">
+        <v>309</v>
+      </c>
+      <c r="G46" s="587" t="s">
+        <v>310</v>
+      </c>
+      <c r="H46" s="587" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="587" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="588" t="s">
+        <v>311</v>
+      </c>
+      <c r="B47" s="588" t="s">
+        <v>311</v>
+      </c>
+      <c r="C47" s="588" t="s">
+        <v>312</v>
+      </c>
+      <c r="D47" s="588" t="s">
+        <v>313</v>
+      </c>
+      <c r="E47" s="588" t="s">
+        <v>314</v>
+      </c>
+      <c r="F47" s="588" t="s">
+        <v>315</v>
+      </c>
+      <c r="G47" s="588" t="s">
+        <v>316</v>
+      </c>
+      <c r="H47" s="588" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="588" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="589" t="s">
+        <v>317</v>
+      </c>
+      <c r="B48" s="589" t="s">
+        <v>317</v>
+      </c>
+      <c r="C48" s="589" t="s">
+        <v>318</v>
+      </c>
+      <c r="D48" s="589" t="s">
+        <v>319</v>
+      </c>
+      <c r="E48" s="589" t="s">
+        <v>320</v>
+      </c>
+      <c r="F48" s="589" t="s">
+        <v>321</v>
+      </c>
+      <c r="G48" s="589" t="s">
+        <v>322</v>
+      </c>
+      <c r="H48" s="589" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="589" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="590" t="s">
+        <v>323</v>
+      </c>
+      <c r="B49" s="590" t="s">
+        <v>323</v>
+      </c>
+      <c r="C49" s="590" t="s">
+        <v>324</v>
+      </c>
+      <c r="D49" s="590" t="s">
+        <v>325</v>
+      </c>
+      <c r="E49" s="590" t="s">
+        <v>326</v>
+      </c>
+      <c r="F49" s="590" t="s">
+        <v>327</v>
+      </c>
+      <c r="G49" s="590" t="s">
+        <v>328</v>
+      </c>
+      <c r="H49" s="590" t="s">
+        <v>329</v>
+      </c>
+      <c r="I49" s="590" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="591" t="s">
+        <v>330</v>
+      </c>
+      <c r="B50" s="591" t="s">
+        <v>330</v>
+      </c>
+      <c r="C50" s="591" t="s">
+        <v>331</v>
+      </c>
+      <c r="D50" s="591" t="s">
+        <v>332</v>
+      </c>
+      <c r="E50" s="591" t="s">
+        <v>333</v>
+      </c>
+      <c r="F50" s="591" t="s">
+        <v>334</v>
+      </c>
+      <c r="G50" s="591" t="s">
+        <v>335</v>
+      </c>
+      <c r="H50" s="591" t="s">
+        <v>329</v>
+      </c>
+      <c r="I50" s="591" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="592" t="s">
+        <v>336</v>
+      </c>
+      <c r="B51" s="592" t="s">
+        <v>336</v>
+      </c>
+      <c r="C51" s="592" t="s">
+        <v>337</v>
+      </c>
+      <c r="D51" s="592" t="s">
+        <v>338</v>
+      </c>
+      <c r="E51" s="592" t="s">
+        <v>339</v>
+      </c>
+      <c r="F51" s="592" t="s">
+        <v>340</v>
+      </c>
+      <c r="G51" s="592" t="s">
+        <v>341</v>
+      </c>
+      <c r="H51" s="592" t="s">
+        <v>329</v>
+      </c>
+      <c r="I51" s="592" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the javadoc for the root and assertions package
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4781" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4817" uniqueCount="342">
   <si>
     <t>URL</t>
   </si>
@@ -1124,7 +1124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="90">
+  <fills count="91">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1572,8 +1572,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="350">
+  <borders count="354">
     <border>
       <left/>
       <right/>
@@ -3162,11 +3167,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="593">
+  <cellXfs count="597">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4942,6 +4965,18 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="90" borderId="353" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="353" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="353" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="353" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -5266,1493 +5301,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="82.36328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="82.36328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="56.2421875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="145.84375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="40.71484375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="133.88671875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="188.4921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="10.87109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="542" t="s">
+      <c r="A1" s="593" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="542" t="s">
+      <c r="B1" s="593" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="542" t="s">
+      <c r="C1" s="593" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="542" t="s">
+      <c r="D1" s="593" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="542" t="s">
+      <c r="E1" s="593" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="542" t="s">
+      <c r="F1" s="593" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="542" t="s">
+      <c r="G1" s="593" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="542" t="s">
+      <c r="H1" s="593" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="542" t="s">
+      <c r="I1" s="593" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="543" t="s">
+      <c r="A2" s="594" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="543" t="s">
+      <c r="B2" s="594" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="543" t="s">
+      <c r="C2" s="594" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="543" t="s">
+      <c r="D2" s="594" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="543" t="s">
+      <c r="E2" s="594" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="543" t="s">
+      <c r="F2" s="594" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="543" t="s">
+      <c r="G2" s="594" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="543" t="s">
+      <c r="H2" s="594" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="543" t="s">
+      <c r="I2" s="594" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="544" t="s">
+      <c r="A3" s="595" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="544" t="s">
+      <c r="B3" s="595" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="544" t="s">
+      <c r="C3" s="595" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="544" t="s">
+      <c r="D3" s="595" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="544" t="s">
+      <c r="E3" s="595" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="544" t="s">
+      <c r="F3" s="595" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="544" t="s">
+      <c r="G3" s="595" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="544" t="s">
+      <c r="H3" s="595" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="544" t="s">
+      <c r="I3" s="595" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="545" t="s">
+      <c r="A4" s="596" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="545" t="s">
+      <c r="B4" s="596" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="545" t="s">
+      <c r="C4" s="596" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="545" t="s">
+      <c r="D4" s="596" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="545" t="s">
+      <c r="E4" s="596" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="545" t="s">
+      <c r="F4" s="596" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="545" t="s">
+      <c r="G4" s="596" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="545" t="s">
+      <c r="H4" s="596" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="545" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="546" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="546" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="546" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="546" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="546" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="546" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="546" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="546" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="546" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="547" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="547" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="547" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="547" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="547" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="547" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="547" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="547" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="547" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="548" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="548" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="548" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="548" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="548" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="548" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="548" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="548" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="548" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="549" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="549" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="549" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="549" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="549" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="549" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="549" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="549" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="549" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="550" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="550" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="550" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="550" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="550" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="550" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="550" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="550" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="550" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="551" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="551" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="551" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="551" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="551" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="551" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="551" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="551" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="551" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="552" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="552" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="552" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="552" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="552" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="552" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="552" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="552" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" s="552" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="553" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="553" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="553" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="553" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="553" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="553" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="553" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="553" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="553" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="554" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="554" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="554" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="554" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="554" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="554" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="554" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="554" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" s="554" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="555" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="555" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="555" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="555" t="s">
-        <v>152</v>
-      </c>
-      <c r="E14" s="555" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="555" t="s">
-        <v>153</v>
-      </c>
-      <c r="G14" s="555" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" s="555" t="s">
-        <v>96</v>
-      </c>
-      <c r="I14" s="555" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="556" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="556" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="556" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="556" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="556" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="556" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="556" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="556" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="556" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="557" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="557" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="557" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="557" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="557" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="557" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="557" t="s">
-        <v>108</v>
-      </c>
-      <c r="H16" s="557" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="557" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="558" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="558" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="558" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="558" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="558" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="558" t="s">
-        <v>113</v>
-      </c>
-      <c r="G17" s="558" t="s">
-        <v>114</v>
-      </c>
-      <c r="H17" s="558" t="s">
-        <v>115</v>
-      </c>
-      <c r="I17" s="558" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="559" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" s="559" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="559" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="559" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="559" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="559" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="559" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" s="559" t="s">
-        <v>115</v>
-      </c>
-      <c r="I18" s="559" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="560" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" s="560" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="560" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="560" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="560" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="560" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" s="560" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="560" t="s">
-        <v>115</v>
-      </c>
-      <c r="I19" s="560" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="561" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="561" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="561" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="561" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="561" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="561" t="s">
-        <v>132</v>
-      </c>
-      <c r="G20" s="561" t="s">
-        <v>133</v>
-      </c>
-      <c r="H20" s="561" t="s">
-        <v>115</v>
-      </c>
-      <c r="I20" s="561" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="562" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="562" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="562" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="562" t="s">
-        <v>136</v>
-      </c>
-      <c r="E21" s="562" t="s">
-        <v>137</v>
-      </c>
-      <c r="F21" s="562" t="s">
-        <v>138</v>
-      </c>
-      <c r="G21" s="562" t="s">
-        <v>139</v>
-      </c>
-      <c r="H21" s="562" t="s">
-        <v>115</v>
-      </c>
-      <c r="I21" s="562" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="563" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" s="563" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="563" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="563" t="s">
-        <v>156</v>
-      </c>
-      <c r="E22" s="563" t="s">
-        <v>157</v>
-      </c>
-      <c r="F22" s="563" t="s">
-        <v>158</v>
-      </c>
-      <c r="G22" s="563" t="s">
-        <v>159</v>
-      </c>
-      <c r="H22" s="563" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" s="563" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="564" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="564" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" s="564" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="564" t="s">
-        <v>162</v>
-      </c>
-      <c r="E23" s="564" t="s">
-        <v>163</v>
-      </c>
-      <c r="F23" s="564" t="s">
-        <v>164</v>
-      </c>
-      <c r="G23" s="564" t="s">
-        <v>165</v>
-      </c>
-      <c r="H23" s="564" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="564" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="565" t="s">
-        <v>166</v>
-      </c>
-      <c r="B24" s="565" t="s">
-        <v>166</v>
-      </c>
-      <c r="C24" s="565" t="s">
-        <v>167</v>
-      </c>
-      <c r="D24" s="565" t="s">
-        <v>168</v>
-      </c>
-      <c r="E24" s="565" t="s">
-        <v>169</v>
-      </c>
-      <c r="F24" s="565" t="s">
-        <v>170</v>
-      </c>
-      <c r="G24" s="565" t="s">
-        <v>171</v>
-      </c>
-      <c r="H24" s="565" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="565" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="566" t="s">
-        <v>173</v>
-      </c>
-      <c r="B25" s="566" t="s">
-        <v>173</v>
-      </c>
-      <c r="C25" s="566" t="s">
-        <v>174</v>
-      </c>
-      <c r="D25" s="566" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="566" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" s="566" t="s">
-        <v>177</v>
-      </c>
-      <c r="G25" s="566" t="s">
-        <v>178</v>
-      </c>
-      <c r="H25" s="566" t="s">
-        <v>172</v>
-      </c>
-      <c r="I25" s="566" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="567" t="s">
-        <v>179</v>
-      </c>
-      <c r="B26" s="567" t="s">
-        <v>179</v>
-      </c>
-      <c r="C26" s="567" t="s">
-        <v>180</v>
-      </c>
-      <c r="D26" s="567" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="567" t="s">
-        <v>182</v>
-      </c>
-      <c r="F26" s="567" t="s">
-        <v>183</v>
-      </c>
-      <c r="G26" s="567" t="s">
-        <v>184</v>
-      </c>
-      <c r="H26" s="567" t="s">
-        <v>185</v>
-      </c>
-      <c r="I26" s="567" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="568" t="s">
-        <v>186</v>
-      </c>
-      <c r="B27" s="568" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="568" t="s">
-        <v>187</v>
-      </c>
-      <c r="D27" s="568" t="s">
-        <v>188</v>
-      </c>
-      <c r="E27" s="568" t="s">
-        <v>189</v>
-      </c>
-      <c r="F27" s="568" t="s">
-        <v>190</v>
-      </c>
-      <c r="G27" s="568" t="s">
-        <v>191</v>
-      </c>
-      <c r="H27" s="568" t="s">
-        <v>185</v>
-      </c>
-      <c r="I27" s="568" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="569" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="569" t="s">
-        <v>192</v>
-      </c>
-      <c r="C28" s="569" t="s">
-        <v>193</v>
-      </c>
-      <c r="D28" s="569" t="s">
-        <v>194</v>
-      </c>
-      <c r="E28" s="569" t="s">
-        <v>195</v>
-      </c>
-      <c r="F28" s="569" t="s">
-        <v>196</v>
-      </c>
-      <c r="G28" s="569" t="s">
-        <v>197</v>
-      </c>
-      <c r="H28" s="569" t="s">
-        <v>185</v>
-      </c>
-      <c r="I28" s="569" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="570" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="570" t="s">
-        <v>198</v>
-      </c>
-      <c r="C29" s="570" t="s">
-        <v>199</v>
-      </c>
-      <c r="D29" s="570" t="s">
-        <v>200</v>
-      </c>
-      <c r="E29" s="570" t="s">
-        <v>201</v>
-      </c>
-      <c r="F29" s="570" t="s">
-        <v>202</v>
-      </c>
-      <c r="G29" s="570" t="s">
-        <v>203</v>
-      </c>
-      <c r="H29" s="570" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="570" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="571" t="s">
-        <v>204</v>
-      </c>
-      <c r="B30" s="571" t="s">
-        <v>204</v>
-      </c>
-      <c r="C30" s="571" t="s">
-        <v>205</v>
-      </c>
-      <c r="D30" s="571" t="s">
-        <v>206</v>
-      </c>
-      <c r="E30" s="571" t="s">
-        <v>207</v>
-      </c>
-      <c r="F30" s="571" t="s">
-        <v>208</v>
-      </c>
-      <c r="G30" s="571" t="s">
-        <v>209</v>
-      </c>
-      <c r="H30" s="571" t="s">
-        <v>210</v>
-      </c>
-      <c r="I30" s="571" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="572" t="s">
-        <v>211</v>
-      </c>
-      <c r="B31" s="572" t="s">
-        <v>211</v>
-      </c>
-      <c r="C31" s="572" t="s">
-        <v>212</v>
-      </c>
-      <c r="D31" s="572" t="s">
-        <v>213</v>
-      </c>
-      <c r="E31" s="572" t="s">
-        <v>214</v>
-      </c>
-      <c r="F31" s="572" t="s">
-        <v>215</v>
-      </c>
-      <c r="G31" s="572" t="s">
-        <v>216</v>
-      </c>
-      <c r="H31" s="572" t="s">
-        <v>210</v>
-      </c>
-      <c r="I31" s="572" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="573" t="s">
-        <v>217</v>
-      </c>
-      <c r="B32" s="573" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="573" t="s">
-        <v>218</v>
-      </c>
-      <c r="D32" s="573" t="s">
-        <v>219</v>
-      </c>
-      <c r="E32" s="573" t="s">
-        <v>220</v>
-      </c>
-      <c r="F32" s="573" t="s">
-        <v>221</v>
-      </c>
-      <c r="G32" s="573" t="s">
-        <v>222</v>
-      </c>
-      <c r="H32" s="573" t="s">
-        <v>223</v>
-      </c>
-      <c r="I32" s="573" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="574" t="s">
-        <v>224</v>
-      </c>
-      <c r="B33" s="574" t="s">
-        <v>224</v>
-      </c>
-      <c r="C33" s="574" t="s">
-        <v>225</v>
-      </c>
-      <c r="D33" s="574" t="s">
-        <v>226</v>
-      </c>
-      <c r="E33" s="574" t="s">
-        <v>227</v>
-      </c>
-      <c r="F33" s="574" t="s">
-        <v>228</v>
-      </c>
-      <c r="G33" s="574" t="s">
-        <v>229</v>
-      </c>
-      <c r="H33" s="574" t="s">
-        <v>24</v>
-      </c>
-      <c r="I33" s="574" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="575" t="s">
-        <v>230</v>
-      </c>
-      <c r="B34" s="575" t="s">
-        <v>230</v>
-      </c>
-      <c r="C34" s="575" t="s">
-        <v>231</v>
-      </c>
-      <c r="D34" s="575" t="s">
-        <v>232</v>
-      </c>
-      <c r="E34" s="575" t="s">
-        <v>233</v>
-      </c>
-      <c r="F34" s="575" t="s">
-        <v>234</v>
-      </c>
-      <c r="G34" s="575" t="s">
-        <v>235</v>
-      </c>
-      <c r="H34" s="575" t="s">
-        <v>236</v>
-      </c>
-      <c r="I34" s="575" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="576" t="s">
-        <v>237</v>
-      </c>
-      <c r="B35" s="576" t="s">
-        <v>237</v>
-      </c>
-      <c r="C35" s="576" t="s">
-        <v>238</v>
-      </c>
-      <c r="D35" s="576" t="s">
-        <v>239</v>
-      </c>
-      <c r="E35" s="576" t="s">
-        <v>240</v>
-      </c>
-      <c r="F35" s="576" t="s">
-        <v>241</v>
-      </c>
-      <c r="G35" s="576" t="s">
-        <v>242</v>
-      </c>
-      <c r="H35" s="576" t="s">
-        <v>236</v>
-      </c>
-      <c r="I35" s="576" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="577" t="s">
-        <v>243</v>
-      </c>
-      <c r="B36" s="577" t="s">
-        <v>243</v>
-      </c>
-      <c r="C36" s="577" t="s">
-        <v>244</v>
-      </c>
-      <c r="D36" s="577" t="s">
-        <v>245</v>
-      </c>
-      <c r="E36" s="577" t="s">
-        <v>246</v>
-      </c>
-      <c r="F36" s="577" t="s">
-        <v>247</v>
-      </c>
-      <c r="G36" s="577" t="s">
-        <v>248</v>
-      </c>
-      <c r="H36" s="577" t="s">
-        <v>236</v>
-      </c>
-      <c r="I36" s="577" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="578" t="s">
-        <v>249</v>
-      </c>
-      <c r="B37" s="578" t="s">
-        <v>249</v>
-      </c>
-      <c r="C37" s="578" t="s">
-        <v>250</v>
-      </c>
-      <c r="D37" s="578" t="s">
-        <v>251</v>
-      </c>
-      <c r="E37" s="578" t="s">
-        <v>252</v>
-      </c>
-      <c r="F37" s="578" t="s">
-        <v>253</v>
-      </c>
-      <c r="G37" s="578" t="s">
-        <v>254</v>
-      </c>
-      <c r="H37" s="578" t="s">
-        <v>236</v>
-      </c>
-      <c r="I37" s="578" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="579" t="s">
-        <v>255</v>
-      </c>
-      <c r="B38" s="579" t="s">
-        <v>255</v>
-      </c>
-      <c r="C38" s="579" t="s">
-        <v>256</v>
-      </c>
-      <c r="D38" s="579" t="s">
-        <v>257</v>
-      </c>
-      <c r="E38" s="579" t="s">
-        <v>258</v>
-      </c>
-      <c r="F38" s="579" t="s">
-        <v>259</v>
-      </c>
-      <c r="G38" s="579" t="s">
-        <v>260</v>
-      </c>
-      <c r="H38" s="579" t="s">
-        <v>261</v>
-      </c>
-      <c r="I38" s="579" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="580" t="s">
-        <v>262</v>
-      </c>
-      <c r="B39" s="580" t="s">
-        <v>262</v>
-      </c>
-      <c r="C39" s="580" t="s">
-        <v>263</v>
-      </c>
-      <c r="D39" s="580" t="s">
-        <v>264</v>
-      </c>
-      <c r="E39" s="580" t="s">
-        <v>265</v>
-      </c>
-      <c r="F39" s="580" t="s">
-        <v>266</v>
-      </c>
-      <c r="G39" s="580" t="s">
-        <v>267</v>
-      </c>
-      <c r="H39" s="580" t="s">
-        <v>210</v>
-      </c>
-      <c r="I39" s="580" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="581" t="s">
-        <v>268</v>
-      </c>
-      <c r="B40" s="581" t="s">
-        <v>268</v>
-      </c>
-      <c r="C40" s="581" t="s">
-        <v>269</v>
-      </c>
-      <c r="D40" s="581" t="s">
-        <v>270</v>
-      </c>
-      <c r="E40" s="581" t="s">
-        <v>271</v>
-      </c>
-      <c r="F40" s="581" t="s">
-        <v>272</v>
-      </c>
-      <c r="G40" s="581" t="s">
-        <v>273</v>
-      </c>
-      <c r="H40" s="581" t="s">
-        <v>24</v>
-      </c>
-      <c r="I40" s="581" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="582" t="s">
-        <v>274</v>
-      </c>
-      <c r="B41" s="582" t="s">
-        <v>274</v>
-      </c>
-      <c r="C41" s="582" t="s">
-        <v>275</v>
-      </c>
-      <c r="D41" s="582" t="s">
-        <v>276</v>
-      </c>
-      <c r="E41" s="582" t="s">
-        <v>277</v>
-      </c>
-      <c r="F41" s="582" t="s">
-        <v>278</v>
-      </c>
-      <c r="G41" s="582" t="s">
-        <v>279</v>
-      </c>
-      <c r="H41" s="582" t="s">
-        <v>280</v>
-      </c>
-      <c r="I41" s="582" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="583" t="s">
-        <v>281</v>
-      </c>
-      <c r="B42" s="583" t="s">
-        <v>281</v>
-      </c>
-      <c r="C42" s="583" t="s">
-        <v>282</v>
-      </c>
-      <c r="D42" s="583" t="s">
-        <v>283</v>
-      </c>
-      <c r="E42" s="583" t="s">
-        <v>284</v>
-      </c>
-      <c r="F42" s="583" t="s">
-        <v>285</v>
-      </c>
-      <c r="G42" s="583" t="s">
-        <v>286</v>
-      </c>
-      <c r="H42" s="583" t="s">
-        <v>280</v>
-      </c>
-      <c r="I42" s="583" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="584" t="s">
-        <v>287</v>
-      </c>
-      <c r="B43" s="584" t="s">
-        <v>287</v>
-      </c>
-      <c r="C43" s="584" t="s">
-        <v>288</v>
-      </c>
-      <c r="D43" s="584" t="s">
-        <v>289</v>
-      </c>
-      <c r="E43" s="584" t="s">
-        <v>290</v>
-      </c>
-      <c r="F43" s="584" t="s">
-        <v>291</v>
-      </c>
-      <c r="G43" s="584" t="s">
-        <v>292</v>
-      </c>
-      <c r="H43" s="584" t="s">
-        <v>280</v>
-      </c>
-      <c r="I43" s="584" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="585" t="s">
-        <v>293</v>
-      </c>
-      <c r="B44" s="585" t="s">
-        <v>293</v>
-      </c>
-      <c r="C44" s="585" t="s">
-        <v>294</v>
-      </c>
-      <c r="D44" s="585" t="s">
-        <v>295</v>
-      </c>
-      <c r="E44" s="585" t="s">
-        <v>296</v>
-      </c>
-      <c r="F44" s="585" t="s">
-        <v>297</v>
-      </c>
-      <c r="G44" s="585" t="s">
-        <v>298</v>
-      </c>
-      <c r="H44" s="585" t="s">
-        <v>280</v>
-      </c>
-      <c r="I44" s="585" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="586" t="s">
-        <v>299</v>
-      </c>
-      <c r="B45" s="586" t="s">
-        <v>299</v>
-      </c>
-      <c r="C45" s="586" t="s">
-        <v>300</v>
-      </c>
-      <c r="D45" s="586" t="s">
-        <v>301</v>
-      </c>
-      <c r="E45" s="586" t="s">
-        <v>302</v>
-      </c>
-      <c r="F45" s="586" t="s">
-        <v>303</v>
-      </c>
-      <c r="G45" s="586" t="s">
-        <v>304</v>
-      </c>
-      <c r="H45" s="586" t="s">
-        <v>280</v>
-      </c>
-      <c r="I45" s="586" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="587" t="s">
-        <v>305</v>
-      </c>
-      <c r="B46" s="587" t="s">
-        <v>305</v>
-      </c>
-      <c r="C46" s="587" t="s">
-        <v>306</v>
-      </c>
-      <c r="D46" s="587" t="s">
-        <v>307</v>
-      </c>
-      <c r="E46" s="587" t="s">
-        <v>308</v>
-      </c>
-      <c r="F46" s="587" t="s">
-        <v>309</v>
-      </c>
-      <c r="G46" s="587" t="s">
-        <v>310</v>
-      </c>
-      <c r="H46" s="587" t="s">
-        <v>17</v>
-      </c>
-      <c r="I46" s="587" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="588" t="s">
-        <v>311</v>
-      </c>
-      <c r="B47" s="588" t="s">
-        <v>311</v>
-      </c>
-      <c r="C47" s="588" t="s">
-        <v>312</v>
-      </c>
-      <c r="D47" s="588" t="s">
-        <v>313</v>
-      </c>
-      <c r="E47" s="588" t="s">
-        <v>314</v>
-      </c>
-      <c r="F47" s="588" t="s">
-        <v>315</v>
-      </c>
-      <c r="G47" s="588" t="s">
-        <v>316</v>
-      </c>
-      <c r="H47" s="588" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="588" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="589" t="s">
-        <v>317</v>
-      </c>
-      <c r="B48" s="589" t="s">
-        <v>317</v>
-      </c>
-      <c r="C48" s="589" t="s">
-        <v>318</v>
-      </c>
-      <c r="D48" s="589" t="s">
-        <v>319</v>
-      </c>
-      <c r="E48" s="589" t="s">
-        <v>320</v>
-      </c>
-      <c r="F48" s="589" t="s">
-        <v>321</v>
-      </c>
-      <c r="G48" s="589" t="s">
-        <v>322</v>
-      </c>
-      <c r="H48" s="589" t="s">
-        <v>24</v>
-      </c>
-      <c r="I48" s="589" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="590" t="s">
-        <v>323</v>
-      </c>
-      <c r="B49" s="590" t="s">
-        <v>323</v>
-      </c>
-      <c r="C49" s="590" t="s">
-        <v>324</v>
-      </c>
-      <c r="D49" s="590" t="s">
-        <v>325</v>
-      </c>
-      <c r="E49" s="590" t="s">
-        <v>326</v>
-      </c>
-      <c r="F49" s="590" t="s">
-        <v>327</v>
-      </c>
-      <c r="G49" s="590" t="s">
-        <v>328</v>
-      </c>
-      <c r="H49" s="590" t="s">
-        <v>329</v>
-      </c>
-      <c r="I49" s="590" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="591" t="s">
-        <v>330</v>
-      </c>
-      <c r="B50" s="591" t="s">
-        <v>330</v>
-      </c>
-      <c r="C50" s="591" t="s">
-        <v>331</v>
-      </c>
-      <c r="D50" s="591" t="s">
-        <v>332</v>
-      </c>
-      <c r="E50" s="591" t="s">
-        <v>333</v>
-      </c>
-      <c r="F50" s="591" t="s">
-        <v>334</v>
-      </c>
-      <c r="G50" s="591" t="s">
-        <v>335</v>
-      </c>
-      <c r="H50" s="591" t="s">
-        <v>329</v>
-      </c>
-      <c r="I50" s="591" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="592" t="s">
-        <v>336</v>
-      </c>
-      <c r="B51" s="592" t="s">
-        <v>336</v>
-      </c>
-      <c r="C51" s="592" t="s">
-        <v>337</v>
-      </c>
-      <c r="D51" s="592" t="s">
-        <v>338</v>
-      </c>
-      <c r="E51" s="592" t="s">
-        <v>339</v>
-      </c>
-      <c r="F51" s="592" t="s">
-        <v>340</v>
-      </c>
-      <c r="G51" s="592" t="s">
-        <v>341</v>
-      </c>
-      <c r="H51" s="592" t="s">
-        <v>329</v>
-      </c>
-      <c r="I51" s="592" t="s">
+      <c r="I4" s="596" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added javadoc for the modules and the util packages
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4817" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5726" uniqueCount="646">
   <si>
     <t>URL</t>
   </si>
@@ -1100,6 +1100,938 @@
   </si>
   <si>
     <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Accessories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+american+classic+blend+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley American Classic Blend Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley American Classic cigars are an affordably-priced edition inspired by the cigars that were popular in America during the early part of the 20th...</t>
+  </si>
+  <si>
+    <t>Alec Bradley American Classic Blend Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley American Classic cigars are an affordably-priced edition inspired by the cigars that were popular in America during the early part of the 20th century. A mild to medium-bodied blend of specially-aged Nicaraguan Estelí and Condega longfillers, Nicaraguan Jalapa binder, and a Honduran-grown Connecticut seed wrapper offer you a smooth, creamy and complex smoke with excellent balance, sweet cedar notes, and a distinct nutty flavor on the finish. Another ABC winner! Order your box now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley American Classic Blend Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+american+sun+grown+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley American Sun Grown Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley American Sun Grown cigars offer you a savory Nicaraguan &lt;i&gt;puro&lt;/i&gt; with a little more depth, body, and spice than their American Classic...</t>
+  </si>
+  <si>
+    <t>Alec Bradley American Sun Grown Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley American Sun Grown cigars offer you a savory Nicaraguan puro with a little more depth, body, and spice than their American Classic sisters. Thanks to a sun-kissed Jalapa Habano capa that's richer in flavor and aroma, this opulent leaf surrounds a full-flavored blend of Esteli &amp; Condega long-fillers, plus a Jalapa binder for a smooth, perfectly-balanced smoke with more spice flavors directed to the palate. Very impressive! Add some to your cart now and compare.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley American Sun Grown Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+black+market+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Black Market Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Black Market cigars are a medium-bodied, luxury-class edition blended with Honduran Jamastran (pronounced ha-mas-tran) and Panamanian...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Black Market Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Black Market cigars are a medium-bodied, luxury-class edition blended with Honduran Jamastran (pronounced ha-mas-tran) and Panamanian longfillers, Sumatra binder, and semi-sweet Nicaraguan Jalapa wrapper cured to a dark, shimmering patina. You'll enjoy an ultra-smooth and creamy smoke laced with spicy notes that finishes with a hint of sweetness on the palate. Order your box of this stunning selection now and discover why Alec Bradley cigars are rated outstanding so often.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Black Market Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+connecticut+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Connecticut Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Connecticut cigars contain a blend of Nicaraguan and Honduran longfillers, with Honduran binders and Ecuadorian Connecticut Shade wrappers....</t>
+  </si>
+  <si>
+    <t>Alec Bradley Connecticut Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Connecticut cigars contain a blend of Nicaraguan and Honduran longfillers, with Honduran binders and Ecuadorian Connecticut Shade wrappers. The cigars are mild to medium in strength, with a little more spice and complexity than you'd expect from a Connecticut cigar. Perfect for those who appreciate a flavorful milder cigar, or for the fuller-bodied smoker looking for a mellow or morning burner that still has plenty of flavor.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Connecticut Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+coyol+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Coyol Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Coyol cigars are something special to say the least. Their cigars are all top notch, but this one puts the brand over the edge. Each cigar is...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Coyol Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Coyol cigars are something special to say the least. Their cigars are all top notch, but this one puts the brand over the edge. Each cigar is hand rolled using tobacco from the land in which the cigar is named. That means that you're getting rare tobaccos that have an incredible flavor and aroma qualities not found anywhere else. Add in some Nicaraguan binder and filler tobaccos, and you have a flavor bomb like you've never experienced. Get your box of Coyol today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Coyol Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+factory+selects+ab1+habano+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB1 Habano Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB1 Habano cigars at Famous Smoke Shop. High-quality, medium-bodied cigars online at discount prices in money-saving bundles.</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB1 Habano Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB1 Habano cigars are one of the best bundle cigar buys in the house. Handmade with a complex recipe of Central American-grown long-fillers aged to perfection, the cigars are expertly rolled in Nicaraguan Habano maduro wrappers (some in natural Habano), for a creamy, medium-bodied pleasure cruise you can sail along with any time of day. When the quality and flavor is this good, why pay more for a box? Choose from a number of popular sizes and get onboard.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Factory Selects AB1 Habano Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+factory+selects+ab3+connecticut+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB3 Connecticut Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Buy Alec Bradley Factory Selects AB3 Connecticut bundle cigars online at Famous Smoke Shop. Top-quality, medium-bodied cigars, great for new cigar smokers.</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB3 Connecticut Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB3 Connecticut cigars look a lot more expensive than they cost. That's because they're up-market, box-quality smokes presented in value-priced bundles to save you money. Rolled in Honduran-grown Connecticut-seed wrappers, the medium-bodied smoke is especially creamy revealing a distinctive, sweet spice component that dovetails with earthy notes, sweet wood, and nuts for a well-balanced, anytime treat. Excellent for new cigar smokers and fans of milder primos!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Factory Selects AB3 Connecticut Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+factory+selects+ab5+maduro+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB5 Maduro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB5 Maduro cigars are discount bundle cigars that taste like the high-priced boxed brands. Order now from Famous Smoke Shop.</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB5 Maduro Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB5 Maduro cigars get you Alec Bradley Cigars' highly-rated flavor at an affordable bundle cigar price. Rolled in oily, Honduran-grown maduro wrappers, these medium-bodied cigars reveal a full-flavored, palate-pleasing smoke brimming with dark, earthy, and spicy notes on a long, satisfying finish. If you're looking for a discount cigar with all the quality of the higher-priced fare, grab this money-saving selection now. Only you have to know what you paid for 'em!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Factory Selects AB5 Maduro Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+factory+selects+ab7+corojo+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB7 Corojo Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB7 Corojo Cigars are a slow burning, full-flavored cigar delivers big time at a price that is too good to pass up from Famous Smoke.</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB7 Corojo Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB7 Corojo Cigars may be a mouthful to ask for by name, but once you light up your first cigar, the only thing you’ll hear is the relaxing slow crisp burn of premium tobacco smoldering in your hand. Using a Cubanesque Corojo wrapper encasing premium filler tobaccos, this slow burning, full-flavored cigar delivers big time at a price that is too good to pass up. It’s not every day you’ll come across a cigar this good at a price like this. Get yours today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Factory Selects AB7 Corojo Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+factory+selects+ab9+sumatra+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB9 Sumatra Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Buy Alec Bradley Factory Selects AB9 Sumatra cigars at Famous Smoke Shop. One of the best bundle cigar values online presented in savory Sumatra wrappers.</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB9 Sumatra Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Factory Selects AB9 Sumatra cigars are high-quality cigars presented in economical bundles for cigar smokers who want a solid, medium-bodied handmade at way below box prices. This selection is blended with perfectly-aged long-fillers &amp; binders rolled in your choice of delicately spicy Sumatra natural or slightly sweeter maduro wrappers. A smart buy for new cigar smokers as well as budget-minded enthusiasts looking for a great cigar value.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Factory Selects AB9 Sumatra Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+family+blend+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Family Blend Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Family Blend cigars are expertly blended at Tabacos Raices Cubanas in Honduras, the factory that also makes Alec Bradley Tempus and Prensado...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Family Blend Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Family Blend cigars are expertly blended at Tabacos Raices Cubanas in Honduras, the factory that also makes Alec Bradley Tempus and Prensado cigars. Family Blend consists of specially selected Honduran &amp; Nicaraguan longfillers, plus an Indonesian binder seamlessly rolled in a gorgeous, carefully aged Honduran Trojes wrapper. Expect a well-balanced, medium-bodied cigar brimming with rich flavor underpinned by delectably subtle nuances. Join the family of Alec Bradley cigar lovers and order a box now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Family Blend Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+maxx+original+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley MAXX Original Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley MAXX cigars represent the apex of big, bold luxury cigars. From their meticulous handcraftsmanship, to their perfectly-balanced fusion of...</t>
+  </si>
+  <si>
+    <t>Alec Bradley MAXX Original Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley MAXX cigars represent the apex of big, bold luxury cigars. From their meticulous handcraftsmanship, to their perfectly-balanced fusion of dark, sweet tobacco flavors and sumptuous aroma, MAXX is one helluva smoke. Each MAXX cigar has a creamy, rich-tasting blend of Ligero &amp; Viso tobaccos from Colombia, Nicaragua, Mexico and Honduras with a savory Costa Rican binder, seamlessly rolled in a hearty Nicaraguan Habano wrapper. Ready to take your taste buds to the max? Try a MAXX today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley MAXX Original Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+mundial+punta+lanza+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Mundial Punta Lanza Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Mundial cigars are quickly turning heads in the industry and has collectors rushing to cigar shops world wide. Alan Rubin, the owner of Alec...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Mundial Punta Lanza Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Mundial cigars are quickly turning heads in the industry and has collectors rushing to cigar shops world wide. Alan Rubin, the owner of Alec Bradley has spent 5 years blending and tweaking this cigar to make sure it is absolutely perfect before releasing it upon the world. The results are incredible. The filler and binders are blended using Honduran and Nicaraguan tobaccos, all wrapped in a lush Honduran leaf from the Trojes region. Perfect in every way. Pick yours up now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Mundial Punta Lanza Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+new+baby+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley New Baby Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley New Baby Cigars</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All It's A Boy. It's A Girl. Brands » Alec Bradley New Baby Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/its+a+boy.+its+a+girl.+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+nica+puro+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Nica Puro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Nica Puro cigars are the first Nicaraguan puro cigar that Alec Bradley has ever introduced to the market. Considered a tribute to the city of...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Nica Puro Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Nica Puro cigars are the first Nicaraguan puro cigar that Alec Bradley has ever introduced to the market. Considered a tribute to the city of Esteli, Nicaragua with the year 1685 being featured on the label, this cigar offers a complex blend of all Nicaraguan long-fillers with an oily Criollo wrapper to tie it all together for a smoking experience that really showcases how fantastic Nicaraguan tobaccos are. A true gem worthy of securing a spot in any cigar enthusiast's humidor.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Nica Puro Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+nica+puro+rosado+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Nica Puro Rosado Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Nica Puro Rosado cigars are the long-awaited sequel to Alec Bradley's highly-rated Nica Puro cigars. The golden Rosado Colorado wrapper is...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Nica Puro Rosado Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Nica Puro Rosado cigars are the long-awaited sequel to Alec Bradley's highly-rated Nica Puro cigars. The golden Rosado Colorado wrapper is what distinguishes this affordable edition from its darker brothers, while living true to its Nicaraguan puro pedigree. Their blend of dense double-binders and tobaccos from Nicaragua's Jalapa, Esteli and Condega growing regions will satisfy both novice and expert palates alike. Discover this truly essential experience by trying some today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Nica Puro Rosado Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+overture+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Overture Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Overture cigars follow Alec Bradley's fine tradition of producing some of the world's most highly-rated full-flavored premium cigars. Overture...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Overture Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Overture cigars follow Alec Bradley's fine tradition of producing some of the world's most highly-rated full-flavored premium cigars. Overture employs a well-balanced blend of Honduran Trojes and Nicaraguan Jalapa longfillers married to a luscious Honduran Trojes Viso wrapper. You'll enjoy a creamy, full-bodied symphony of complex flavors offering traces of oak, cedar, sweet spices, and espresso on the finish. Add a box or a 5-pack of these savory cigars to your cart today.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Overture Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+prensado+1+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Prensado Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Prensado cigars are the first all BOX-PRESSED selection from Alec Bradley Cigars, and arguably their most muscular to-date. Made at Raices...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Prensado Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Prensado cigars are the first all BOX-PRESSED selection from Alec Bradley Cigars, and arguably their most muscular to-date. Made at Raices Cubanas in Honduras, the blend starts with carefully chosen Honduran and Nicaraguan longfillers girded in a Nicaraguan Jalapa binder. But the pièce de résistance of these cigars are the Honduran Trojes Corojo 2006 wrappers. Expect a very smooth, yet potent smoke rife with deep, dark-roasted coffee and pepper flavors. Very impressive!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Prensado Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+raices+cubanas+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Raices Cubanas Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Raices Cubanas pits the well-known tobaccos of Nicaraguan against Honduran tobacco, in an all out battle royal to see who's flavor comes out...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Raices Cubanas Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Raices Cubanas pits the well-known tobaccos of Nicaraguan against Honduran tobacco, in an all out battle royal to see who's flavor comes out on top, and your taste buds are the judge. The binder and filler are where these two titans of tobacco duke it out, with Honduras hosting a Criollo wrapper. This full bodied beauty will entertain your palate better than any prized heavyweight fight there ever was or will be. Don't pass up a chance to experience this epic battle. Get yours now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Raices Cubanas Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+sanctum+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Sanctum Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Sanctum cigars present another flavor-packed edition from one of the world's best boutique cigar brands. Perfectly-aged long-fillers from...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Sanctum Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Sanctum cigars present another flavor-packed edition from one of the world's best boutique cigar brands. Perfectly-aged long-fillers from Nicaragua, Honduras and Colombia meld with a Costa Rican binder for extra body, as a gorgeous Honduran Corojo wrapper completes the blend for a dense, creamy and balanced smoke with a seductive aroma. An earthy-woody base gives rise to layers of sweet spice, espresso and pepper for a complex, medium-bodied treat. Pick up a box or a 5-pack now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Sanctum Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+sun+grown+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Sun Grown Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Sungrown cigars are a fine addition to our ever-expanding repertoire of private labels. These affordably-priced cigars have a full-bodied...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Sun Grown Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Sungrown cigars are a fine addition to our ever-expanding repertoire of private labels. These affordably-priced cigars have a full-bodied blend of Nicaraguan Esteli &amp; Jalapa plus Colombian longfillers, Honduran binder and dark, mouthwatering Brazilian Mata Fina wrappers. In the Alec Bradley tradition, expect a creamy, complex smoke with plenty of depth and a savory aroma. Try a box today and taste why Alec Bradley Cigars have received some of the industry's highest rating scores.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Sun Grown Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+supervisor+selection+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Supervisor Selection Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Supervisor Selection premium cigars come by way of Alec Bradley Cigars. These dark, mysterious cigars are virtually identical to another fine...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Supervisor Selection Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Supervisor Selection premium cigars come by way of Alec Bradley Cigars. These dark, mysterious cigars are virtually identical to another fine Alec Bradley selection, but it's no mystery that the construction and flavor in these full-bodied bundle cigars is outstanding. A recipe of hearty tobaccos from numerous Central American countries make for a well-balanced smoke loaded with rich caramelized flavors and a sweet, head-turning aroma. Want a first-rate cigar at a cut-rate price? This is it!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Supervisor Selection Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+supervisor+selection+jalapa+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Supervisor Selection Jalapa Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Supervisor Selection Jalapa cigars bring you all of that outstanding, award-winning Alec Bradley cigar flavor in an affordably-priced bundle...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Supervisor Selection Jalapa Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Supervisor Selection Jalapa cigars bring you all of that outstanding, award-winning Alec Bradley cigar flavor in an affordably-priced bundle selection featuring a rich-tasting Nicaraguan Jalapa wrapper that's a tad lighter and sweeter in flavor, and a little more aromatic than the Supervisor Selection Habano. If you want a full-bodied, multi-layered smoke that will appease your palate at a price that will satisfy your wallet, order a bundle of these delicious cigars right now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Supervisor Selection Jalapa Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+tempus+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Tempus Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Tempus cigars (Latin for 'TIME,') offers you a choice of a rare, 7-year aged Honduran Criollo '98 Viso or an opulent Mexican San Andrés Maduro...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Tempus Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Tempus cigars (Latin for 'TIME,') offers you a choice of a rare, 7-year aged Honduran Criollo '98 Viso or an opulent Mexican San Andrés Maduro wrapper. A perfectly-balanced blend of Nicaraguan &amp; Honduran Criollo '98 &amp; Corojo '99 Ligero and Viso tobaccos make for a smooth, enticingly complex smoke brimming with robust tobacco flavors. Having received rave reviews from the top cigar magazines, Tempus is now a modern classic. Try a box or a 5-pack of these outstanding cigars now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Tempus Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+tempus+nicaragua+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Tempus Nicaragua Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Tempus Nicaragua cigars present a selection of outstanding puros that take their award-winning of Tempus line to a whole new dimension in...</t>
+  </si>
+  <si>
+    <t>Alec Bradley Tempus Nicaragua Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Tempus Nicaragua cigars present a selection of outstanding puros that take their award-winning of Tempus line to a whole new dimension in flavor. Tempus Nicaragua is handmade with premium Ligero &amp; Viso long-fillers from the fertile growing regions of Esteli, Condega, and Jalapa tobaccos in the same class as the 94 rated Tempus, rolled in a choice Jalapa wrapper. Sure to satisfy fans of the best Nicaraguan cigars, these rich, earthy premiums deserve a place in your humidor.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Tempus Nicaragua Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+texas+lancero+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Texas Lancero Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Texas Lancero cigars are a big-ash, big ring smoke with flavor to match. At 7x70, this delivers flavor for hours on end – order your box today!</t>
+  </si>
+  <si>
+    <t>Alec Bradley Texas Lancero Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Texas Lancero cigars are a tribute to the expression that “everything is bigger in Texas.” Coming in at a whopping seven inches long by a seventy ring gauge, this flavorful behemoth will surely appease those who love those big ring gauged beasts. Covered in a gorgeous Nicaraguan wrapper, the three-nation filler blend consists of Costa Rican, Nicaraguan and Honduran aged tobaccos. The flavor profile features notes of woodiness, coffee and nuts. Order now – and get ready to enjoy this big-boy for a good long time.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley Texas Lancero Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+the+lineage+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley The Lineage Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alec Bradley Lineage 1996 cigars are the 'next generation' of their bestselling Family Blend series. This line was made to commemorate company prez Alan...</t>
+  </si>
+  <si>
+    <t>Alec Bradley The Lineage Cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley Lineage 1996 cigars are the 'next generation' of their bestselling Family Blend series. This line was made to commemorate company prez Alan Rubin's sons, Alec &amp; Bradley, who became of legal smoking age in 2014. Made at Raíces Cubanas in Danli, Honduras, except for the Torpedo, the cigars all have pigtail caps, while the blend boasts a full-flavored Honduran-Nicaraguan recipe with a stunning Trojes wrapper. Lineage also features the company's first 70-ring cigar. Order yours NOW.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley The Lineage Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/alec+bradley+the+maxx+cigars</t>
+  </si>
+  <si>
+    <t>Alec Bradley The MAXX Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Alex Bradley The Maxx cigars boast classy new bands and packaging, yet their high-scoring blend remains unchanged. (After all, if it ain't broke don't fix...</t>
+  </si>
+  <si>
+    <t>Alec Bradley The MAXX Cigars</t>
+  </si>
+  <si>
+    <t>Alex Bradley The Maxx cigars boast classy new bands and packaging, yet their high-scoring blend remains unchanged. (After all, if it ain't broke don't fix it, right?) All 5 vitolas are handcrafted with long-fillers from Honduras, Nicaragua, Colombia, and Mexico. A Costa Rican binder adds balance and a layer of complexity, while the Nicaraguan Habano wrapper completes this rich, medium-bodied, and affordably-priced offering. Perfect for lovers of wide-body cigars, try a box of THE MAXX today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Alec Bradley Brands » Alec Bradley The MAXX Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/altadis+accessories+and+samplers+cigars</t>
+  </si>
+  <si>
+    <t>Altadis Accessories And Cigar Samplers | Famous Smoke</t>
+  </si>
+  <si>
+    <t>If you have ever enjoyed a premium cigar, there's a good chance you've enjoyed a cigar handcrafted by Altadis U.S.A. Responsible for many of the world's...</t>
+  </si>
+  <si>
+    <t>Altadis Accessories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>If you have ever enjoyed a premium cigar, there's a good chance you've enjoyed a cigar handcrafted by Altadis U.S.A. Responsible for many of the world's most renowned brands including Montecristo, Romeo y Julieta, H. Upmann, and Trinidad, Altadis U.S.A. has been crafting great cigars since 1918. Across all their brands connoisseurs have come to enjoy the consistency and well-made construction that signify Altadis U.S.A. cigars and make their cigars some of the finest time-and-time again.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » Altadis Accessories And Cigar Samplers</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/ambos+mundos+cigars</t>
+  </si>
+  <si>
+    <t>Ambos Mundos Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Ambos Mundos cigars are made for Tatuaje brand owner Pete Johnson in Jaime Garcia's Esteli, Nicaragua factory. To meet demand for a value-priced cigar, the...</t>
+  </si>
+  <si>
+    <t>Ambos Mundos Cigars</t>
+  </si>
+  <si>
+    <t>Ambos Mundos cigars are made for Tatuaje brand owner Pete Johnson in Jaime Garcia's Esteli, Nicaragua factory. To meet demand for a value-priced cigar, the cigars contain Nicaraguan longfillers that didn't quite make the grade for Pete's Tatuaje line. Ambos Mundos means both worlds, which is exactly what you get: your choice of Ecuadorian Sumatra or Nicaraguan Habano wrappers. Both are medium-plus bodied, with the Sumatra offering a meaty, leathery smoke, and the Habano woody, spicy notes.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Tatuaje Brands » Ambos Mundos Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/tatuaje+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/ambrosia+cigars</t>
+  </si>
+  <si>
+    <t>Ambrosia Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Ambrosia cigars are the result of taking experimental blending to its most extreme dimension. Available in Cameroon, Connecticut and Sumatra wrappers...</t>
+  </si>
+  <si>
+    <t>Ambrosia Cigars</t>
+  </si>
+  <si>
+    <t>Ambrosia cigars are the result of taking experimental blending to its most extreme dimension. Available in Cameroon, Connecticut and Sumatra wrappers blended with select Honduran and Nicaraguan tobaccos, the key to Ambrosia's marvelous flavors and aroma comes from exotic native spices from South Asia and Europe. Made in limited quantity and appropriately referred to as 'Tobaccos Exxotica,' Ambrosia cigars are some of Drew Estate's finest and most aromatic cigars.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Drew Estate Brands » Ambrosia Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/drew+estate+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/american+legion+cigars</t>
+  </si>
+  <si>
+    <t>American Legion Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>American Legion cigars offer you a smooth, satisfying smoke brimming with rich, creamy flavors from end-to-end, thanks to its diverse Nicaraguan core and...</t>
+  </si>
+  <si>
+    <t>American Legion Cigars</t>
+  </si>
+  <si>
+    <t>American Legion cigars offer you a smooth, satisfying smoke brimming with rich, creamy flavors from end-to-end, thanks to its diverse Nicaraguan core and flawless Habano Rosado wrapper. A portion of the proceeds from the sales of these cigars goes towards supporting American Legions and their members nationwide. Made in 3 sizes, order yours now and discover a truly outstanding medium-bodied cigar, while getting the satisfaction of helping those who have given so much to keep our nation free.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » American Legion Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/amilcar+perez+castro+cigars</t>
+  </si>
+  <si>
+    <t>Amilcar Perez Castro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Amilcar Perez Castro cigars (APC) come by way of the man behind some of Rocky Patel's best cigars. Now you can enjoy these full-flavored cigars created by,...</t>
+  </si>
+  <si>
+    <t>Amilcar Perez Castro Cigars</t>
+  </si>
+  <si>
+    <t>Amilcar Perez Castro cigars (APC) come by way of the man behind some of Rocky Patel's best cigars. Now you can enjoy these full-flavored cigars created by, as Rocky calls him, The Master, in an affordably-priced, 3-shape edition handcrafted with Nicaraguan &amp; Honduran longfillers and binders rolled in toothy, U.S. Pennsylvania-grown Maduro wrappers. The smoke is ultra-creamy with a base of earthy, woody and spicy flavors on a long, semi-sweet finish. Try a box of these scrumptious cigars now.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Rocky Patel Brands » Amilcar Perez Castro Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/rocky+patel+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/amos+de+santiago+corojo+cigars</t>
+  </si>
+  <si>
+    <t>Amos De Santiago Corojo Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Amos de Santiago Corojo cigars at Famous Smoke Shop. These premium boutique cigars are made with the finest Dominican tobaccos for a rich, rewarding smoke.</t>
+  </si>
+  <si>
+    <t>Amos De Santiago Corojo Cigars</t>
+  </si>
+  <si>
+    <t>Amos de Santiago Corojo cigars come from the talented hands of Consuelo Gomez, the daughter of a tobacco growing family in Santiago, DR. Her skills are clearly shown in this blend of choice Dominican longfiller tobaccos deftly rolled in an attractive and savory Corojo wrapper. The smoke is rich, creamy, and medium-bodied with flavors of sweet wood, leather, and spice in the mix. Reasonably-priced for premium boutique cigars of this quality, Amos de Santiago is one of the rising stars to watch.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » Amos De Santiago Corojo Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/anoranzas+cigars</t>
+  </si>
+  <si>
+    <t>Anoranzas Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Anoranzas cigars are Nicaraguan puros with a classic Cuban cigar appearance and flavor profile. These boutique cigars are sold online at Famous Smoke Shop.</t>
+  </si>
+  <si>
+    <t>Anoranzas Cigars</t>
+  </si>
+  <si>
+    <t>Anoranzas cigars are a boutique cigar selection from Miami Cigar Co. Spanish for "nostalgia," Añoranzas cigars even look like the great Cuban cigars of old with their dark, oily Nicaraguan Habano Oscuro wrappers and semi-box pressed shape. Made at the My Father factory in Estelí, a Nicaraguan long-filler &amp; dual binder core melds with the Nicaraguan Habano Oscuro wrapper for an impressive, full-bodied smoke with a perfectly-balanced serving of earth, pepper, cocoa, citrus, and nut flavors.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All My Father Brands » Anoranzas Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/my+father+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/antonio+y+cleopatra+cigars</t>
+  </si>
+  <si>
+    <t>Antonio y Cleopatra Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>The highly popular Antonio y Cleopatra cigars brand dates back to 1879. Today, these low-cost cigars, (also made in flavored 'Wise Guys' selections), offer...</t>
+  </si>
+  <si>
+    <t>Antonio y Cleopatra Cigars</t>
+  </si>
+  <si>
+    <t>The highly popular Antonio y Cleopatra cigars brand dates back to 1879. Today, these low-cost cigars, (also made in flavored 'Wise Guys' selections), offer a mild and satisfying flavor rolled in your choice of Connecticut Shade natural, Broadleaf Maduro, and Indonesian wrappers. Machine-made in Cayey, Puerto Rico, the filler tobaccos are all Cuban-seed with a sheet binder. Sold at discount store cigar prices daily, you'll be as smitten by these cigars as Tony &amp; Cleo were to each other.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » Antonio y Cleopatra Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/arandoza+cigars</t>
+  </si>
+  <si>
+    <t>Arandoza Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Arandoza cigars on sale at Famous Smoke Shop. Affordable, high-quality Nicaraguan boutique cigars offered in 3 lines: Blue Label, Red Label, and White Label.</t>
+  </si>
+  <si>
+    <t>Arandoza Cigars</t>
+  </si>
+  <si>
+    <t>Arandoza Cigars are a boutique cigar brand founded in 2011 by Robert Arango. The cigars are produced at the La Zona cigar factory in Estelí, Nicaragua, which is owned and operated by Erik Espinosa, known for his Espinosa Habano, 601, and Laranja cigars, to name but a few.
+In a story about Arango Cigars, cigarweekly.com wrote: "Arango is driven by a passion to do things well and make really good cigars. He's intense in a good way…The idea of [smoking] bans, and the seemingly hypocritical divide between cigarette smokers and cigar smokers, cigarette-friendly establishments being hostile to cigars, animates him and drives him, urging him to succeed all the more."
+All Arandoza cigars start with 15 test blends. As the test "ligas" are eliminated, they are narrowed down to a final three, from which only one is finally decided on to produce and market. The Blue and White offerings are made with all Nicaraguan tobacco blends, while the Red offers a rich-tasting San Andrés maduro wrapper from Mexico.
+Cigar smokers who are drawn to Nicaraguan cigars, and artisan cigar blends in particular, will discover that Arandoza are not only among the best boutique cigars in terms of flavor, but some of the most affordable Nicaraguan cigars, too.
+Arandoza Blue Label
+Arandoza Blue Label cigars were the first release from Robert Arango. Made at the La Zona factory in Nicaragua, he used a diverse Nicaraguan long-filler and binder recipe finished in a plush Nicaraguan Habano wrapper leaf. The medium-bodied smoke enters with a shot of pepper, then rounds-out to a more earthy-nutty character joined by flavors of sweet spice and citrusy notes for an impressively complex journey.
+Arandoza Red Label
+Arandoza Red Label cigars feature a diverse Nicaraguan tobacco core blend rolled in dark Mexican San Andrés maduro wrappers. The Red Label selection is also the heartiest in terms of strength, offering a creamy-smooth mix of earthy Nicaraguan spice, sweet tobacco, and a note of hickory. A smart, reasonably-priced choice for fans of the best full-bodied cigars.
+Arandoza White Label
+Arandoza White Label cigars are similar to their Blue Label brothers in terms of their all-Nicaraguan tobacco blend, but they differ greatly in strength. The White has a more medium-full character that offers excellent balance, complex flavors and an engaging aroma. A spicy start pulls notes of cream and nuts along with it, eventually moving to a more robust smoke in which the spicy-nutty flavors escalate while maintaining its inherent creaminess.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » Arandoza Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arandoza+blue+label+cigars</t>
+  </si>
+  <si>
+    <t>Arandoza Blue Label Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Arandoza Blue Label cigars are an affordably-priced selection from the Arandoza Family, who, through hard work and dedication, plus their knowledge and...</t>
+  </si>
+  <si>
+    <t>Arandoza Blue Label Cigars</t>
+  </si>
+  <si>
+    <t>Arandoza Blue Label cigars are an affordably-priced selection from the Arandoza Family, who, through hard work and dedication, plus their knowledge and passion for tobacco create premium class cigars that honor the cigar trade's great tradition and history. These puros, made at the La Zona factory in Estelí, use a medium blend of choice Nicaraguan long-fillers &amp; binders deftly rolled in Nicaraguan Habano wrappers for a bold, yet balanced taste with a silky-smooth finish. Try some today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Arandoza Brands » Arandoza Blue Label Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/arandoza+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arandoza+red+label+cigars</t>
+  </si>
+  <si>
+    <t>Arandoza Red Label Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Arandoza Red Label cigars are the latest blend to join this premium cigar family. Made at Erik Espinosa's La Zona factory in Estelí, they boast a diverse,...</t>
+  </si>
+  <si>
+    <t>Arandoza Red Label Cigars</t>
+  </si>
+  <si>
+    <t>Arandoza Red Label cigars are the latest blend to join this premium cigar family. Made at Erik Espinosa's La Zona factory in Estelí, they boast a diverse, all-Nicaraguan core seamlessly rolled in rich-tasting Mexican San Andres maduro wrappers, and are the most full-bodied cigars among all 3 affordably-priced Arandoza lines. Their effortless draw and perfect balance reveal notes of earth, hickory, spices, and pepper on a creamy-smooth finish. If you love deep, dark flavor, try some today!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Arandoza Brands » Arandoza Red Label Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arandoza+white+label+cigars</t>
+  </si>
+  <si>
+    <t>Arandoza White Label Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Arandoza White Label cigars serve-up a well-balanced, medium-full puro handcrafted in Estelí, Nicaragua at Erik Espinosa's La Zona factory. Using fillers &amp;...</t>
+  </si>
+  <si>
+    <t>Arandoza White Label Cigars</t>
+  </si>
+  <si>
+    <t>Arandoza White Label cigars serve-up a well-balanced, medium-full puro handcrafted in Estelí, Nicaragua at Erik Espinosa's La Zona factory. Using fillers &amp; binders from Nicaragua, the blend is sealed in a spicy dark Habano wrapper, offering excellent balance, complex flavors and a fragrant aroma you won't forget. Their affordable-prices make them accessible to cigar smokers at every level. Try some today and discover the unique character and flavor you'll find only in Arandoza Cigars.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Arandoza Brands » Arandoza White Label Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/artisan+honduran+cigars</t>
+  </si>
+  <si>
+    <t>Artisan Honduran Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Artisan Honduran cigars are handmade in Honduras by the Plasencia family, legendary tobacco farmers and cigar makers in their own rite. Three blends are...</t>
+  </si>
+  <si>
+    <t>Artisan Honduran Cigars</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Artisans Brands » Artisan Honduran Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/artisans+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/artisan+nicaraguan+1+cigars</t>
+  </si>
+  <si>
+    <t>Artisan Nicaraguan Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Artisan Nicaraguan cigars are handmade by the gifted rollers at Tabacalera San Rafael. The cigars contain select Nicaraguan longfillers rolled in your...</t>
+  </si>
+  <si>
+    <t>Artisan Nicaraguan Cigars</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Artisans Brands » Artisan Nicaraguan Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/artisans+cigars</t>
+  </si>
+  <si>
+    <t>Artisans Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Find Artisan Honduran and Nicaraguan cigars, plus many more of the best boutique cigars online at discount prices from Famous Smoke Shop. Guaranteed fresh.</t>
+  </si>
+  <si>
+    <t>Artisans Cigars</t>
+  </si>
+  <si>
+    <t>Artisan cigars are made exclusively for Famous Smoke Shop by the Plasencia family, one of the biggest suppliers of high-quality tobaccos in the cigar business. Their experience dates back five generations to their roots in Pinar del Rio, Cuba where they worked on the famed "El Corojo" farm, the tobacco source for most of the world's best Cuban cigars. After the Revolution of 1959, the Castro regime nationalized the farmlands, forcing the Plasencias and many other tobacco growing families to flee, taking their seeds, skills, and expert knowledge with them to countries like Honduras and Nicaragua. Today, under the direction of Nestor Plasencia and his son, Nestor Andrés, they've become legendary.
+Artisan cigars may represent a mere fraction of the millions of cigars made by Plasencia, yet, despite their incredibly low price, they come with the same fine craftsmanship Plasencia applies to all of their cigars. Presented in two selections, Artisan Honduran and Artisan Nicaraguan, cigar enthusiasts can now enjoy a well-made, rich-tasting smoke that's affordable enough to smoke daily. So, if you're a bargain hunter, you just may have found the ideal cigar.
+Artisan Honduran cigars feature a natural Nicaraguan Habano wrapper that surrounds a well-balanced blend of Nicaraguan, Honduran, and Mexican long-filler tobaccos. You can expect a rich-tasting, medium-bodied smoke with a well-balanced and complex character usually found in much more expensive cigars. In addition to the inherent earthiness found in Nicaraguan tobacco, depending on your palate, you may also discover flavors of oak, sweet spice, and some toasty-nutty flavors.
+Artisan Nicaraguan cigars are puros, or cigars all made with tobaccos from the same country. For this blend, Plasencia uses choice Nicaraguan long filler tobaccos neatly rolled in a Nicaraguan Habano natural wrapper. Also medium-bodied, this well-balanced cigar offers rich Nicaraguan earth and spice flavors laced with notes of wood, some subtle sweetness, and a pinch of peppery spice.
+When it comes to REAL value, these Artisan cigars are a wallet-friendly best bet. Try some today and taste for yourself. You may find yourself reordering them more often than you thought.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » Artisans Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brandgroup/arturo+fuente+cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Looking for the best prices on Arturo Fuente cigars? Renowned for their impeccable quality, flavor, and aroma, start saving on Arturo Fuente cigars today!</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Cigars have become renowned for the quality and consistency they offer cigar smokers worldwide. Fuente considers themselves to be the pride of the Dominican Cigars using mainly Dominican tobacco in all of their blends. Highly popular Arturo Fuente lines include the Chateau Fuente, Hemingway Cigars, Flor Fina 858, Don Carlos cigars, the King and Queen B, and the most lauded cigar in their history, the all Domincan grown Fuente Fuente Opus X.
+At the forefront of it all is the father and son team of Carlos and Carlito Fuente. The two tobacco men are seen together in all company marketing vehicles, displaying their unbridled passion for cigar making. Carlos’s crowning achievement is the creation of the Opus X, a full bodied Dominican puro that he claims was his way of proving to the world that a full flavored, powerful, all-Domincan cigar could be made.
+The legendary Arturo Fuente family history is one that might be easier to make into a film than to summarize in a series of paragraphs. Their story begins in 1887 Cuba, the year Arturo Fuente was born. From the time he was a child, his father taught him how to cultivate prime tobacco and make handmade cigars. Overcoming several setbacks over the years, the company continues to thrive, and today Arturo Fuente cigars are made in the Dominican Republic.
+Some people might presume that the Fuente family was part of the post Cuban Revolution exile, but the family left Cuba in 1906. Resettling in Key West, Florida, Arturo found work as a cigar roller, and eventually the family moved to Ybor City in Tampa (at the time, the cigar capital of the world.) Then in 1912, as his reputation for making excellent cigars grew, the first cigars to bear the Fuente family name were produced. Until 1961 when the U.S. embargo went into effect, the cigars were made with imported Cuban tobacco. There was a six year period from 1924-1930 when damage from a fire destroyed the factory, but success continued then as it does today.
+Almost as legendary as his father was Arturo's son, Carlos. Like his father, Carlos was born into the cigar business and learned every aspect of the trade. Years later, Don Arturo passed the business on to Carlos and when Carlos Fuente, Jr., was born, just like his father and grandfather, Carlos Jr. (a.k.a. "Carlito") learned the business. Since the 1990's cigar boom, Carlos Fuente, Jr. has been "the face" of Arturo Fuente cigars.
+In 1980, production moved to the Dominican Republic, where began growing their own tobaccos at the family's private estate plantation, Chateau de la Fuente. It's there that Carlos and Carlito developed the company's most famous cigars, the Fuente Fuente OpusX selection. "OpusX" cigars were the first Arturo Fuente cigars to be made with an all-Dominican filler, binder and wrapper, and though it took years to develop this extraordinary leaf, until the Fuentes arrived, other cigar makers had no success growing quality wrapper leaf in the Dominican Republic. The Fuente Opus X proved that it could be done.
+"We are a family business," said Carlos Fuente, Jr. "Our factories and our plantations comprise our family 'kitchen.' By staying in the kitchen, we're able to consistently produce outstanding tobacco leaves and rich flavored, perfectly balanced cigars that please cigar aficionados every time, everywhere. And because tobacco is in our blood, that is all my family and I ever aspired to achieve."
+Whether it’s the in your face power of the Opus X cigar, the rich smoothness of the Hemingways cigars, or the always tasty Chateau Fuente, Famous Smoke Shop carries the full line up of A Fuente cigars, and as always, our legendary service and super low prices cannot be beat!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Cigars » Cigar Brand List » Arturo Fuente Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arturo+fuente+1+cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Brand Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Though they aren't always readily available, Arturo Fuente cigars sell fast when they're in stock. With patience and painstaking handcraftsmanship, the...</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Brand Cigars</t>
+  </si>
+  <si>
+    <t>Though they aren't always readily available, Arturo Fuente cigars sell fast when they're in stock. With patience and painstaking handcraftsmanship, the famed Fuente family has been producing affordably-priced cigars with outstanding quality for generations. Blended with tobaccos grown exclusively on the family's estate farms in the Dominican Republic, expect a cigar that's always rich in taste, well-balanced, and satisfying. If you haven't yet had the pleasure of these cigars, do so now!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Arturo Fuente Brands » Arturo Fuente Brand Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/,https://www.famous-smoke.com/cigars,https://www.famous-smoke.com/cigar-brand-list,https://www.famous-smoke.com/brandgroup/arturo+fuente+cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arturo+fuente+anejo+cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Anejo Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>A. Fuente Añejo cigars are made with the same filler and binder as the OpusX cigars and are just about as hard to find, too, except they're wrapped in a...</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Anejo Cigars</t>
+  </si>
+  <si>
+    <t>A. Fuente Añejo cigars are made with the same filler and binder as the OpusX cigars and are just about as hard to find, too, except they're wrapped in a dark, oily U.S. Connecticut broadleaf Maduro leaf that's aged for one full year in oak cognac barrels. The result is a smooth-smoking, full-bodied cigar with a unique, complex flavor and sweetness that only the hands of Arturo Fuente could create. Called 'the Maduro OpusX,' if you're lucky enough to find them in stock, grab them, and FAST!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Arturo Fuente Brands » Arturo Fuente Anejo Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arturo+fuente+don+carlos+cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Don Carlos Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Don Carlos Fuente Sr. spent years deciding which rare, vintage tobaccos would go into Don Carlos cigars, considered by many aficionados to be the finest of...</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Don Carlos Cigars</t>
+  </si>
+  <si>
+    <t>Don Carlos Fuente Sr. spent years deciding which rare, vintage tobaccos would go into Don Carlos cigars, considered by many aficionados to be the finest of all Arturo Fuente cigars, including Fuente Fuente OpusX! The Don Carlos is rich, spicy, full-bodied, and wrapped in the most aromatic, specially-selected Cameroon wrappers. To be sure, these luxurious cigars offer the ultimate in construction, consistency and flavor, and deserve a place of honor in any cigar smoker's humidor.</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Arturo Fuente Brands » Arturo Fuente Don Carlos Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arturo+fuente+hemingway+cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Hemingway Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Hemingway cigars are made with an exquisite, mild to medium blend of vintage Dominican filler tobaccos and very delicate African Cameroon...</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Hemingway Cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Hemingway cigars are made with an exquisite, mild to medium blend of vintage Dominican filler tobaccos and very delicate African Cameroon wrappers (or Maduro, if you can find them). The Fuente family have been making some of the free world's best cigars for generations, and these are right up there with Opus X and Añejo Reserva. If you truly desire getting your hands on a box, we suggest checking the box indicating favorite, and checking your e-mail often. They're THAT good!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Arturo Fuente Brands » Arturo Fuente Hemingway Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arturo+fuente+new+baby+cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente New Baby Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Arturo Fuente New Baby cigars offer the signature flavor they are known for to help you celebrate your newborn! Get your Arturo Fuente New Baby Cigars on sale.</t>
+  </si>
+  <si>
+    <t>Arturo Fuente New Baby Cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente New Baby cigars are perfect to celebrate the birth of a little bundle of joy. There’s nothing more special than welcoming a newborn into the world, and if you’re a proud papa or grandpa, than this is the best way to spread your joy to the world. You and whomever you share one of these cigars with will rejoice with each puff, and be met with the famous flavor that has propelled Arturo Fuente to the top spot in cigar legendry! Pick up your box today, and start celebrating!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All It's A Boy. It's A Girl. Brands » Arturo Fuente New Baby Cigars</t>
+  </si>
+  <si>
+    <t>https://www.famous-smoke.com/brand/arturo+fuente+seleccion+doro+cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Seleccion D'Oro Cigars | Famous Smoke</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Seleccion D'Oro cigars use the highest quality, vintage Dominican tobaccos and patient hand workmanship to wrap them in the most select,...</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Seleccion D'Oro Cigars</t>
+  </si>
+  <si>
+    <t>Arturo Fuente Seleccion D'Oro cigars use the highest quality, vintage Dominican tobaccos and patient hand workmanship to wrap them in the most select, golden, Ecuadorian-grown Connecticut wrappers for a smoother and more flavorful cigar. A must-try if you like the Arturo Fuente Chateau Fuente cigars or just have an irrepressible craving for Arturo Fuente cigars, period!</t>
+  </si>
+  <si>
+    <t>» Famous Smoke Shop Cigars » Discount Cigars Online » Cigar Brand List » All Arturo Fuente Brands » Arturo Fuente Seleccion D'Oro Cigars</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +2056,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="91">
+  <fills count="92">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1577,8 +2509,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="354">
+  <borders count="358">
     <border>
       <left/>
       <right/>
@@ -3185,11 +4122,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="597">
+  <cellXfs count="698">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4977,6 +5932,309 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="353" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="91" borderId="357" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -5301,130 +6559,2943 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.08984375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="85.92578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="85.92578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="62.68359375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="146.671875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="47.15625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="136.05078125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="188.4921875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="10.87109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="593" t="s">
+      <c r="A1" s="597" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="593" t="s">
+      <c r="B1" s="597" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="593" t="s">
+      <c r="C1" s="597" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="593" t="s">
+      <c r="D1" s="597" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="593" t="s">
+      <c r="E1" s="597" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="593" t="s">
+      <c r="F1" s="597" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="593" t="s">
+      <c r="G1" s="597" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="593" t="s">
+      <c r="H1" s="597" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="593" t="s">
+      <c r="I1" s="597" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="594" t="s">
+      <c r="A2" s="598" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="594" t="s">
+      <c r="B2" s="598" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="594" t="s">
+      <c r="C2" s="598" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="594" t="s">
+      <c r="D2" s="598" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="594" t="s">
+      <c r="E2" s="598" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="594" t="s">
+      <c r="F2" s="598" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="594" t="s">
+      <c r="G2" s="598" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="594" t="s">
+      <c r="H2" s="598" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="594" t="s">
+      <c r="I2" s="598" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="595" t="s">
+      <c r="A3" s="599" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="595" t="s">
+      <c r="B3" s="599" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="595" t="s">
+      <c r="C3" s="599" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="595" t="s">
+      <c r="D3" s="599" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="595" t="s">
+      <c r="E3" s="599" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="595" t="s">
+      <c r="F3" s="599" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="595" t="s">
+      <c r="G3" s="599" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="595" t="s">
+      <c r="H3" s="599" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="595" t="s">
+      <c r="I3" s="599" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="596" t="s">
+      <c r="A4" s="600" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="596" t="s">
+      <c r="B4" s="600" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="596" t="s">
+      <c r="C4" s="600" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="596" t="s">
+      <c r="D4" s="600" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="596" t="s">
+      <c r="E4" s="600" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="596" t="s">
+      <c r="F4" s="600" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="596" t="s">
+      <c r="G4" s="600" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="596" t="s">
+      <c r="H4" s="600" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="596" t="s">
+      <c r="I4" s="600" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="601" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="601" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="601" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="601" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="601" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="601" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="601" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="601" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="601" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="602" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="602" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="602" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="602" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="602" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="602" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="602" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="602" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="602" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="603" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="603" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="603" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="603" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="603" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="603" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="603" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="603" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="603" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="604" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="604" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="604" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="604" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="604" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="604" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="604" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="604" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="604" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="605" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="605" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="605" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="605" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="605" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="605" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="605" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="605" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="605" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="606" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="606" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="606" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="606" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="606" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="606" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="606" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="606" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="606" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="607" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="607" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="607" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="607" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="607" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="607" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="607" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="607" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="607" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="608" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="608" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="608" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="608" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="608" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="608" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="608" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="608" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="608" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="609" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="609" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="609" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="609" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="609" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="609" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="609" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="609" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="609" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="610" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="610" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="610" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="610" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="610" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="610" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="610" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="610" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="610" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="611" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="611" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="611" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="611" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="611" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="611" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="611" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="611" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="611" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="612" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="612" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="612" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="612" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="612" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="612" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="612" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" s="612" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="612" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="613" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="613" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="613" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="613" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="613" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="613" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="613" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" s="613" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" s="613" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="614" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="614" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="614" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="614" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="614" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="614" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="614" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" s="614" t="s">
+        <v>115</v>
+      </c>
+      <c r="I18" s="614" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="615" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="615" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="615" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="615" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="615" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="615" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" s="615" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="615" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" s="615" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="616" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="616" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="616" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="616" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="616" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="616" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="616" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="616" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" s="616" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="617" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="617" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="617" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="617" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="617" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="617" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="617" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="617" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="617" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="618" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" s="618" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="618" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="618" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="618" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="618" t="s">
+        <v>158</v>
+      </c>
+      <c r="G22" s="618" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" s="618" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" s="618" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="619" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="619" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="619" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="619" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" s="619" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" s="619" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" s="619" t="s">
+        <v>165</v>
+      </c>
+      <c r="H23" s="619" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="619" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="620" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="620" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="620" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" s="620" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" s="620" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24" s="620" t="s">
+        <v>170</v>
+      </c>
+      <c r="G24" s="620" t="s">
+        <v>171</v>
+      </c>
+      <c r="H24" s="620" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24" s="620" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="621" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25" s="621" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="621" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="621" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" s="621" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" s="621" t="s">
+        <v>177</v>
+      </c>
+      <c r="G25" s="621" t="s">
+        <v>178</v>
+      </c>
+      <c r="H25" s="621" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" s="621" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="622" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="622" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="622" t="s">
+        <v>180</v>
+      </c>
+      <c r="D26" s="622" t="s">
+        <v>181</v>
+      </c>
+      <c r="E26" s="622" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26" s="622" t="s">
+        <v>183</v>
+      </c>
+      <c r="G26" s="622" t="s">
+        <v>184</v>
+      </c>
+      <c r="H26" s="622" t="s">
+        <v>185</v>
+      </c>
+      <c r="I26" s="622" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="623" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="623" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="623" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="623" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="623" t="s">
+        <v>189</v>
+      </c>
+      <c r="F27" s="623" t="s">
+        <v>190</v>
+      </c>
+      <c r="G27" s="623" t="s">
+        <v>191</v>
+      </c>
+      <c r="H27" s="623" t="s">
+        <v>185</v>
+      </c>
+      <c r="I27" s="623" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="624" t="s">
+        <v>192</v>
+      </c>
+      <c r="B28" s="624" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" s="624" t="s">
+        <v>193</v>
+      </c>
+      <c r="D28" s="624" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="624" t="s">
+        <v>195</v>
+      </c>
+      <c r="F28" s="624" t="s">
+        <v>196</v>
+      </c>
+      <c r="G28" s="624" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" s="624" t="s">
+        <v>185</v>
+      </c>
+      <c r="I28" s="624" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="625" t="s">
+        <v>198</v>
+      </c>
+      <c r="B29" s="625" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="625" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" s="625" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="625" t="s">
+        <v>201</v>
+      </c>
+      <c r="F29" s="625" t="s">
+        <v>202</v>
+      </c>
+      <c r="G29" s="625" t="s">
+        <v>203</v>
+      </c>
+      <c r="H29" s="625" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="625" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="626" t="s">
+        <v>204</v>
+      </c>
+      <c r="B30" s="626" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" s="626" t="s">
+        <v>205</v>
+      </c>
+      <c r="D30" s="626" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="626" t="s">
+        <v>207</v>
+      </c>
+      <c r="F30" s="626" t="s">
+        <v>208</v>
+      </c>
+      <c r="G30" s="626" t="s">
+        <v>209</v>
+      </c>
+      <c r="H30" s="626" t="s">
+        <v>210</v>
+      </c>
+      <c r="I30" s="626" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="627" t="s">
+        <v>211</v>
+      </c>
+      <c r="B31" s="627" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" s="627" t="s">
+        <v>212</v>
+      </c>
+      <c r="D31" s="627" t="s">
+        <v>213</v>
+      </c>
+      <c r="E31" s="627" t="s">
+        <v>214</v>
+      </c>
+      <c r="F31" s="627" t="s">
+        <v>215</v>
+      </c>
+      <c r="G31" s="627" t="s">
+        <v>216</v>
+      </c>
+      <c r="H31" s="627" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="627" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="628" t="s">
+        <v>217</v>
+      </c>
+      <c r="B32" s="628" t="s">
+        <v>217</v>
+      </c>
+      <c r="C32" s="628" t="s">
+        <v>218</v>
+      </c>
+      <c r="D32" s="628" t="s">
+        <v>219</v>
+      </c>
+      <c r="E32" s="628" t="s">
+        <v>220</v>
+      </c>
+      <c r="F32" s="628" t="s">
+        <v>221</v>
+      </c>
+      <c r="G32" s="628" t="s">
+        <v>222</v>
+      </c>
+      <c r="H32" s="628" t="s">
+        <v>223</v>
+      </c>
+      <c r="I32" s="628" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="629" t="s">
+        <v>224</v>
+      </c>
+      <c r="B33" s="629" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" s="629" t="s">
+        <v>225</v>
+      </c>
+      <c r="D33" s="629" t="s">
+        <v>226</v>
+      </c>
+      <c r="E33" s="629" t="s">
+        <v>227</v>
+      </c>
+      <c r="F33" s="629" t="s">
+        <v>228</v>
+      </c>
+      <c r="G33" s="629" t="s">
+        <v>229</v>
+      </c>
+      <c r="H33" s="629" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="629" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="630" t="s">
+        <v>230</v>
+      </c>
+      <c r="B34" s="630" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="630" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="630" t="s">
+        <v>232</v>
+      </c>
+      <c r="E34" s="630" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" s="630" t="s">
+        <v>234</v>
+      </c>
+      <c r="G34" s="630" t="s">
+        <v>235</v>
+      </c>
+      <c r="H34" s="630" t="s">
+        <v>236</v>
+      </c>
+      <c r="I34" s="630" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="631" t="s">
+        <v>237</v>
+      </c>
+      <c r="B35" s="631" t="s">
+        <v>237</v>
+      </c>
+      <c r="C35" s="631" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" s="631" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" s="631" t="s">
+        <v>240</v>
+      </c>
+      <c r="F35" s="631" t="s">
+        <v>241</v>
+      </c>
+      <c r="G35" s="631" t="s">
+        <v>242</v>
+      </c>
+      <c r="H35" s="631" t="s">
+        <v>236</v>
+      </c>
+      <c r="I35" s="631" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="632" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="632" t="s">
+        <v>243</v>
+      </c>
+      <c r="C36" s="632" t="s">
+        <v>244</v>
+      </c>
+      <c r="D36" s="632" t="s">
+        <v>245</v>
+      </c>
+      <c r="E36" s="632" t="s">
+        <v>246</v>
+      </c>
+      <c r="F36" s="632" t="s">
+        <v>247</v>
+      </c>
+      <c r="G36" s="632" t="s">
+        <v>248</v>
+      </c>
+      <c r="H36" s="632" t="s">
+        <v>236</v>
+      </c>
+      <c r="I36" s="632" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="633" t="s">
+        <v>249</v>
+      </c>
+      <c r="B37" s="633" t="s">
+        <v>249</v>
+      </c>
+      <c r="C37" s="633" t="s">
+        <v>250</v>
+      </c>
+      <c r="D37" s="633" t="s">
+        <v>251</v>
+      </c>
+      <c r="E37" s="633" t="s">
+        <v>252</v>
+      </c>
+      <c r="F37" s="633" t="s">
+        <v>253</v>
+      </c>
+      <c r="G37" s="633" t="s">
+        <v>254</v>
+      </c>
+      <c r="H37" s="633" t="s">
+        <v>236</v>
+      </c>
+      <c r="I37" s="633" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="634" t="s">
+        <v>255</v>
+      </c>
+      <c r="B38" s="634" t="s">
+        <v>255</v>
+      </c>
+      <c r="C38" s="634" t="s">
+        <v>256</v>
+      </c>
+      <c r="D38" s="634" t="s">
+        <v>257</v>
+      </c>
+      <c r="E38" s="634" t="s">
+        <v>258</v>
+      </c>
+      <c r="F38" s="634" t="s">
+        <v>259</v>
+      </c>
+      <c r="G38" s="634" t="s">
+        <v>260</v>
+      </c>
+      <c r="H38" s="634" t="s">
+        <v>261</v>
+      </c>
+      <c r="I38" s="634" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="635" t="s">
+        <v>262</v>
+      </c>
+      <c r="B39" s="635" t="s">
+        <v>262</v>
+      </c>
+      <c r="C39" s="635" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" s="635" t="s">
+        <v>264</v>
+      </c>
+      <c r="E39" s="635" t="s">
+        <v>265</v>
+      </c>
+      <c r="F39" s="635" t="s">
+        <v>266</v>
+      </c>
+      <c r="G39" s="635" t="s">
+        <v>267</v>
+      </c>
+      <c r="H39" s="635" t="s">
+        <v>210</v>
+      </c>
+      <c r="I39" s="635" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="636" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" s="636" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" s="636" t="s">
+        <v>269</v>
+      </c>
+      <c r="D40" s="636" t="s">
+        <v>270</v>
+      </c>
+      <c r="E40" s="636" t="s">
+        <v>271</v>
+      </c>
+      <c r="F40" s="636" t="s">
+        <v>272</v>
+      </c>
+      <c r="G40" s="636" t="s">
+        <v>273</v>
+      </c>
+      <c r="H40" s="636" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="636" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="637" t="s">
+        <v>274</v>
+      </c>
+      <c r="B41" s="637" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" s="637" t="s">
+        <v>275</v>
+      </c>
+      <c r="D41" s="637" t="s">
+        <v>276</v>
+      </c>
+      <c r="E41" s="637" t="s">
+        <v>277</v>
+      </c>
+      <c r="F41" s="637" t="s">
+        <v>278</v>
+      </c>
+      <c r="G41" s="637" t="s">
+        <v>279</v>
+      </c>
+      <c r="H41" s="637" t="s">
+        <v>280</v>
+      </c>
+      <c r="I41" s="637" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="638" t="s">
+        <v>281</v>
+      </c>
+      <c r="B42" s="638" t="s">
+        <v>281</v>
+      </c>
+      <c r="C42" s="638" t="s">
+        <v>282</v>
+      </c>
+      <c r="D42" s="638" t="s">
+        <v>283</v>
+      </c>
+      <c r="E42" s="638" t="s">
+        <v>284</v>
+      </c>
+      <c r="F42" s="638" t="s">
+        <v>285</v>
+      </c>
+      <c r="G42" s="638" t="s">
+        <v>286</v>
+      </c>
+      <c r="H42" s="638" t="s">
+        <v>280</v>
+      </c>
+      <c r="I42" s="638" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="639" t="s">
+        <v>287</v>
+      </c>
+      <c r="B43" s="639" t="s">
+        <v>287</v>
+      </c>
+      <c r="C43" s="639" t="s">
+        <v>288</v>
+      </c>
+      <c r="D43" s="639" t="s">
+        <v>289</v>
+      </c>
+      <c r="E43" s="639" t="s">
+        <v>290</v>
+      </c>
+      <c r="F43" s="639" t="s">
+        <v>291</v>
+      </c>
+      <c r="G43" s="639" t="s">
+        <v>292</v>
+      </c>
+      <c r="H43" s="639" t="s">
+        <v>280</v>
+      </c>
+      <c r="I43" s="639" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="640" t="s">
+        <v>293</v>
+      </c>
+      <c r="B44" s="640" t="s">
+        <v>293</v>
+      </c>
+      <c r="C44" s="640" t="s">
+        <v>294</v>
+      </c>
+      <c r="D44" s="640" t="s">
+        <v>295</v>
+      </c>
+      <c r="E44" s="640" t="s">
+        <v>296</v>
+      </c>
+      <c r="F44" s="640" t="s">
+        <v>297</v>
+      </c>
+      <c r="G44" s="640" t="s">
+        <v>298</v>
+      </c>
+      <c r="H44" s="640" t="s">
+        <v>280</v>
+      </c>
+      <c r="I44" s="640" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="641" t="s">
+        <v>299</v>
+      </c>
+      <c r="B45" s="641" t="s">
+        <v>299</v>
+      </c>
+      <c r="C45" s="641" t="s">
+        <v>300</v>
+      </c>
+      <c r="D45" s="641" t="s">
+        <v>301</v>
+      </c>
+      <c r="E45" s="641" t="s">
+        <v>302</v>
+      </c>
+      <c r="F45" s="641" t="s">
+        <v>303</v>
+      </c>
+      <c r="G45" s="641" t="s">
+        <v>304</v>
+      </c>
+      <c r="H45" s="641" t="s">
+        <v>280</v>
+      </c>
+      <c r="I45" s="641" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="642" t="s">
+        <v>305</v>
+      </c>
+      <c r="B46" s="642" t="s">
+        <v>305</v>
+      </c>
+      <c r="C46" s="642" t="s">
+        <v>306</v>
+      </c>
+      <c r="D46" s="642" t="s">
+        <v>307</v>
+      </c>
+      <c r="E46" s="642" t="s">
+        <v>308</v>
+      </c>
+      <c r="F46" s="642" t="s">
+        <v>309</v>
+      </c>
+      <c r="G46" s="642" t="s">
+        <v>310</v>
+      </c>
+      <c r="H46" s="642" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="642" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="643" t="s">
+        <v>311</v>
+      </c>
+      <c r="B47" s="643" t="s">
+        <v>311</v>
+      </c>
+      <c r="C47" s="643" t="s">
+        <v>312</v>
+      </c>
+      <c r="D47" s="643" t="s">
+        <v>313</v>
+      </c>
+      <c r="E47" s="643" t="s">
+        <v>314</v>
+      </c>
+      <c r="F47" s="643" t="s">
+        <v>315</v>
+      </c>
+      <c r="G47" s="643" t="s">
+        <v>316</v>
+      </c>
+      <c r="H47" s="643" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="643" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="644" t="s">
+        <v>317</v>
+      </c>
+      <c r="B48" s="644" t="s">
+        <v>317</v>
+      </c>
+      <c r="C48" s="644" t="s">
+        <v>318</v>
+      </c>
+      <c r="D48" s="644" t="s">
+        <v>319</v>
+      </c>
+      <c r="E48" s="644" t="s">
+        <v>320</v>
+      </c>
+      <c r="F48" s="644" t="s">
+        <v>321</v>
+      </c>
+      <c r="G48" s="644" t="s">
+        <v>322</v>
+      </c>
+      <c r="H48" s="644" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="644" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="645" t="s">
+        <v>323</v>
+      </c>
+      <c r="B49" s="645" t="s">
+        <v>323</v>
+      </c>
+      <c r="C49" s="645" t="s">
+        <v>324</v>
+      </c>
+      <c r="D49" s="645" t="s">
+        <v>325</v>
+      </c>
+      <c r="E49" s="645" t="s">
+        <v>326</v>
+      </c>
+      <c r="F49" s="645" t="s">
+        <v>327</v>
+      </c>
+      <c r="G49" s="645" t="s">
+        <v>328</v>
+      </c>
+      <c r="H49" s="645" t="s">
+        <v>329</v>
+      </c>
+      <c r="I49" s="645" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="646" t="s">
+        <v>330</v>
+      </c>
+      <c r="B50" s="646" t="s">
+        <v>330</v>
+      </c>
+      <c r="C50" s="646" t="s">
+        <v>331</v>
+      </c>
+      <c r="D50" s="646" t="s">
+        <v>332</v>
+      </c>
+      <c r="E50" s="646" t="s">
+        <v>333</v>
+      </c>
+      <c r="F50" s="646" t="s">
+        <v>334</v>
+      </c>
+      <c r="G50" s="646" t="s">
+        <v>335</v>
+      </c>
+      <c r="H50" s="646" t="s">
+        <v>329</v>
+      </c>
+      <c r="I50" s="646" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="647" t="s">
+        <v>336</v>
+      </c>
+      <c r="B51" s="647" t="s">
+        <v>336</v>
+      </c>
+      <c r="C51" s="647" t="s">
+        <v>337</v>
+      </c>
+      <c r="D51" s="647" t="s">
+        <v>338</v>
+      </c>
+      <c r="E51" s="647" t="s">
+        <v>339</v>
+      </c>
+      <c r="F51" s="647" t="s">
+        <v>340</v>
+      </c>
+      <c r="G51" s="647" t="s">
+        <v>341</v>
+      </c>
+      <c r="H51" s="647" t="s">
+        <v>329</v>
+      </c>
+      <c r="I51" s="647" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="648" t="s">
+        <v>342</v>
+      </c>
+      <c r="B52" s="648" t="s">
+        <v>342</v>
+      </c>
+      <c r="C52" s="648" t="s">
+        <v>343</v>
+      </c>
+      <c r="D52" s="648" t="s">
+        <v>344</v>
+      </c>
+      <c r="E52" s="648" t="s">
+        <v>345</v>
+      </c>
+      <c r="F52" s="648" t="s">
+        <v>346</v>
+      </c>
+      <c r="G52" s="648" t="s">
+        <v>347</v>
+      </c>
+      <c r="H52" s="648" t="s">
+        <v>329</v>
+      </c>
+      <c r="I52" s="648" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="649" t="s">
+        <v>348</v>
+      </c>
+      <c r="B53" s="649" t="s">
+        <v>348</v>
+      </c>
+      <c r="C53" s="649" t="s">
+        <v>349</v>
+      </c>
+      <c r="D53" s="649" t="s">
+        <v>350</v>
+      </c>
+      <c r="E53" s="649" t="s">
+        <v>351</v>
+      </c>
+      <c r="F53" s="649" t="s">
+        <v>352</v>
+      </c>
+      <c r="G53" s="649" t="s">
+        <v>353</v>
+      </c>
+      <c r="H53" s="649" t="s">
+        <v>329</v>
+      </c>
+      <c r="I53" s="649" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="650" t="s">
+        <v>354</v>
+      </c>
+      <c r="B54" s="650" t="s">
+        <v>354</v>
+      </c>
+      <c r="C54" s="650" t="s">
+        <v>355</v>
+      </c>
+      <c r="D54" s="650" t="s">
+        <v>356</v>
+      </c>
+      <c r="E54" s="650" t="s">
+        <v>357</v>
+      </c>
+      <c r="F54" s="650" t="s">
+        <v>358</v>
+      </c>
+      <c r="G54" s="650" t="s">
+        <v>359</v>
+      </c>
+      <c r="H54" s="650" t="s">
+        <v>329</v>
+      </c>
+      <c r="I54" s="650" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="651" t="s">
+        <v>360</v>
+      </c>
+      <c r="B55" s="651" t="s">
+        <v>360</v>
+      </c>
+      <c r="C55" s="651" t="s">
+        <v>361</v>
+      </c>
+      <c r="D55" s="651" t="s">
+        <v>362</v>
+      </c>
+      <c r="E55" s="651" t="s">
+        <v>363</v>
+      </c>
+      <c r="F55" s="651" t="s">
+        <v>364</v>
+      </c>
+      <c r="G55" s="651" t="s">
+        <v>365</v>
+      </c>
+      <c r="H55" s="651" t="s">
+        <v>329</v>
+      </c>
+      <c r="I55" s="651" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="652" t="s">
+        <v>366</v>
+      </c>
+      <c r="B56" s="652" t="s">
+        <v>366</v>
+      </c>
+      <c r="C56" s="652" t="s">
+        <v>367</v>
+      </c>
+      <c r="D56" s="652" t="s">
+        <v>368</v>
+      </c>
+      <c r="E56" s="652" t="s">
+        <v>369</v>
+      </c>
+      <c r="F56" s="652" t="s">
+        <v>370</v>
+      </c>
+      <c r="G56" s="652" t="s">
+        <v>371</v>
+      </c>
+      <c r="H56" s="652" t="s">
+        <v>329</v>
+      </c>
+      <c r="I56" s="652" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="653" t="s">
+        <v>372</v>
+      </c>
+      <c r="B57" s="653" t="s">
+        <v>372</v>
+      </c>
+      <c r="C57" s="653" t="s">
+        <v>373</v>
+      </c>
+      <c r="D57" s="653" t="s">
+        <v>374</v>
+      </c>
+      <c r="E57" s="653" t="s">
+        <v>375</v>
+      </c>
+      <c r="F57" s="653" t="s">
+        <v>376</v>
+      </c>
+      <c r="G57" s="653" t="s">
+        <v>377</v>
+      </c>
+      <c r="H57" s="653" t="s">
+        <v>329</v>
+      </c>
+      <c r="I57" s="653" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="654" t="s">
+        <v>378</v>
+      </c>
+      <c r="B58" s="654" t="s">
+        <v>378</v>
+      </c>
+      <c r="C58" s="654" t="s">
+        <v>379</v>
+      </c>
+      <c r="D58" s="654" t="s">
+        <v>380</v>
+      </c>
+      <c r="E58" s="654" t="s">
+        <v>381</v>
+      </c>
+      <c r="F58" s="654" t="s">
+        <v>382</v>
+      </c>
+      <c r="G58" s="654" t="s">
+        <v>383</v>
+      </c>
+      <c r="H58" s="654" t="s">
+        <v>329</v>
+      </c>
+      <c r="I58" s="654" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="655" t="s">
+        <v>384</v>
+      </c>
+      <c r="B59" s="655" t="s">
+        <v>384</v>
+      </c>
+      <c r="C59" s="655" t="s">
+        <v>385</v>
+      </c>
+      <c r="D59" s="655" t="s">
+        <v>386</v>
+      </c>
+      <c r="E59" s="655" t="s">
+        <v>387</v>
+      </c>
+      <c r="F59" s="655" t="s">
+        <v>388</v>
+      </c>
+      <c r="G59" s="655" t="s">
+        <v>389</v>
+      </c>
+      <c r="H59" s="655" t="s">
+        <v>329</v>
+      </c>
+      <c r="I59" s="655" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="656" t="s">
+        <v>390</v>
+      </c>
+      <c r="B60" s="656" t="s">
+        <v>390</v>
+      </c>
+      <c r="C60" s="656" t="s">
+        <v>391</v>
+      </c>
+      <c r="D60" s="656" t="s">
+        <v>392</v>
+      </c>
+      <c r="E60" s="656" t="s">
+        <v>393</v>
+      </c>
+      <c r="F60" s="656" t="s">
+        <v>394</v>
+      </c>
+      <c r="G60" s="656" t="s">
+        <v>395</v>
+      </c>
+      <c r="H60" s="656" t="s">
+        <v>329</v>
+      </c>
+      <c r="I60" s="656" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="657" t="s">
+        <v>396</v>
+      </c>
+      <c r="B61" s="657" t="s">
+        <v>396</v>
+      </c>
+      <c r="C61" s="657" t="s">
+        <v>397</v>
+      </c>
+      <c r="D61" s="657" t="s">
+        <v>398</v>
+      </c>
+      <c r="E61" s="657" t="s">
+        <v>399</v>
+      </c>
+      <c r="F61" s="657" t="s">
+        <v>400</v>
+      </c>
+      <c r="G61" s="657" t="s">
+        <v>401</v>
+      </c>
+      <c r="H61" s="657" t="s">
+        <v>329</v>
+      </c>
+      <c r="I61" s="657" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="658" t="s">
+        <v>402</v>
+      </c>
+      <c r="B62" s="658" t="s">
+        <v>402</v>
+      </c>
+      <c r="C62" s="658" t="s">
+        <v>403</v>
+      </c>
+      <c r="D62" s="658" t="s">
+        <v>404</v>
+      </c>
+      <c r="E62" s="658" t="s">
+        <v>405</v>
+      </c>
+      <c r="F62" s="658" t="s">
+        <v>406</v>
+      </c>
+      <c r="G62" s="658" t="s">
+        <v>407</v>
+      </c>
+      <c r="H62" s="658" t="s">
+        <v>329</v>
+      </c>
+      <c r="I62" s="658" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="659" t="s">
+        <v>408</v>
+      </c>
+      <c r="B63" s="659" t="s">
+        <v>408</v>
+      </c>
+      <c r="C63" s="659" t="s">
+        <v>409</v>
+      </c>
+      <c r="D63" s="659" t="s">
+        <v>410</v>
+      </c>
+      <c r="E63" s="659" t="s">
+        <v>411</v>
+      </c>
+      <c r="F63" s="659" t="s">
+        <v>412</v>
+      </c>
+      <c r="G63" s="659" t="s">
+        <v>413</v>
+      </c>
+      <c r="H63" s="659" t="s">
+        <v>329</v>
+      </c>
+      <c r="I63" s="659" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="660" t="s">
+        <v>414</v>
+      </c>
+      <c r="B64" s="660" t="s">
+        <v>414</v>
+      </c>
+      <c r="C64" s="660" t="s">
+        <v>415</v>
+      </c>
+      <c r="D64" s="660" t="s">
+        <v>416</v>
+      </c>
+      <c r="E64" s="660" t="s">
+        <v>417</v>
+      </c>
+      <c r="F64" s="660" t="s">
+        <v>418</v>
+      </c>
+      <c r="G64" s="660" t="s">
+        <v>419</v>
+      </c>
+      <c r="H64" s="660" t="s">
+        <v>329</v>
+      </c>
+      <c r="I64" s="660" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="661" t="s">
+        <v>420</v>
+      </c>
+      <c r="B65" s="661" t="s">
+        <v>420</v>
+      </c>
+      <c r="C65" s="661" t="s">
+        <v>421</v>
+      </c>
+      <c r="D65" s="661" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" s="661" t="s">
+        <v>422</v>
+      </c>
+      <c r="F65" s="661" t="s">
+        <v>93</v>
+      </c>
+      <c r="G65" s="661" t="s">
+        <v>423</v>
+      </c>
+      <c r="H65" s="661" t="s">
+        <v>424</v>
+      </c>
+      <c r="I65" s="661" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="662" t="s">
+        <v>425</v>
+      </c>
+      <c r="B66" s="662" t="s">
+        <v>425</v>
+      </c>
+      <c r="C66" s="662" t="s">
+        <v>426</v>
+      </c>
+      <c r="D66" s="662" t="s">
+        <v>427</v>
+      </c>
+      <c r="E66" s="662" t="s">
+        <v>428</v>
+      </c>
+      <c r="F66" s="662" t="s">
+        <v>429</v>
+      </c>
+      <c r="G66" s="662" t="s">
+        <v>430</v>
+      </c>
+      <c r="H66" s="662" t="s">
+        <v>329</v>
+      </c>
+      <c r="I66" s="662" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="663" t="s">
+        <v>431</v>
+      </c>
+      <c r="B67" s="663" t="s">
+        <v>431</v>
+      </c>
+      <c r="C67" s="663" t="s">
+        <v>432</v>
+      </c>
+      <c r="D67" s="663" t="s">
+        <v>433</v>
+      </c>
+      <c r="E67" s="663" t="s">
+        <v>434</v>
+      </c>
+      <c r="F67" s="663" t="s">
+        <v>435</v>
+      </c>
+      <c r="G67" s="663" t="s">
+        <v>436</v>
+      </c>
+      <c r="H67" s="663" t="s">
+        <v>329</v>
+      </c>
+      <c r="I67" s="663" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="664" t="s">
+        <v>437</v>
+      </c>
+      <c r="B68" s="664" t="s">
+        <v>437</v>
+      </c>
+      <c r="C68" s="664" t="s">
+        <v>438</v>
+      </c>
+      <c r="D68" s="664" t="s">
+        <v>439</v>
+      </c>
+      <c r="E68" s="664" t="s">
+        <v>440</v>
+      </c>
+      <c r="F68" s="664" t="s">
+        <v>441</v>
+      </c>
+      <c r="G68" s="664" t="s">
+        <v>442</v>
+      </c>
+      <c r="H68" s="664" t="s">
+        <v>329</v>
+      </c>
+      <c r="I68" s="664" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="665" t="s">
+        <v>443</v>
+      </c>
+      <c r="B69" s="665" t="s">
+        <v>443</v>
+      </c>
+      <c r="C69" s="665" t="s">
+        <v>444</v>
+      </c>
+      <c r="D69" s="665" t="s">
+        <v>445</v>
+      </c>
+      <c r="E69" s="665" t="s">
+        <v>446</v>
+      </c>
+      <c r="F69" s="665" t="s">
+        <v>447</v>
+      </c>
+      <c r="G69" s="665" t="s">
+        <v>448</v>
+      </c>
+      <c r="H69" s="665" t="s">
+        <v>329</v>
+      </c>
+      <c r="I69" s="665" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="666" t="s">
+        <v>449</v>
+      </c>
+      <c r="B70" s="666" t="s">
+        <v>449</v>
+      </c>
+      <c r="C70" s="666" t="s">
+        <v>450</v>
+      </c>
+      <c r="D70" s="666" t="s">
+        <v>451</v>
+      </c>
+      <c r="E70" s="666" t="s">
+        <v>452</v>
+      </c>
+      <c r="F70" s="666" t="s">
+        <v>453</v>
+      </c>
+      <c r="G70" s="666" t="s">
+        <v>454</v>
+      </c>
+      <c r="H70" s="666" t="s">
+        <v>329</v>
+      </c>
+      <c r="I70" s="666" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="667" t="s">
+        <v>455</v>
+      </c>
+      <c r="B71" s="667" t="s">
+        <v>455</v>
+      </c>
+      <c r="C71" s="667" t="s">
+        <v>456</v>
+      </c>
+      <c r="D71" s="667" t="s">
+        <v>457</v>
+      </c>
+      <c r="E71" s="667" t="s">
+        <v>458</v>
+      </c>
+      <c r="F71" s="667" t="s">
+        <v>459</v>
+      </c>
+      <c r="G71" s="667" t="s">
+        <v>460</v>
+      </c>
+      <c r="H71" s="667" t="s">
+        <v>329</v>
+      </c>
+      <c r="I71" s="667" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="668" t="s">
+        <v>461</v>
+      </c>
+      <c r="B72" s="668" t="s">
+        <v>461</v>
+      </c>
+      <c r="C72" s="668" t="s">
+        <v>462</v>
+      </c>
+      <c r="D72" s="668" t="s">
+        <v>463</v>
+      </c>
+      <c r="E72" s="668" t="s">
+        <v>464</v>
+      </c>
+      <c r="F72" s="668" t="s">
+        <v>465</v>
+      </c>
+      <c r="G72" s="668" t="s">
+        <v>466</v>
+      </c>
+      <c r="H72" s="668" t="s">
+        <v>329</v>
+      </c>
+      <c r="I72" s="668" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="669" t="s">
+        <v>467</v>
+      </c>
+      <c r="B73" s="669" t="s">
+        <v>467</v>
+      </c>
+      <c r="C73" s="669" t="s">
+        <v>468</v>
+      </c>
+      <c r="D73" s="669" t="s">
+        <v>469</v>
+      </c>
+      <c r="E73" s="669" t="s">
+        <v>470</v>
+      </c>
+      <c r="F73" s="669" t="s">
+        <v>471</v>
+      </c>
+      <c r="G73" s="669" t="s">
+        <v>472</v>
+      </c>
+      <c r="H73" s="669" t="s">
+        <v>329</v>
+      </c>
+      <c r="I73" s="669" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="670" t="s">
+        <v>473</v>
+      </c>
+      <c r="B74" s="670" t="s">
+        <v>473</v>
+      </c>
+      <c r="C74" s="670" t="s">
+        <v>474</v>
+      </c>
+      <c r="D74" s="670" t="s">
+        <v>475</v>
+      </c>
+      <c r="E74" s="670" t="s">
+        <v>476</v>
+      </c>
+      <c r="F74" s="670" t="s">
+        <v>477</v>
+      </c>
+      <c r="G74" s="670" t="s">
+        <v>478</v>
+      </c>
+      <c r="H74" s="670" t="s">
+        <v>329</v>
+      </c>
+      <c r="I74" s="670" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="671" t="s">
+        <v>479</v>
+      </c>
+      <c r="B75" s="671" t="s">
+        <v>479</v>
+      </c>
+      <c r="C75" s="671" t="s">
+        <v>480</v>
+      </c>
+      <c r="D75" s="671" t="s">
+        <v>481</v>
+      </c>
+      <c r="E75" s="671" t="s">
+        <v>482</v>
+      </c>
+      <c r="F75" s="671" t="s">
+        <v>483</v>
+      </c>
+      <c r="G75" s="671" t="s">
+        <v>484</v>
+      </c>
+      <c r="H75" s="671" t="s">
+        <v>329</v>
+      </c>
+      <c r="I75" s="671" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="672" t="s">
+        <v>485</v>
+      </c>
+      <c r="B76" s="672" t="s">
+        <v>485</v>
+      </c>
+      <c r="C76" s="672" t="s">
+        <v>486</v>
+      </c>
+      <c r="D76" s="672" t="s">
+        <v>487</v>
+      </c>
+      <c r="E76" s="672" t="s">
+        <v>488</v>
+      </c>
+      <c r="F76" s="672" t="s">
+        <v>489</v>
+      </c>
+      <c r="G76" s="672" t="s">
+        <v>490</v>
+      </c>
+      <c r="H76" s="672" t="s">
+        <v>329</v>
+      </c>
+      <c r="I76" s="672" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="673" t="s">
+        <v>491</v>
+      </c>
+      <c r="B77" s="673" t="s">
+        <v>491</v>
+      </c>
+      <c r="C77" s="673" t="s">
+        <v>492</v>
+      </c>
+      <c r="D77" s="673" t="s">
+        <v>493</v>
+      </c>
+      <c r="E77" s="673" t="s">
+        <v>494</v>
+      </c>
+      <c r="F77" s="673" t="s">
+        <v>495</v>
+      </c>
+      <c r="G77" s="673" t="s">
+        <v>496</v>
+      </c>
+      <c r="H77" s="673" t="s">
+        <v>329</v>
+      </c>
+      <c r="I77" s="673" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="674" t="s">
+        <v>497</v>
+      </c>
+      <c r="B78" s="674" t="s">
+        <v>497</v>
+      </c>
+      <c r="C78" s="674" t="s">
+        <v>498</v>
+      </c>
+      <c r="D78" s="674" t="s">
+        <v>499</v>
+      </c>
+      <c r="E78" s="674" t="s">
+        <v>500</v>
+      </c>
+      <c r="F78" s="674" t="s">
+        <v>501</v>
+      </c>
+      <c r="G78" s="674" t="s">
+        <v>502</v>
+      </c>
+      <c r="H78" s="674" t="s">
+        <v>329</v>
+      </c>
+      <c r="I78" s="674" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="675" t="s">
+        <v>503</v>
+      </c>
+      <c r="B79" s="675" t="s">
+        <v>503</v>
+      </c>
+      <c r="C79" s="675" t="s">
+        <v>504</v>
+      </c>
+      <c r="D79" s="675" t="s">
+        <v>505</v>
+      </c>
+      <c r="E79" s="675" t="s">
+        <v>506</v>
+      </c>
+      <c r="F79" s="675" t="s">
+        <v>507</v>
+      </c>
+      <c r="G79" s="675" t="s">
+        <v>508</v>
+      </c>
+      <c r="H79" s="675" t="s">
+        <v>329</v>
+      </c>
+      <c r="I79" s="675" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="676" t="s">
+        <v>509</v>
+      </c>
+      <c r="B80" s="676" t="s">
+        <v>509</v>
+      </c>
+      <c r="C80" s="676" t="s">
+        <v>510</v>
+      </c>
+      <c r="D80" s="676" t="s">
+        <v>511</v>
+      </c>
+      <c r="E80" s="676" t="s">
+        <v>512</v>
+      </c>
+      <c r="F80" s="676" t="s">
+        <v>513</v>
+      </c>
+      <c r="G80" s="676" t="s">
+        <v>514</v>
+      </c>
+      <c r="H80" s="676" t="s">
+        <v>17</v>
+      </c>
+      <c r="I80" s="676" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="677" t="s">
+        <v>515</v>
+      </c>
+      <c r="B81" s="677" t="s">
+        <v>515</v>
+      </c>
+      <c r="C81" s="677" t="s">
+        <v>516</v>
+      </c>
+      <c r="D81" s="677" t="s">
+        <v>517</v>
+      </c>
+      <c r="E81" s="677" t="s">
+        <v>518</v>
+      </c>
+      <c r="F81" s="677" t="s">
+        <v>519</v>
+      </c>
+      <c r="G81" s="677" t="s">
+        <v>520</v>
+      </c>
+      <c r="H81" s="677" t="s">
+        <v>521</v>
+      </c>
+      <c r="I81" s="677" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="678" t="s">
+        <v>522</v>
+      </c>
+      <c r="B82" s="678" t="s">
+        <v>522</v>
+      </c>
+      <c r="C82" s="678" t="s">
+        <v>523</v>
+      </c>
+      <c r="D82" s="678" t="s">
+        <v>524</v>
+      </c>
+      <c r="E82" s="678" t="s">
+        <v>525</v>
+      </c>
+      <c r="F82" s="678" t="s">
+        <v>526</v>
+      </c>
+      <c r="G82" s="678" t="s">
+        <v>527</v>
+      </c>
+      <c r="H82" s="678" t="s">
+        <v>528</v>
+      </c>
+      <c r="I82" s="678" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="679" t="s">
+        <v>529</v>
+      </c>
+      <c r="B83" s="679" t="s">
+        <v>529</v>
+      </c>
+      <c r="C83" s="679" t="s">
+        <v>530</v>
+      </c>
+      <c r="D83" s="679" t="s">
+        <v>531</v>
+      </c>
+      <c r="E83" s="679" t="s">
+        <v>532</v>
+      </c>
+      <c r="F83" s="679" t="s">
+        <v>533</v>
+      </c>
+      <c r="G83" s="679" t="s">
+        <v>534</v>
+      </c>
+      <c r="H83" s="679" t="s">
+        <v>17</v>
+      </c>
+      <c r="I83" s="679" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="680" t="s">
+        <v>535</v>
+      </c>
+      <c r="B84" s="680" t="s">
+        <v>535</v>
+      </c>
+      <c r="C84" s="680" t="s">
+        <v>536</v>
+      </c>
+      <c r="D84" s="680" t="s">
+        <v>537</v>
+      </c>
+      <c r="E84" s="680" t="s">
+        <v>538</v>
+      </c>
+      <c r="F84" s="680" t="s">
+        <v>539</v>
+      </c>
+      <c r="G84" s="680" t="s">
+        <v>540</v>
+      </c>
+      <c r="H84" s="680" t="s">
+        <v>541</v>
+      </c>
+      <c r="I84" s="680" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="681" t="s">
+        <v>542</v>
+      </c>
+      <c r="B85" s="681" t="s">
+        <v>542</v>
+      </c>
+      <c r="C85" s="681" t="s">
+        <v>543</v>
+      </c>
+      <c r="D85" s="681" t="s">
+        <v>544</v>
+      </c>
+      <c r="E85" s="681" t="s">
+        <v>545</v>
+      </c>
+      <c r="F85" s="681" t="s">
+        <v>546</v>
+      </c>
+      <c r="G85" s="681" t="s">
+        <v>547</v>
+      </c>
+      <c r="H85" s="681" t="s">
+        <v>17</v>
+      </c>
+      <c r="I85" s="681" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="682" t="s">
+        <v>548</v>
+      </c>
+      <c r="B86" s="682" t="s">
+        <v>548</v>
+      </c>
+      <c r="C86" s="682" t="s">
+        <v>549</v>
+      </c>
+      <c r="D86" s="682" t="s">
+        <v>550</v>
+      </c>
+      <c r="E86" s="682" t="s">
+        <v>551</v>
+      </c>
+      <c r="F86" s="682" t="s">
+        <v>552</v>
+      </c>
+      <c r="G86" s="682" t="s">
+        <v>553</v>
+      </c>
+      <c r="H86" s="682" t="s">
+        <v>554</v>
+      </c>
+      <c r="I86" s="682" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="683" t="s">
+        <v>555</v>
+      </c>
+      <c r="B87" s="683" t="s">
+        <v>555</v>
+      </c>
+      <c r="C87" s="683" t="s">
+        <v>556</v>
+      </c>
+      <c r="D87" s="683" t="s">
+        <v>557</v>
+      </c>
+      <c r="E87" s="683" t="s">
+        <v>558</v>
+      </c>
+      <c r="F87" s="683" t="s">
+        <v>559</v>
+      </c>
+      <c r="G87" s="683" t="s">
+        <v>560</v>
+      </c>
+      <c r="H87" s="683" t="s">
+        <v>17</v>
+      </c>
+      <c r="I87" s="683" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="684" t="s">
+        <v>561</v>
+      </c>
+      <c r="B88" s="684" t="s">
+        <v>561</v>
+      </c>
+      <c r="C88" s="684" t="s">
+        <v>562</v>
+      </c>
+      <c r="D88" s="684" t="s">
+        <v>563</v>
+      </c>
+      <c r="E88" s="684" t="s">
+        <v>564</v>
+      </c>
+      <c r="F88" s="684" t="s">
+        <v>565</v>
+      </c>
+      <c r="G88" s="684" t="s">
+        <v>566</v>
+      </c>
+      <c r="H88" s="684" t="s">
+        <v>24</v>
+      </c>
+      <c r="I88" s="684" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="685" t="s">
+        <v>567</v>
+      </c>
+      <c r="B89" s="685" t="s">
+        <v>567</v>
+      </c>
+      <c r="C89" s="685" t="s">
+        <v>568</v>
+      </c>
+      <c r="D89" s="685" t="s">
+        <v>569</v>
+      </c>
+      <c r="E89" s="685" t="s">
+        <v>570</v>
+      </c>
+      <c r="F89" s="685" t="s">
+        <v>571</v>
+      </c>
+      <c r="G89" s="685" t="s">
+        <v>572</v>
+      </c>
+      <c r="H89" s="685" t="s">
+        <v>573</v>
+      </c>
+      <c r="I89" s="685" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="686" t="s">
+        <v>574</v>
+      </c>
+      <c r="B90" s="686" t="s">
+        <v>574</v>
+      </c>
+      <c r="C90" s="686" t="s">
+        <v>575</v>
+      </c>
+      <c r="D90" s="686" t="s">
+        <v>576</v>
+      </c>
+      <c r="E90" s="686" t="s">
+        <v>577</v>
+      </c>
+      <c r="F90" s="686" t="s">
+        <v>578</v>
+      </c>
+      <c r="G90" s="686" t="s">
+        <v>579</v>
+      </c>
+      <c r="H90" s="686" t="s">
+        <v>573</v>
+      </c>
+      <c r="I90" s="686" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="687" t="s">
+        <v>580</v>
+      </c>
+      <c r="B91" s="687" t="s">
+        <v>580</v>
+      </c>
+      <c r="C91" s="687" t="s">
+        <v>581</v>
+      </c>
+      <c r="D91" s="687" t="s">
+        <v>582</v>
+      </c>
+      <c r="E91" s="687" t="s">
+        <v>583</v>
+      </c>
+      <c r="F91" s="687" t="s">
+        <v>584</v>
+      </c>
+      <c r="G91" s="687" t="s">
+        <v>585</v>
+      </c>
+      <c r="H91" s="687" t="s">
+        <v>573</v>
+      </c>
+      <c r="I91" s="687" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="688" t="s">
+        <v>586</v>
+      </c>
+      <c r="B92" s="688" t="s">
+        <v>586</v>
+      </c>
+      <c r="C92" s="688" t="s">
+        <v>587</v>
+      </c>
+      <c r="D92" s="688" t="s">
+        <v>588</v>
+      </c>
+      <c r="E92" s="688" t="s">
+        <v>589</v>
+      </c>
+      <c r="F92" s="688" t="s">
+        <v>93</v>
+      </c>
+      <c r="G92" s="688" t="s">
+        <v>590</v>
+      </c>
+      <c r="H92" s="688" t="s">
+        <v>591</v>
+      </c>
+      <c r="I92" s="688" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="689" t="s">
+        <v>592</v>
+      </c>
+      <c r="B93" s="689" t="s">
+        <v>592</v>
+      </c>
+      <c r="C93" s="689" t="s">
+        <v>593</v>
+      </c>
+      <c r="D93" s="689" t="s">
+        <v>594</v>
+      </c>
+      <c r="E93" s="689" t="s">
+        <v>595</v>
+      </c>
+      <c r="F93" s="689" t="s">
+        <v>93</v>
+      </c>
+      <c r="G93" s="689" t="s">
+        <v>596</v>
+      </c>
+      <c r="H93" s="689" t="s">
+        <v>591</v>
+      </c>
+      <c r="I93" s="689" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="690" t="s">
+        <v>597</v>
+      </c>
+      <c r="B94" s="690" t="s">
+        <v>597</v>
+      </c>
+      <c r="C94" s="690" t="s">
+        <v>598</v>
+      </c>
+      <c r="D94" s="690" t="s">
+        <v>599</v>
+      </c>
+      <c r="E94" s="690" t="s">
+        <v>600</v>
+      </c>
+      <c r="F94" s="690" t="s">
+        <v>601</v>
+      </c>
+      <c r="G94" s="690" t="s">
+        <v>602</v>
+      </c>
+      <c r="H94" s="690" t="s">
+        <v>24</v>
+      </c>
+      <c r="I94" s="690" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="691" t="s">
+        <v>603</v>
+      </c>
+      <c r="B95" s="691" t="s">
+        <v>603</v>
+      </c>
+      <c r="C95" s="691" t="s">
+        <v>604</v>
+      </c>
+      <c r="D95" s="691" t="s">
+        <v>605</v>
+      </c>
+      <c r="E95" s="691" t="s">
+        <v>606</v>
+      </c>
+      <c r="F95" s="691" t="s">
+        <v>607</v>
+      </c>
+      <c r="G95" s="691" t="s">
+        <v>608</v>
+      </c>
+      <c r="H95" s="691" t="s">
+        <v>24</v>
+      </c>
+      <c r="I95" s="691" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="692" t="s">
+        <v>609</v>
+      </c>
+      <c r="B96" s="692" t="s">
+        <v>609</v>
+      </c>
+      <c r="C96" s="692" t="s">
+        <v>610</v>
+      </c>
+      <c r="D96" s="692" t="s">
+        <v>611</v>
+      </c>
+      <c r="E96" s="692" t="s">
+        <v>612</v>
+      </c>
+      <c r="F96" s="692" t="s">
+        <v>613</v>
+      </c>
+      <c r="G96" s="692" t="s">
+        <v>614</v>
+      </c>
+      <c r="H96" s="692" t="s">
+        <v>615</v>
+      </c>
+      <c r="I96" s="692" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="693" t="s">
+        <v>616</v>
+      </c>
+      <c r="B97" s="693" t="s">
+        <v>616</v>
+      </c>
+      <c r="C97" s="693" t="s">
+        <v>617</v>
+      </c>
+      <c r="D97" s="693" t="s">
+        <v>618</v>
+      </c>
+      <c r="E97" s="693" t="s">
+        <v>619</v>
+      </c>
+      <c r="F97" s="693" t="s">
+        <v>620</v>
+      </c>
+      <c r="G97" s="693" t="s">
+        <v>621</v>
+      </c>
+      <c r="H97" s="693" t="s">
+        <v>615</v>
+      </c>
+      <c r="I97" s="693" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="694" t="s">
+        <v>622</v>
+      </c>
+      <c r="B98" s="694" t="s">
+        <v>622</v>
+      </c>
+      <c r="C98" s="694" t="s">
+        <v>623</v>
+      </c>
+      <c r="D98" s="694" t="s">
+        <v>624</v>
+      </c>
+      <c r="E98" s="694" t="s">
+        <v>625</v>
+      </c>
+      <c r="F98" s="694" t="s">
+        <v>626</v>
+      </c>
+      <c r="G98" s="694" t="s">
+        <v>627</v>
+      </c>
+      <c r="H98" s="694" t="s">
+        <v>615</v>
+      </c>
+      <c r="I98" s="694" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="695" t="s">
+        <v>628</v>
+      </c>
+      <c r="B99" s="695" t="s">
+        <v>628</v>
+      </c>
+      <c r="C99" s="695" t="s">
+        <v>629</v>
+      </c>
+      <c r="D99" s="695" t="s">
+        <v>630</v>
+      </c>
+      <c r="E99" s="695" t="s">
+        <v>631</v>
+      </c>
+      <c r="F99" s="695" t="s">
+        <v>632</v>
+      </c>
+      <c r="G99" s="695" t="s">
+        <v>633</v>
+      </c>
+      <c r="H99" s="695" t="s">
+        <v>615</v>
+      </c>
+      <c r="I99" s="695" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="696" t="s">
+        <v>634</v>
+      </c>
+      <c r="B100" s="696" t="s">
+        <v>634</v>
+      </c>
+      <c r="C100" s="696" t="s">
+        <v>635</v>
+      </c>
+      <c r="D100" s="696" t="s">
+        <v>636</v>
+      </c>
+      <c r="E100" s="696" t="s">
+        <v>637</v>
+      </c>
+      <c r="F100" s="696" t="s">
+        <v>638</v>
+      </c>
+      <c r="G100" s="696" t="s">
+        <v>639</v>
+      </c>
+      <c r="H100" s="696" t="s">
+        <v>424</v>
+      </c>
+      <c r="I100" s="696" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="697" t="s">
+        <v>640</v>
+      </c>
+      <c r="B101" s="697" t="s">
+        <v>640</v>
+      </c>
+      <c r="C101" s="697" t="s">
+        <v>641</v>
+      </c>
+      <c r="D101" s="697" t="s">
+        <v>642</v>
+      </c>
+      <c r="E101" s="697" t="s">
+        <v>643</v>
+      </c>
+      <c r="F101" s="697" t="s">
+        <v>644</v>
+      </c>
+      <c r="G101" s="697" t="s">
+        <v>645</v>
+      </c>
+      <c r="H101" s="697" t="s">
+        <v>615</v>
+      </c>
+      <c r="I101" s="697" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the javadoc for the pageobjects, fixed closingpromo invocations in the modules
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5726" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5762" uniqueCount="646">
   <si>
     <t>URL</t>
   </si>
@@ -2056,7 +2056,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="92">
+  <fills count="93">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2514,8 +2514,13 @@
         <fgColor indexed="49"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="358">
+  <borders count="362">
     <border>
       <left/>
       <right/>
@@ -4140,11 +4145,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="698">
+  <cellXfs count="702">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -6235,6 +6258,18 @@
       <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="357" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="92" borderId="361" xfId="0" applyFill="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="361" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="361" xfId="0" applyBorder="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="361" xfId="0" applyBorder="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -6559,2943 +6594,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="85.92578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="85.92578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="62.68359375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="146.671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="47.15625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="59.07421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="36.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="143.35546875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="24.2265625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="136.05078125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="188.4921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="103.52734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="165.984375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="10.87109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="597" t="s">
+      <c r="A1" s="698" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="597" t="s">
+      <c r="B1" s="698" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="597" t="s">
+      <c r="C1" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="597" t="s">
+      <c r="D1" s="698" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="597" t="s">
+      <c r="E1" s="698" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="597" t="s">
+      <c r="F1" s="698" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="597" t="s">
+      <c r="G1" s="698" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="597" t="s">
+      <c r="H1" s="698" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="597" t="s">
+      <c r="I1" s="698" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="598" t="s">
+      <c r="A2" s="699" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="598" t="s">
+      <c r="B2" s="699" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="598" t="s">
+      <c r="C2" s="699" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="598" t="s">
+      <c r="D2" s="699" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="598" t="s">
-        <v>14</v>
+      <c r="E2" s="699" t="s">
+        <v>44</v>
       </c>
-      <c r="F2" s="598" t="s">
+      <c r="F2" s="699" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="598" t="s">
+      <c r="G2" s="699" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="598" t="s">
+      <c r="H2" s="699" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="598" t="s">
+      <c r="I2" s="699" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="599" t="s">
+      <c r="A3" s="700" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="599" t="s">
+      <c r="B3" s="700" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="599" t="s">
+      <c r="C3" s="700" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="599" t="s">
+      <c r="D3" s="700" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="599" t="s">
-        <v>21</v>
+      <c r="E3" s="700" t="s">
+        <v>45</v>
       </c>
-      <c r="F3" s="599" t="s">
-        <v>141</v>
+      <c r="F3" s="700" t="s">
+        <v>145</v>
       </c>
-      <c r="G3" s="599" t="s">
+      <c r="G3" s="700" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="599" t="s">
+      <c r="H3" s="700" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="599" t="s">
+      <c r="I3" s="700" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="600" t="s">
+      <c r="A4" s="701" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="600" t="s">
+      <c r="B4" s="701" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="600" t="s">
+      <c r="C4" s="701" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="600" t="s">
+      <c r="D4" s="701" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="600" t="s">
-        <v>28</v>
+      <c r="E4" s="701" t="s">
+        <v>146</v>
       </c>
-      <c r="F4" s="600" t="s">
+      <c r="F4" s="701" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="600" t="s">
+      <c r="G4" s="701" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="600" t="s">
+      <c r="H4" s="701" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="600" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="601" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="601" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="601" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="601" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="601" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="601" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="601" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="601" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="601" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="602" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="602" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="602" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="602" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="602" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="602" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="602" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="602" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="602" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="603" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="603" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="603" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="603" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="603" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="603" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="603" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="603" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="603" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="604" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="604" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="604" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="604" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="604" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="604" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="604" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="604" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="604" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="605" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="605" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="605" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="605" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="605" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="605" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="605" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="605" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="605" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="606" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="606" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="606" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="606" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="606" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="606" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="606" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="606" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="606" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="607" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="607" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="607" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="607" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="607" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="607" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="607" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="607" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" s="607" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="608" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="608" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="608" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="608" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="608" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="608" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="608" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="608" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="608" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="609" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="609" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="609" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="609" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="609" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="609" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="609" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="609" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" s="609" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="610" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="610" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="610" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="610" t="s">
-        <v>152</v>
-      </c>
-      <c r="E14" s="610" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="610" t="s">
-        <v>153</v>
-      </c>
-      <c r="G14" s="610" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" s="610" t="s">
-        <v>96</v>
-      </c>
-      <c r="I14" s="610" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="611" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="611" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="611" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="611" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="611" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="611" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="611" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="611" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="611" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="612" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="612" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="612" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="612" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="612" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="612" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="612" t="s">
-        <v>108</v>
-      </c>
-      <c r="H16" s="612" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="612" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="613" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="613" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="613" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="613" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="613" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="613" t="s">
-        <v>113</v>
-      </c>
-      <c r="G17" s="613" t="s">
-        <v>114</v>
-      </c>
-      <c r="H17" s="613" t="s">
-        <v>115</v>
-      </c>
-      <c r="I17" s="613" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="614" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" s="614" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="614" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="614" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="614" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="614" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="614" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" s="614" t="s">
-        <v>115</v>
-      </c>
-      <c r="I18" s="614" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="615" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" s="615" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="615" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="615" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="615" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="615" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" s="615" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="615" t="s">
-        <v>115</v>
-      </c>
-      <c r="I19" s="615" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="616" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="616" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="616" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="616" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="616" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="616" t="s">
-        <v>132</v>
-      </c>
-      <c r="G20" s="616" t="s">
-        <v>133</v>
-      </c>
-      <c r="H20" s="616" t="s">
-        <v>115</v>
-      </c>
-      <c r="I20" s="616" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="617" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="617" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="617" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="617" t="s">
-        <v>136</v>
-      </c>
-      <c r="E21" s="617" t="s">
-        <v>137</v>
-      </c>
-      <c r="F21" s="617" t="s">
-        <v>138</v>
-      </c>
-      <c r="G21" s="617" t="s">
-        <v>139</v>
-      </c>
-      <c r="H21" s="617" t="s">
-        <v>115</v>
-      </c>
-      <c r="I21" s="617" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="618" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" s="618" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="618" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="618" t="s">
-        <v>156</v>
-      </c>
-      <c r="E22" s="618" t="s">
-        <v>157</v>
-      </c>
-      <c r="F22" s="618" t="s">
-        <v>158</v>
-      </c>
-      <c r="G22" s="618" t="s">
-        <v>159</v>
-      </c>
-      <c r="H22" s="618" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" s="618" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="619" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="619" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" s="619" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="619" t="s">
-        <v>162</v>
-      </c>
-      <c r="E23" s="619" t="s">
-        <v>163</v>
-      </c>
-      <c r="F23" s="619" t="s">
-        <v>164</v>
-      </c>
-      <c r="G23" s="619" t="s">
-        <v>165</v>
-      </c>
-      <c r="H23" s="619" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="619" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="620" t="s">
-        <v>166</v>
-      </c>
-      <c r="B24" s="620" t="s">
-        <v>166</v>
-      </c>
-      <c r="C24" s="620" t="s">
-        <v>167</v>
-      </c>
-      <c r="D24" s="620" t="s">
-        <v>168</v>
-      </c>
-      <c r="E24" s="620" t="s">
-        <v>169</v>
-      </c>
-      <c r="F24" s="620" t="s">
-        <v>170</v>
-      </c>
-      <c r="G24" s="620" t="s">
-        <v>171</v>
-      </c>
-      <c r="H24" s="620" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="620" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="621" t="s">
-        <v>173</v>
-      </c>
-      <c r="B25" s="621" t="s">
-        <v>173</v>
-      </c>
-      <c r="C25" s="621" t="s">
-        <v>174</v>
-      </c>
-      <c r="D25" s="621" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="621" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" s="621" t="s">
-        <v>177</v>
-      </c>
-      <c r="G25" s="621" t="s">
-        <v>178</v>
-      </c>
-      <c r="H25" s="621" t="s">
-        <v>172</v>
-      </c>
-      <c r="I25" s="621" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="622" t="s">
-        <v>179</v>
-      </c>
-      <c r="B26" s="622" t="s">
-        <v>179</v>
-      </c>
-      <c r="C26" s="622" t="s">
-        <v>180</v>
-      </c>
-      <c r="D26" s="622" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="622" t="s">
-        <v>182</v>
-      </c>
-      <c r="F26" s="622" t="s">
-        <v>183</v>
-      </c>
-      <c r="G26" s="622" t="s">
-        <v>184</v>
-      </c>
-      <c r="H26" s="622" t="s">
-        <v>185</v>
-      </c>
-      <c r="I26" s="622" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="623" t="s">
-        <v>186</v>
-      </c>
-      <c r="B27" s="623" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="623" t="s">
-        <v>187</v>
-      </c>
-      <c r="D27" s="623" t="s">
-        <v>188</v>
-      </c>
-      <c r="E27" s="623" t="s">
-        <v>189</v>
-      </c>
-      <c r="F27" s="623" t="s">
-        <v>190</v>
-      </c>
-      <c r="G27" s="623" t="s">
-        <v>191</v>
-      </c>
-      <c r="H27" s="623" t="s">
-        <v>185</v>
-      </c>
-      <c r="I27" s="623" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="624" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="624" t="s">
-        <v>192</v>
-      </c>
-      <c r="C28" s="624" t="s">
-        <v>193</v>
-      </c>
-      <c r="D28" s="624" t="s">
-        <v>194</v>
-      </c>
-      <c r="E28" s="624" t="s">
-        <v>195</v>
-      </c>
-      <c r="F28" s="624" t="s">
-        <v>196</v>
-      </c>
-      <c r="G28" s="624" t="s">
-        <v>197</v>
-      </c>
-      <c r="H28" s="624" t="s">
-        <v>185</v>
-      </c>
-      <c r="I28" s="624" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="625" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="625" t="s">
-        <v>198</v>
-      </c>
-      <c r="C29" s="625" t="s">
-        <v>199</v>
-      </c>
-      <c r="D29" s="625" t="s">
-        <v>200</v>
-      </c>
-      <c r="E29" s="625" t="s">
-        <v>201</v>
-      </c>
-      <c r="F29" s="625" t="s">
-        <v>202</v>
-      </c>
-      <c r="G29" s="625" t="s">
-        <v>203</v>
-      </c>
-      <c r="H29" s="625" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="625" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="626" t="s">
-        <v>204</v>
-      </c>
-      <c r="B30" s="626" t="s">
-        <v>204</v>
-      </c>
-      <c r="C30" s="626" t="s">
-        <v>205</v>
-      </c>
-      <c r="D30" s="626" t="s">
-        <v>206</v>
-      </c>
-      <c r="E30" s="626" t="s">
-        <v>207</v>
-      </c>
-      <c r="F30" s="626" t="s">
-        <v>208</v>
-      </c>
-      <c r="G30" s="626" t="s">
-        <v>209</v>
-      </c>
-      <c r="H30" s="626" t="s">
-        <v>210</v>
-      </c>
-      <c r="I30" s="626" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="627" t="s">
-        <v>211</v>
-      </c>
-      <c r="B31" s="627" t="s">
-        <v>211</v>
-      </c>
-      <c r="C31" s="627" t="s">
-        <v>212</v>
-      </c>
-      <c r="D31" s="627" t="s">
-        <v>213</v>
-      </c>
-      <c r="E31" s="627" t="s">
-        <v>214</v>
-      </c>
-      <c r="F31" s="627" t="s">
-        <v>215</v>
-      </c>
-      <c r="G31" s="627" t="s">
-        <v>216</v>
-      </c>
-      <c r="H31" s="627" t="s">
-        <v>210</v>
-      </c>
-      <c r="I31" s="627" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="628" t="s">
-        <v>217</v>
-      </c>
-      <c r="B32" s="628" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="628" t="s">
-        <v>218</v>
-      </c>
-      <c r="D32" s="628" t="s">
-        <v>219</v>
-      </c>
-      <c r="E32" s="628" t="s">
-        <v>220</v>
-      </c>
-      <c r="F32" s="628" t="s">
-        <v>221</v>
-      </c>
-      <c r="G32" s="628" t="s">
-        <v>222</v>
-      </c>
-      <c r="H32" s="628" t="s">
-        <v>223</v>
-      </c>
-      <c r="I32" s="628" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="629" t="s">
-        <v>224</v>
-      </c>
-      <c r="B33" s="629" t="s">
-        <v>224</v>
-      </c>
-      <c r="C33" s="629" t="s">
-        <v>225</v>
-      </c>
-      <c r="D33" s="629" t="s">
-        <v>226</v>
-      </c>
-      <c r="E33" s="629" t="s">
-        <v>227</v>
-      </c>
-      <c r="F33" s="629" t="s">
-        <v>228</v>
-      </c>
-      <c r="G33" s="629" t="s">
-        <v>229</v>
-      </c>
-      <c r="H33" s="629" t="s">
-        <v>24</v>
-      </c>
-      <c r="I33" s="629" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="630" t="s">
-        <v>230</v>
-      </c>
-      <c r="B34" s="630" t="s">
-        <v>230</v>
-      </c>
-      <c r="C34" s="630" t="s">
-        <v>231</v>
-      </c>
-      <c r="D34" s="630" t="s">
-        <v>232</v>
-      </c>
-      <c r="E34" s="630" t="s">
-        <v>233</v>
-      </c>
-      <c r="F34" s="630" t="s">
-        <v>234</v>
-      </c>
-      <c r="G34" s="630" t="s">
-        <v>235</v>
-      </c>
-      <c r="H34" s="630" t="s">
-        <v>236</v>
-      </c>
-      <c r="I34" s="630" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="631" t="s">
-        <v>237</v>
-      </c>
-      <c r="B35" s="631" t="s">
-        <v>237</v>
-      </c>
-      <c r="C35" s="631" t="s">
-        <v>238</v>
-      </c>
-      <c r="D35" s="631" t="s">
-        <v>239</v>
-      </c>
-      <c r="E35" s="631" t="s">
-        <v>240</v>
-      </c>
-      <c r="F35" s="631" t="s">
-        <v>241</v>
-      </c>
-      <c r="G35" s="631" t="s">
-        <v>242</v>
-      </c>
-      <c r="H35" s="631" t="s">
-        <v>236</v>
-      </c>
-      <c r="I35" s="631" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="632" t="s">
-        <v>243</v>
-      </c>
-      <c r="B36" s="632" t="s">
-        <v>243</v>
-      </c>
-      <c r="C36" s="632" t="s">
-        <v>244</v>
-      </c>
-      <c r="D36" s="632" t="s">
-        <v>245</v>
-      </c>
-      <c r="E36" s="632" t="s">
-        <v>246</v>
-      </c>
-      <c r="F36" s="632" t="s">
-        <v>247</v>
-      </c>
-      <c r="G36" s="632" t="s">
-        <v>248</v>
-      </c>
-      <c r="H36" s="632" t="s">
-        <v>236</v>
-      </c>
-      <c r="I36" s="632" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="633" t="s">
-        <v>249</v>
-      </c>
-      <c r="B37" s="633" t="s">
-        <v>249</v>
-      </c>
-      <c r="C37" s="633" t="s">
-        <v>250</v>
-      </c>
-      <c r="D37" s="633" t="s">
-        <v>251</v>
-      </c>
-      <c r="E37" s="633" t="s">
-        <v>252</v>
-      </c>
-      <c r="F37" s="633" t="s">
-        <v>253</v>
-      </c>
-      <c r="G37" s="633" t="s">
-        <v>254</v>
-      </c>
-      <c r="H37" s="633" t="s">
-        <v>236</v>
-      </c>
-      <c r="I37" s="633" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="634" t="s">
-        <v>255</v>
-      </c>
-      <c r="B38" s="634" t="s">
-        <v>255</v>
-      </c>
-      <c r="C38" s="634" t="s">
-        <v>256</v>
-      </c>
-      <c r="D38" s="634" t="s">
-        <v>257</v>
-      </c>
-      <c r="E38" s="634" t="s">
-        <v>258</v>
-      </c>
-      <c r="F38" s="634" t="s">
-        <v>259</v>
-      </c>
-      <c r="G38" s="634" t="s">
-        <v>260</v>
-      </c>
-      <c r="H38" s="634" t="s">
-        <v>261</v>
-      </c>
-      <c r="I38" s="634" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="635" t="s">
-        <v>262</v>
-      </c>
-      <c r="B39" s="635" t="s">
-        <v>262</v>
-      </c>
-      <c r="C39" s="635" t="s">
-        <v>263</v>
-      </c>
-      <c r="D39" s="635" t="s">
-        <v>264</v>
-      </c>
-      <c r="E39" s="635" t="s">
-        <v>265</v>
-      </c>
-      <c r="F39" s="635" t="s">
-        <v>266</v>
-      </c>
-      <c r="G39" s="635" t="s">
-        <v>267</v>
-      </c>
-      <c r="H39" s="635" t="s">
-        <v>210</v>
-      </c>
-      <c r="I39" s="635" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="636" t="s">
-        <v>268</v>
-      </c>
-      <c r="B40" s="636" t="s">
-        <v>268</v>
-      </c>
-      <c r="C40" s="636" t="s">
-        <v>269</v>
-      </c>
-      <c r="D40" s="636" t="s">
-        <v>270</v>
-      </c>
-      <c r="E40" s="636" t="s">
-        <v>271</v>
-      </c>
-      <c r="F40" s="636" t="s">
-        <v>272</v>
-      </c>
-      <c r="G40" s="636" t="s">
-        <v>273</v>
-      </c>
-      <c r="H40" s="636" t="s">
-        <v>24</v>
-      </c>
-      <c r="I40" s="636" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="637" t="s">
-        <v>274</v>
-      </c>
-      <c r="B41" s="637" t="s">
-        <v>274</v>
-      </c>
-      <c r="C41" s="637" t="s">
-        <v>275</v>
-      </c>
-      <c r="D41" s="637" t="s">
-        <v>276</v>
-      </c>
-      <c r="E41" s="637" t="s">
-        <v>277</v>
-      </c>
-      <c r="F41" s="637" t="s">
-        <v>278</v>
-      </c>
-      <c r="G41" s="637" t="s">
-        <v>279</v>
-      </c>
-      <c r="H41" s="637" t="s">
-        <v>280</v>
-      </c>
-      <c r="I41" s="637" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="638" t="s">
-        <v>281</v>
-      </c>
-      <c r="B42" s="638" t="s">
-        <v>281</v>
-      </c>
-      <c r="C42" s="638" t="s">
-        <v>282</v>
-      </c>
-      <c r="D42" s="638" t="s">
-        <v>283</v>
-      </c>
-      <c r="E42" s="638" t="s">
-        <v>284</v>
-      </c>
-      <c r="F42" s="638" t="s">
-        <v>285</v>
-      </c>
-      <c r="G42" s="638" t="s">
-        <v>286</v>
-      </c>
-      <c r="H42" s="638" t="s">
-        <v>280</v>
-      </c>
-      <c r="I42" s="638" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="639" t="s">
-        <v>287</v>
-      </c>
-      <c r="B43" s="639" t="s">
-        <v>287</v>
-      </c>
-      <c r="C43" s="639" t="s">
-        <v>288</v>
-      </c>
-      <c r="D43" s="639" t="s">
-        <v>289</v>
-      </c>
-      <c r="E43" s="639" t="s">
-        <v>290</v>
-      </c>
-      <c r="F43" s="639" t="s">
-        <v>291</v>
-      </c>
-      <c r="G43" s="639" t="s">
-        <v>292</v>
-      </c>
-      <c r="H43" s="639" t="s">
-        <v>280</v>
-      </c>
-      <c r="I43" s="639" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="640" t="s">
-        <v>293</v>
-      </c>
-      <c r="B44" s="640" t="s">
-        <v>293</v>
-      </c>
-      <c r="C44" s="640" t="s">
-        <v>294</v>
-      </c>
-      <c r="D44" s="640" t="s">
-        <v>295</v>
-      </c>
-      <c r="E44" s="640" t="s">
-        <v>296</v>
-      </c>
-      <c r="F44" s="640" t="s">
-        <v>297</v>
-      </c>
-      <c r="G44" s="640" t="s">
-        <v>298</v>
-      </c>
-      <c r="H44" s="640" t="s">
-        <v>280</v>
-      </c>
-      <c r="I44" s="640" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="641" t="s">
-        <v>299</v>
-      </c>
-      <c r="B45" s="641" t="s">
-        <v>299</v>
-      </c>
-      <c r="C45" s="641" t="s">
-        <v>300</v>
-      </c>
-      <c r="D45" s="641" t="s">
-        <v>301</v>
-      </c>
-      <c r="E45" s="641" t="s">
-        <v>302</v>
-      </c>
-      <c r="F45" s="641" t="s">
-        <v>303</v>
-      </c>
-      <c r="G45" s="641" t="s">
-        <v>304</v>
-      </c>
-      <c r="H45" s="641" t="s">
-        <v>280</v>
-      </c>
-      <c r="I45" s="641" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="642" t="s">
-        <v>305</v>
-      </c>
-      <c r="B46" s="642" t="s">
-        <v>305</v>
-      </c>
-      <c r="C46" s="642" t="s">
-        <v>306</v>
-      </c>
-      <c r="D46" s="642" t="s">
-        <v>307</v>
-      </c>
-      <c r="E46" s="642" t="s">
-        <v>308</v>
-      </c>
-      <c r="F46" s="642" t="s">
-        <v>309</v>
-      </c>
-      <c r="G46" s="642" t="s">
-        <v>310</v>
-      </c>
-      <c r="H46" s="642" t="s">
-        <v>17</v>
-      </c>
-      <c r="I46" s="642" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="643" t="s">
-        <v>311</v>
-      </c>
-      <c r="B47" s="643" t="s">
-        <v>311</v>
-      </c>
-      <c r="C47" s="643" t="s">
-        <v>312</v>
-      </c>
-      <c r="D47" s="643" t="s">
-        <v>313</v>
-      </c>
-      <c r="E47" s="643" t="s">
-        <v>314</v>
-      </c>
-      <c r="F47" s="643" t="s">
-        <v>315</v>
-      </c>
-      <c r="G47" s="643" t="s">
-        <v>316</v>
-      </c>
-      <c r="H47" s="643" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="643" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="644" t="s">
-        <v>317</v>
-      </c>
-      <c r="B48" s="644" t="s">
-        <v>317</v>
-      </c>
-      <c r="C48" s="644" t="s">
-        <v>318</v>
-      </c>
-      <c r="D48" s="644" t="s">
-        <v>319</v>
-      </c>
-      <c r="E48" s="644" t="s">
-        <v>320</v>
-      </c>
-      <c r="F48" s="644" t="s">
-        <v>321</v>
-      </c>
-      <c r="G48" s="644" t="s">
-        <v>322</v>
-      </c>
-      <c r="H48" s="644" t="s">
-        <v>24</v>
-      </c>
-      <c r="I48" s="644" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="645" t="s">
-        <v>323</v>
-      </c>
-      <c r="B49" s="645" t="s">
-        <v>323</v>
-      </c>
-      <c r="C49" s="645" t="s">
-        <v>324</v>
-      </c>
-      <c r="D49" s="645" t="s">
-        <v>325</v>
-      </c>
-      <c r="E49" s="645" t="s">
-        <v>326</v>
-      </c>
-      <c r="F49" s="645" t="s">
-        <v>327</v>
-      </c>
-      <c r="G49" s="645" t="s">
-        <v>328</v>
-      </c>
-      <c r="H49" s="645" t="s">
-        <v>329</v>
-      </c>
-      <c r="I49" s="645" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="646" t="s">
-        <v>330</v>
-      </c>
-      <c r="B50" s="646" t="s">
-        <v>330</v>
-      </c>
-      <c r="C50" s="646" t="s">
-        <v>331</v>
-      </c>
-      <c r="D50" s="646" t="s">
-        <v>332</v>
-      </c>
-      <c r="E50" s="646" t="s">
-        <v>333</v>
-      </c>
-      <c r="F50" s="646" t="s">
-        <v>334</v>
-      </c>
-      <c r="G50" s="646" t="s">
-        <v>335</v>
-      </c>
-      <c r="H50" s="646" t="s">
-        <v>329</v>
-      </c>
-      <c r="I50" s="646" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="647" t="s">
-        <v>336</v>
-      </c>
-      <c r="B51" s="647" t="s">
-        <v>336</v>
-      </c>
-      <c r="C51" s="647" t="s">
-        <v>337</v>
-      </c>
-      <c r="D51" s="647" t="s">
-        <v>338</v>
-      </c>
-      <c r="E51" s="647" t="s">
-        <v>339</v>
-      </c>
-      <c r="F51" s="647" t="s">
-        <v>340</v>
-      </c>
-      <c r="G51" s="647" t="s">
-        <v>341</v>
-      </c>
-      <c r="H51" s="647" t="s">
-        <v>329</v>
-      </c>
-      <c r="I51" s="647" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="648" t="s">
-        <v>342</v>
-      </c>
-      <c r="B52" s="648" t="s">
-        <v>342</v>
-      </c>
-      <c r="C52" s="648" t="s">
-        <v>343</v>
-      </c>
-      <c r="D52" s="648" t="s">
-        <v>344</v>
-      </c>
-      <c r="E52" s="648" t="s">
-        <v>345</v>
-      </c>
-      <c r="F52" s="648" t="s">
-        <v>346</v>
-      </c>
-      <c r="G52" s="648" t="s">
-        <v>347</v>
-      </c>
-      <c r="H52" s="648" t="s">
-        <v>329</v>
-      </c>
-      <c r="I52" s="648" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="649" t="s">
-        <v>348</v>
-      </c>
-      <c r="B53" s="649" t="s">
-        <v>348</v>
-      </c>
-      <c r="C53" s="649" t="s">
-        <v>349</v>
-      </c>
-      <c r="D53" s="649" t="s">
-        <v>350</v>
-      </c>
-      <c r="E53" s="649" t="s">
-        <v>351</v>
-      </c>
-      <c r="F53" s="649" t="s">
-        <v>352</v>
-      </c>
-      <c r="G53" s="649" t="s">
-        <v>353</v>
-      </c>
-      <c r="H53" s="649" t="s">
-        <v>329</v>
-      </c>
-      <c r="I53" s="649" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="650" t="s">
-        <v>354</v>
-      </c>
-      <c r="B54" s="650" t="s">
-        <v>354</v>
-      </c>
-      <c r="C54" s="650" t="s">
-        <v>355</v>
-      </c>
-      <c r="D54" s="650" t="s">
-        <v>356</v>
-      </c>
-      <c r="E54" s="650" t="s">
-        <v>357</v>
-      </c>
-      <c r="F54" s="650" t="s">
-        <v>358</v>
-      </c>
-      <c r="G54" s="650" t="s">
-        <v>359</v>
-      </c>
-      <c r="H54" s="650" t="s">
-        <v>329</v>
-      </c>
-      <c r="I54" s="650" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="651" t="s">
-        <v>360</v>
-      </c>
-      <c r="B55" s="651" t="s">
-        <v>360</v>
-      </c>
-      <c r="C55" s="651" t="s">
-        <v>361</v>
-      </c>
-      <c r="D55" s="651" t="s">
-        <v>362</v>
-      </c>
-      <c r="E55" s="651" t="s">
-        <v>363</v>
-      </c>
-      <c r="F55" s="651" t="s">
-        <v>364</v>
-      </c>
-      <c r="G55" s="651" t="s">
-        <v>365</v>
-      </c>
-      <c r="H55" s="651" t="s">
-        <v>329</v>
-      </c>
-      <c r="I55" s="651" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="652" t="s">
-        <v>366</v>
-      </c>
-      <c r="B56" s="652" t="s">
-        <v>366</v>
-      </c>
-      <c r="C56" s="652" t="s">
-        <v>367</v>
-      </c>
-      <c r="D56" s="652" t="s">
-        <v>368</v>
-      </c>
-      <c r="E56" s="652" t="s">
-        <v>369</v>
-      </c>
-      <c r="F56" s="652" t="s">
-        <v>370</v>
-      </c>
-      <c r="G56" s="652" t="s">
-        <v>371</v>
-      </c>
-      <c r="H56" s="652" t="s">
-        <v>329</v>
-      </c>
-      <c r="I56" s="652" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="653" t="s">
-        <v>372</v>
-      </c>
-      <c r="B57" s="653" t="s">
-        <v>372</v>
-      </c>
-      <c r="C57" s="653" t="s">
-        <v>373</v>
-      </c>
-      <c r="D57" s="653" t="s">
-        <v>374</v>
-      </c>
-      <c r="E57" s="653" t="s">
-        <v>375</v>
-      </c>
-      <c r="F57" s="653" t="s">
-        <v>376</v>
-      </c>
-      <c r="G57" s="653" t="s">
-        <v>377</v>
-      </c>
-      <c r="H57" s="653" t="s">
-        <v>329</v>
-      </c>
-      <c r="I57" s="653" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="654" t="s">
-        <v>378</v>
-      </c>
-      <c r="B58" s="654" t="s">
-        <v>378</v>
-      </c>
-      <c r="C58" s="654" t="s">
-        <v>379</v>
-      </c>
-      <c r="D58" s="654" t="s">
-        <v>380</v>
-      </c>
-      <c r="E58" s="654" t="s">
-        <v>381</v>
-      </c>
-      <c r="F58" s="654" t="s">
-        <v>382</v>
-      </c>
-      <c r="G58" s="654" t="s">
-        <v>383</v>
-      </c>
-      <c r="H58" s="654" t="s">
-        <v>329</v>
-      </c>
-      <c r="I58" s="654" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="655" t="s">
-        <v>384</v>
-      </c>
-      <c r="B59" s="655" t="s">
-        <v>384</v>
-      </c>
-      <c r="C59" s="655" t="s">
-        <v>385</v>
-      </c>
-      <c r="D59" s="655" t="s">
-        <v>386</v>
-      </c>
-      <c r="E59" s="655" t="s">
-        <v>387</v>
-      </c>
-      <c r="F59" s="655" t="s">
-        <v>388</v>
-      </c>
-      <c r="G59" s="655" t="s">
-        <v>389</v>
-      </c>
-      <c r="H59" s="655" t="s">
-        <v>329</v>
-      </c>
-      <c r="I59" s="655" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="656" t="s">
-        <v>390</v>
-      </c>
-      <c r="B60" s="656" t="s">
-        <v>390</v>
-      </c>
-      <c r="C60" s="656" t="s">
-        <v>391</v>
-      </c>
-      <c r="D60" s="656" t="s">
-        <v>392</v>
-      </c>
-      <c r="E60" s="656" t="s">
-        <v>393</v>
-      </c>
-      <c r="F60" s="656" t="s">
-        <v>394</v>
-      </c>
-      <c r="G60" s="656" t="s">
-        <v>395</v>
-      </c>
-      <c r="H60" s="656" t="s">
-        <v>329</v>
-      </c>
-      <c r="I60" s="656" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="657" t="s">
-        <v>396</v>
-      </c>
-      <c r="B61" s="657" t="s">
-        <v>396</v>
-      </c>
-      <c r="C61" s="657" t="s">
-        <v>397</v>
-      </c>
-      <c r="D61" s="657" t="s">
-        <v>398</v>
-      </c>
-      <c r="E61" s="657" t="s">
-        <v>399</v>
-      </c>
-      <c r="F61" s="657" t="s">
-        <v>400</v>
-      </c>
-      <c r="G61" s="657" t="s">
-        <v>401</v>
-      </c>
-      <c r="H61" s="657" t="s">
-        <v>329</v>
-      </c>
-      <c r="I61" s="657" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="658" t="s">
-        <v>402</v>
-      </c>
-      <c r="B62" s="658" t="s">
-        <v>402</v>
-      </c>
-      <c r="C62" s="658" t="s">
-        <v>403</v>
-      </c>
-      <c r="D62" s="658" t="s">
-        <v>404</v>
-      </c>
-      <c r="E62" s="658" t="s">
-        <v>405</v>
-      </c>
-      <c r="F62" s="658" t="s">
-        <v>406</v>
-      </c>
-      <c r="G62" s="658" t="s">
-        <v>407</v>
-      </c>
-      <c r="H62" s="658" t="s">
-        <v>329</v>
-      </c>
-      <c r="I62" s="658" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="659" t="s">
-        <v>408</v>
-      </c>
-      <c r="B63" s="659" t="s">
-        <v>408</v>
-      </c>
-      <c r="C63" s="659" t="s">
-        <v>409</v>
-      </c>
-      <c r="D63" s="659" t="s">
-        <v>410</v>
-      </c>
-      <c r="E63" s="659" t="s">
-        <v>411</v>
-      </c>
-      <c r="F63" s="659" t="s">
-        <v>412</v>
-      </c>
-      <c r="G63" s="659" t="s">
-        <v>413</v>
-      </c>
-      <c r="H63" s="659" t="s">
-        <v>329</v>
-      </c>
-      <c r="I63" s="659" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="660" t="s">
-        <v>414</v>
-      </c>
-      <c r="B64" s="660" t="s">
-        <v>414</v>
-      </c>
-      <c r="C64" s="660" t="s">
-        <v>415</v>
-      </c>
-      <c r="D64" s="660" t="s">
-        <v>416</v>
-      </c>
-      <c r="E64" s="660" t="s">
-        <v>417</v>
-      </c>
-      <c r="F64" s="660" t="s">
-        <v>418</v>
-      </c>
-      <c r="G64" s="660" t="s">
-        <v>419</v>
-      </c>
-      <c r="H64" s="660" t="s">
-        <v>329</v>
-      </c>
-      <c r="I64" s="660" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="661" t="s">
-        <v>420</v>
-      </c>
-      <c r="B65" s="661" t="s">
-        <v>420</v>
-      </c>
-      <c r="C65" s="661" t="s">
-        <v>421</v>
-      </c>
-      <c r="D65" s="661" t="s">
-        <v>93</v>
-      </c>
-      <c r="E65" s="661" t="s">
-        <v>422</v>
-      </c>
-      <c r="F65" s="661" t="s">
-        <v>93</v>
-      </c>
-      <c r="G65" s="661" t="s">
-        <v>423</v>
-      </c>
-      <c r="H65" s="661" t="s">
-        <v>424</v>
-      </c>
-      <c r="I65" s="661" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="662" t="s">
-        <v>425</v>
-      </c>
-      <c r="B66" s="662" t="s">
-        <v>425</v>
-      </c>
-      <c r="C66" s="662" t="s">
-        <v>426</v>
-      </c>
-      <c r="D66" s="662" t="s">
-        <v>427</v>
-      </c>
-      <c r="E66" s="662" t="s">
-        <v>428</v>
-      </c>
-      <c r="F66" s="662" t="s">
-        <v>429</v>
-      </c>
-      <c r="G66" s="662" t="s">
-        <v>430</v>
-      </c>
-      <c r="H66" s="662" t="s">
-        <v>329</v>
-      </c>
-      <c r="I66" s="662" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="663" t="s">
-        <v>431</v>
-      </c>
-      <c r="B67" s="663" t="s">
-        <v>431</v>
-      </c>
-      <c r="C67" s="663" t="s">
-        <v>432</v>
-      </c>
-      <c r="D67" s="663" t="s">
-        <v>433</v>
-      </c>
-      <c r="E67" s="663" t="s">
-        <v>434</v>
-      </c>
-      <c r="F67" s="663" t="s">
-        <v>435</v>
-      </c>
-      <c r="G67" s="663" t="s">
-        <v>436</v>
-      </c>
-      <c r="H67" s="663" t="s">
-        <v>329</v>
-      </c>
-      <c r="I67" s="663" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="664" t="s">
-        <v>437</v>
-      </c>
-      <c r="B68" s="664" t="s">
-        <v>437</v>
-      </c>
-      <c r="C68" s="664" t="s">
-        <v>438</v>
-      </c>
-      <c r="D68" s="664" t="s">
-        <v>439</v>
-      </c>
-      <c r="E68" s="664" t="s">
-        <v>440</v>
-      </c>
-      <c r="F68" s="664" t="s">
-        <v>441</v>
-      </c>
-      <c r="G68" s="664" t="s">
-        <v>442</v>
-      </c>
-      <c r="H68" s="664" t="s">
-        <v>329</v>
-      </c>
-      <c r="I68" s="664" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="665" t="s">
-        <v>443</v>
-      </c>
-      <c r="B69" s="665" t="s">
-        <v>443</v>
-      </c>
-      <c r="C69" s="665" t="s">
-        <v>444</v>
-      </c>
-      <c r="D69" s="665" t="s">
-        <v>445</v>
-      </c>
-      <c r="E69" s="665" t="s">
-        <v>446</v>
-      </c>
-      <c r="F69" s="665" t="s">
-        <v>447</v>
-      </c>
-      <c r="G69" s="665" t="s">
-        <v>448</v>
-      </c>
-      <c r="H69" s="665" t="s">
-        <v>329</v>
-      </c>
-      <c r="I69" s="665" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="666" t="s">
-        <v>449</v>
-      </c>
-      <c r="B70" s="666" t="s">
-        <v>449</v>
-      </c>
-      <c r="C70" s="666" t="s">
-        <v>450</v>
-      </c>
-      <c r="D70" s="666" t="s">
-        <v>451</v>
-      </c>
-      <c r="E70" s="666" t="s">
-        <v>452</v>
-      </c>
-      <c r="F70" s="666" t="s">
-        <v>453</v>
-      </c>
-      <c r="G70" s="666" t="s">
-        <v>454</v>
-      </c>
-      <c r="H70" s="666" t="s">
-        <v>329</v>
-      </c>
-      <c r="I70" s="666" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="667" t="s">
-        <v>455</v>
-      </c>
-      <c r="B71" s="667" t="s">
-        <v>455</v>
-      </c>
-      <c r="C71" s="667" t="s">
-        <v>456</v>
-      </c>
-      <c r="D71" s="667" t="s">
-        <v>457</v>
-      </c>
-      <c r="E71" s="667" t="s">
-        <v>458</v>
-      </c>
-      <c r="F71" s="667" t="s">
-        <v>459</v>
-      </c>
-      <c r="G71" s="667" t="s">
-        <v>460</v>
-      </c>
-      <c r="H71" s="667" t="s">
-        <v>329</v>
-      </c>
-      <c r="I71" s="667" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="668" t="s">
-        <v>461</v>
-      </c>
-      <c r="B72" s="668" t="s">
-        <v>461</v>
-      </c>
-      <c r="C72" s="668" t="s">
-        <v>462</v>
-      </c>
-      <c r="D72" s="668" t="s">
-        <v>463</v>
-      </c>
-      <c r="E72" s="668" t="s">
-        <v>464</v>
-      </c>
-      <c r="F72" s="668" t="s">
-        <v>465</v>
-      </c>
-      <c r="G72" s="668" t="s">
-        <v>466</v>
-      </c>
-      <c r="H72" s="668" t="s">
-        <v>329</v>
-      </c>
-      <c r="I72" s="668" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="669" t="s">
-        <v>467</v>
-      </c>
-      <c r="B73" s="669" t="s">
-        <v>467</v>
-      </c>
-      <c r="C73" s="669" t="s">
-        <v>468</v>
-      </c>
-      <c r="D73" s="669" t="s">
-        <v>469</v>
-      </c>
-      <c r="E73" s="669" t="s">
-        <v>470</v>
-      </c>
-      <c r="F73" s="669" t="s">
-        <v>471</v>
-      </c>
-      <c r="G73" s="669" t="s">
-        <v>472</v>
-      </c>
-      <c r="H73" s="669" t="s">
-        <v>329</v>
-      </c>
-      <c r="I73" s="669" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="670" t="s">
-        <v>473</v>
-      </c>
-      <c r="B74" s="670" t="s">
-        <v>473</v>
-      </c>
-      <c r="C74" s="670" t="s">
-        <v>474</v>
-      </c>
-      <c r="D74" s="670" t="s">
-        <v>475</v>
-      </c>
-      <c r="E74" s="670" t="s">
-        <v>476</v>
-      </c>
-      <c r="F74" s="670" t="s">
-        <v>477</v>
-      </c>
-      <c r="G74" s="670" t="s">
-        <v>478</v>
-      </c>
-      <c r="H74" s="670" t="s">
-        <v>329</v>
-      </c>
-      <c r="I74" s="670" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="671" t="s">
-        <v>479</v>
-      </c>
-      <c r="B75" s="671" t="s">
-        <v>479</v>
-      </c>
-      <c r="C75" s="671" t="s">
-        <v>480</v>
-      </c>
-      <c r="D75" s="671" t="s">
-        <v>481</v>
-      </c>
-      <c r="E75" s="671" t="s">
-        <v>482</v>
-      </c>
-      <c r="F75" s="671" t="s">
-        <v>483</v>
-      </c>
-      <c r="G75" s="671" t="s">
-        <v>484</v>
-      </c>
-      <c r="H75" s="671" t="s">
-        <v>329</v>
-      </c>
-      <c r="I75" s="671" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="672" t="s">
-        <v>485</v>
-      </c>
-      <c r="B76" s="672" t="s">
-        <v>485</v>
-      </c>
-      <c r="C76" s="672" t="s">
-        <v>486</v>
-      </c>
-      <c r="D76" s="672" t="s">
-        <v>487</v>
-      </c>
-      <c r="E76" s="672" t="s">
-        <v>488</v>
-      </c>
-      <c r="F76" s="672" t="s">
-        <v>489</v>
-      </c>
-      <c r="G76" s="672" t="s">
-        <v>490</v>
-      </c>
-      <c r="H76" s="672" t="s">
-        <v>329</v>
-      </c>
-      <c r="I76" s="672" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="673" t="s">
-        <v>491</v>
-      </c>
-      <c r="B77" s="673" t="s">
-        <v>491</v>
-      </c>
-      <c r="C77" s="673" t="s">
-        <v>492</v>
-      </c>
-      <c r="D77" s="673" t="s">
-        <v>493</v>
-      </c>
-      <c r="E77" s="673" t="s">
-        <v>494</v>
-      </c>
-      <c r="F77" s="673" t="s">
-        <v>495</v>
-      </c>
-      <c r="G77" s="673" t="s">
-        <v>496</v>
-      </c>
-      <c r="H77" s="673" t="s">
-        <v>329</v>
-      </c>
-      <c r="I77" s="673" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="674" t="s">
-        <v>497</v>
-      </c>
-      <c r="B78" s="674" t="s">
-        <v>497</v>
-      </c>
-      <c r="C78" s="674" t="s">
-        <v>498</v>
-      </c>
-      <c r="D78" s="674" t="s">
-        <v>499</v>
-      </c>
-      <c r="E78" s="674" t="s">
-        <v>500</v>
-      </c>
-      <c r="F78" s="674" t="s">
-        <v>501</v>
-      </c>
-      <c r="G78" s="674" t="s">
-        <v>502</v>
-      </c>
-      <c r="H78" s="674" t="s">
-        <v>329</v>
-      </c>
-      <c r="I78" s="674" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="675" t="s">
-        <v>503</v>
-      </c>
-      <c r="B79" s="675" t="s">
-        <v>503</v>
-      </c>
-      <c r="C79" s="675" t="s">
-        <v>504</v>
-      </c>
-      <c r="D79" s="675" t="s">
-        <v>505</v>
-      </c>
-      <c r="E79" s="675" t="s">
-        <v>506</v>
-      </c>
-      <c r="F79" s="675" t="s">
-        <v>507</v>
-      </c>
-      <c r="G79" s="675" t="s">
-        <v>508</v>
-      </c>
-      <c r="H79" s="675" t="s">
-        <v>329</v>
-      </c>
-      <c r="I79" s="675" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="676" t="s">
-        <v>509</v>
-      </c>
-      <c r="B80" s="676" t="s">
-        <v>509</v>
-      </c>
-      <c r="C80" s="676" t="s">
-        <v>510</v>
-      </c>
-      <c r="D80" s="676" t="s">
-        <v>511</v>
-      </c>
-      <c r="E80" s="676" t="s">
-        <v>512</v>
-      </c>
-      <c r="F80" s="676" t="s">
-        <v>513</v>
-      </c>
-      <c r="G80" s="676" t="s">
-        <v>514</v>
-      </c>
-      <c r="H80" s="676" t="s">
-        <v>17</v>
-      </c>
-      <c r="I80" s="676" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="677" t="s">
-        <v>515</v>
-      </c>
-      <c r="B81" s="677" t="s">
-        <v>515</v>
-      </c>
-      <c r="C81" s="677" t="s">
-        <v>516</v>
-      </c>
-      <c r="D81" s="677" t="s">
-        <v>517</v>
-      </c>
-      <c r="E81" s="677" t="s">
-        <v>518</v>
-      </c>
-      <c r="F81" s="677" t="s">
-        <v>519</v>
-      </c>
-      <c r="G81" s="677" t="s">
-        <v>520</v>
-      </c>
-      <c r="H81" s="677" t="s">
-        <v>521</v>
-      </c>
-      <c r="I81" s="677" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="678" t="s">
-        <v>522</v>
-      </c>
-      <c r="B82" s="678" t="s">
-        <v>522</v>
-      </c>
-      <c r="C82" s="678" t="s">
-        <v>523</v>
-      </c>
-      <c r="D82" s="678" t="s">
-        <v>524</v>
-      </c>
-      <c r="E82" s="678" t="s">
-        <v>525</v>
-      </c>
-      <c r="F82" s="678" t="s">
-        <v>526</v>
-      </c>
-      <c r="G82" s="678" t="s">
-        <v>527</v>
-      </c>
-      <c r="H82" s="678" t="s">
-        <v>528</v>
-      </c>
-      <c r="I82" s="678" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="679" t="s">
-        <v>529</v>
-      </c>
-      <c r="B83" s="679" t="s">
-        <v>529</v>
-      </c>
-      <c r="C83" s="679" t="s">
-        <v>530</v>
-      </c>
-      <c r="D83" s="679" t="s">
-        <v>531</v>
-      </c>
-      <c r="E83" s="679" t="s">
-        <v>532</v>
-      </c>
-      <c r="F83" s="679" t="s">
-        <v>533</v>
-      </c>
-      <c r="G83" s="679" t="s">
-        <v>534</v>
-      </c>
-      <c r="H83" s="679" t="s">
-        <v>17</v>
-      </c>
-      <c r="I83" s="679" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="680" t="s">
-        <v>535</v>
-      </c>
-      <c r="B84" s="680" t="s">
-        <v>535</v>
-      </c>
-      <c r="C84" s="680" t="s">
-        <v>536</v>
-      </c>
-      <c r="D84" s="680" t="s">
-        <v>537</v>
-      </c>
-      <c r="E84" s="680" t="s">
-        <v>538</v>
-      </c>
-      <c r="F84" s="680" t="s">
-        <v>539</v>
-      </c>
-      <c r="G84" s="680" t="s">
-        <v>540</v>
-      </c>
-      <c r="H84" s="680" t="s">
-        <v>541</v>
-      </c>
-      <c r="I84" s="680" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="681" t="s">
-        <v>542</v>
-      </c>
-      <c r="B85" s="681" t="s">
-        <v>542</v>
-      </c>
-      <c r="C85" s="681" t="s">
-        <v>543</v>
-      </c>
-      <c r="D85" s="681" t="s">
-        <v>544</v>
-      </c>
-      <c r="E85" s="681" t="s">
-        <v>545</v>
-      </c>
-      <c r="F85" s="681" t="s">
-        <v>546</v>
-      </c>
-      <c r="G85" s="681" t="s">
-        <v>547</v>
-      </c>
-      <c r="H85" s="681" t="s">
-        <v>17</v>
-      </c>
-      <c r="I85" s="681" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="682" t="s">
-        <v>548</v>
-      </c>
-      <c r="B86" s="682" t="s">
-        <v>548</v>
-      </c>
-      <c r="C86" s="682" t="s">
-        <v>549</v>
-      </c>
-      <c r="D86" s="682" t="s">
-        <v>550</v>
-      </c>
-      <c r="E86" s="682" t="s">
-        <v>551</v>
-      </c>
-      <c r="F86" s="682" t="s">
-        <v>552</v>
-      </c>
-      <c r="G86" s="682" t="s">
-        <v>553</v>
-      </c>
-      <c r="H86" s="682" t="s">
-        <v>554</v>
-      </c>
-      <c r="I86" s="682" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="683" t="s">
-        <v>555</v>
-      </c>
-      <c r="B87" s="683" t="s">
-        <v>555</v>
-      </c>
-      <c r="C87" s="683" t="s">
-        <v>556</v>
-      </c>
-      <c r="D87" s="683" t="s">
-        <v>557</v>
-      </c>
-      <c r="E87" s="683" t="s">
-        <v>558</v>
-      </c>
-      <c r="F87" s="683" t="s">
-        <v>559</v>
-      </c>
-      <c r="G87" s="683" t="s">
-        <v>560</v>
-      </c>
-      <c r="H87" s="683" t="s">
-        <v>17</v>
-      </c>
-      <c r="I87" s="683" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="684" t="s">
-        <v>561</v>
-      </c>
-      <c r="B88" s="684" t="s">
-        <v>561</v>
-      </c>
-      <c r="C88" s="684" t="s">
-        <v>562</v>
-      </c>
-      <c r="D88" s="684" t="s">
-        <v>563</v>
-      </c>
-      <c r="E88" s="684" t="s">
-        <v>564</v>
-      </c>
-      <c r="F88" s="684" t="s">
-        <v>565</v>
-      </c>
-      <c r="G88" s="684" t="s">
-        <v>566</v>
-      </c>
-      <c r="H88" s="684" t="s">
-        <v>24</v>
-      </c>
-      <c r="I88" s="684" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="685" t="s">
-        <v>567</v>
-      </c>
-      <c r="B89" s="685" t="s">
-        <v>567</v>
-      </c>
-      <c r="C89" s="685" t="s">
-        <v>568</v>
-      </c>
-      <c r="D89" s="685" t="s">
-        <v>569</v>
-      </c>
-      <c r="E89" s="685" t="s">
-        <v>570</v>
-      </c>
-      <c r="F89" s="685" t="s">
-        <v>571</v>
-      </c>
-      <c r="G89" s="685" t="s">
-        <v>572</v>
-      </c>
-      <c r="H89" s="685" t="s">
-        <v>573</v>
-      </c>
-      <c r="I89" s="685" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="686" t="s">
-        <v>574</v>
-      </c>
-      <c r="B90" s="686" t="s">
-        <v>574</v>
-      </c>
-      <c r="C90" s="686" t="s">
-        <v>575</v>
-      </c>
-      <c r="D90" s="686" t="s">
-        <v>576</v>
-      </c>
-      <c r="E90" s="686" t="s">
-        <v>577</v>
-      </c>
-      <c r="F90" s="686" t="s">
-        <v>578</v>
-      </c>
-      <c r="G90" s="686" t="s">
-        <v>579</v>
-      </c>
-      <c r="H90" s="686" t="s">
-        <v>573</v>
-      </c>
-      <c r="I90" s="686" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="687" t="s">
-        <v>580</v>
-      </c>
-      <c r="B91" s="687" t="s">
-        <v>580</v>
-      </c>
-      <c r="C91" s="687" t="s">
-        <v>581</v>
-      </c>
-      <c r="D91" s="687" t="s">
-        <v>582</v>
-      </c>
-      <c r="E91" s="687" t="s">
-        <v>583</v>
-      </c>
-      <c r="F91" s="687" t="s">
-        <v>584</v>
-      </c>
-      <c r="G91" s="687" t="s">
-        <v>585</v>
-      </c>
-      <c r="H91" s="687" t="s">
-        <v>573</v>
-      </c>
-      <c r="I91" s="687" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="688" t="s">
-        <v>586</v>
-      </c>
-      <c r="B92" s="688" t="s">
-        <v>586</v>
-      </c>
-      <c r="C92" s="688" t="s">
-        <v>587</v>
-      </c>
-      <c r="D92" s="688" t="s">
-        <v>588</v>
-      </c>
-      <c r="E92" s="688" t="s">
-        <v>589</v>
-      </c>
-      <c r="F92" s="688" t="s">
-        <v>93</v>
-      </c>
-      <c r="G92" s="688" t="s">
-        <v>590</v>
-      </c>
-      <c r="H92" s="688" t="s">
-        <v>591</v>
-      </c>
-      <c r="I92" s="688" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="689" t="s">
-        <v>592</v>
-      </c>
-      <c r="B93" s="689" t="s">
-        <v>592</v>
-      </c>
-      <c r="C93" s="689" t="s">
-        <v>593</v>
-      </c>
-      <c r="D93" s="689" t="s">
-        <v>594</v>
-      </c>
-      <c r="E93" s="689" t="s">
-        <v>595</v>
-      </c>
-      <c r="F93" s="689" t="s">
-        <v>93</v>
-      </c>
-      <c r="G93" s="689" t="s">
-        <v>596</v>
-      </c>
-      <c r="H93" s="689" t="s">
-        <v>591</v>
-      </c>
-      <c r="I93" s="689" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="690" t="s">
-        <v>597</v>
-      </c>
-      <c r="B94" s="690" t="s">
-        <v>597</v>
-      </c>
-      <c r="C94" s="690" t="s">
-        <v>598</v>
-      </c>
-      <c r="D94" s="690" t="s">
-        <v>599</v>
-      </c>
-      <c r="E94" s="690" t="s">
-        <v>600</v>
-      </c>
-      <c r="F94" s="690" t="s">
-        <v>601</v>
-      </c>
-      <c r="G94" s="690" t="s">
-        <v>602</v>
-      </c>
-      <c r="H94" s="690" t="s">
-        <v>24</v>
-      </c>
-      <c r="I94" s="690" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="691" t="s">
-        <v>603</v>
-      </c>
-      <c r="B95" s="691" t="s">
-        <v>603</v>
-      </c>
-      <c r="C95" s="691" t="s">
-        <v>604</v>
-      </c>
-      <c r="D95" s="691" t="s">
-        <v>605</v>
-      </c>
-      <c r="E95" s="691" t="s">
-        <v>606</v>
-      </c>
-      <c r="F95" s="691" t="s">
-        <v>607</v>
-      </c>
-      <c r="G95" s="691" t="s">
-        <v>608</v>
-      </c>
-      <c r="H95" s="691" t="s">
-        <v>24</v>
-      </c>
-      <c r="I95" s="691" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="692" t="s">
-        <v>609</v>
-      </c>
-      <c r="B96" s="692" t="s">
-        <v>609</v>
-      </c>
-      <c r="C96" s="692" t="s">
-        <v>610</v>
-      </c>
-      <c r="D96" s="692" t="s">
-        <v>611</v>
-      </c>
-      <c r="E96" s="692" t="s">
-        <v>612</v>
-      </c>
-      <c r="F96" s="692" t="s">
-        <v>613</v>
-      </c>
-      <c r="G96" s="692" t="s">
-        <v>614</v>
-      </c>
-      <c r="H96" s="692" t="s">
-        <v>615</v>
-      </c>
-      <c r="I96" s="692" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="693" t="s">
-        <v>616</v>
-      </c>
-      <c r="B97" s="693" t="s">
-        <v>616</v>
-      </c>
-      <c r="C97" s="693" t="s">
-        <v>617</v>
-      </c>
-      <c r="D97" s="693" t="s">
-        <v>618</v>
-      </c>
-      <c r="E97" s="693" t="s">
-        <v>619</v>
-      </c>
-      <c r="F97" s="693" t="s">
-        <v>620</v>
-      </c>
-      <c r="G97" s="693" t="s">
-        <v>621</v>
-      </c>
-      <c r="H97" s="693" t="s">
-        <v>615</v>
-      </c>
-      <c r="I97" s="693" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="694" t="s">
-        <v>622</v>
-      </c>
-      <c r="B98" s="694" t="s">
-        <v>622</v>
-      </c>
-      <c r="C98" s="694" t="s">
-        <v>623</v>
-      </c>
-      <c r="D98" s="694" t="s">
-        <v>624</v>
-      </c>
-      <c r="E98" s="694" t="s">
-        <v>625</v>
-      </c>
-      <c r="F98" s="694" t="s">
-        <v>626</v>
-      </c>
-      <c r="G98" s="694" t="s">
-        <v>627</v>
-      </c>
-      <c r="H98" s="694" t="s">
-        <v>615</v>
-      </c>
-      <c r="I98" s="694" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="695" t="s">
-        <v>628</v>
-      </c>
-      <c r="B99" s="695" t="s">
-        <v>628</v>
-      </c>
-      <c r="C99" s="695" t="s">
-        <v>629</v>
-      </c>
-      <c r="D99" s="695" t="s">
-        <v>630</v>
-      </c>
-      <c r="E99" s="695" t="s">
-        <v>631</v>
-      </c>
-      <c r="F99" s="695" t="s">
-        <v>632</v>
-      </c>
-      <c r="G99" s="695" t="s">
-        <v>633</v>
-      </c>
-      <c r="H99" s="695" t="s">
-        <v>615</v>
-      </c>
-      <c r="I99" s="695" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="696" t="s">
-        <v>634</v>
-      </c>
-      <c r="B100" s="696" t="s">
-        <v>634</v>
-      </c>
-      <c r="C100" s="696" t="s">
-        <v>635</v>
-      </c>
-      <c r="D100" s="696" t="s">
-        <v>636</v>
-      </c>
-      <c r="E100" s="696" t="s">
-        <v>637</v>
-      </c>
-      <c r="F100" s="696" t="s">
-        <v>638</v>
-      </c>
-      <c r="G100" s="696" t="s">
-        <v>639</v>
-      </c>
-      <c r="H100" s="696" t="s">
-        <v>424</v>
-      </c>
-      <c r="I100" s="696" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="697" t="s">
-        <v>640</v>
-      </c>
-      <c r="B101" s="697" t="s">
-        <v>640</v>
-      </c>
-      <c r="C101" s="697" t="s">
-        <v>641</v>
-      </c>
-      <c r="D101" s="697" t="s">
-        <v>642</v>
-      </c>
-      <c r="E101" s="697" t="s">
-        <v>643</v>
-      </c>
-      <c r="F101" s="697" t="s">
-        <v>644</v>
-      </c>
-      <c r="G101" s="697" t="s">
-        <v>645</v>
-      </c>
-      <c r="H101" s="697" t="s">
-        <v>615</v>
-      </c>
-      <c r="I101" s="697" t="s">
+      <c r="I4" s="701" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>